<commit_message>
More Color Models Results. NEXT: finish color models and start color mixing.
</commit_message>
<xml_diff>
--- a/Analysis/First Study/centroids_allquestions.xlsx
+++ b/Analysis/First Study/centroids_allquestions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="52">
   <si>
     <t>Question 1</t>
   </si>
@@ -138,6 +138,51 @@
   <si>
     <t>Demographic (gender Other)</t>
   </si>
+  <si>
+    <t>distr</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>mediana</t>
+  </si>
+  <si>
+    <t>maximo</t>
+  </si>
+  <si>
+    <t>minimo</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>LCh</t>
+  </si>
+  <si>
+    <t>Laboratory Regular</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>normal = media</t>
+  </si>
+  <si>
+    <t>non = mediana</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>(dispersão)</t>
+  </si>
+  <si>
+    <t>variancia</t>
+  </si>
 </sst>
 </file>
 
@@ -175,12 +220,72 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -272,7 +377,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,8 +389,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -301,15 +418,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,19 +428,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="23">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,7 +772,7 @@
   <dimension ref="A1:AG41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="AG27" sqref="AG27"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,55 +782,62 @@
     <col min="19" max="33" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="20"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O2" s="17"/>
+      <c r="P2" s="18"/>
+      <c r="T2" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>28</v>
@@ -715,14 +884,29 @@
       <c r="P3" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4">
+      <c r="D4" s="32">
         <v>0.06</v>
       </c>
       <c r="E4" s="4"/>
@@ -732,37 +916,55 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="4">
+      <c r="J4" s="37">
         <v>0.06</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4">
+      <c r="M4" s="37">
         <v>0.08</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="5">
+      <c r="P4" s="46">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4">
+      <c r="D5" s="36">
         <v>0.09</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4">
+      <c r="G5" s="30">
         <v>0.13</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4">
+      <c r="J5" s="37">
         <v>0.06</v>
       </c>
       <c r="K5" s="4"/>
@@ -772,47 +974,83 @@
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="5">
+      <c r="P5" s="46">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5">
+        <v>8.6499999999999994E-2</v>
+      </c>
+      <c r="U5" s="26">
+        <v>0.1812</v>
+      </c>
+      <c r="V5">
+        <v>0.1053</v>
+      </c>
+      <c r="W5">
+        <v>0.1047</v>
+      </c>
+      <c r="X5" s="25">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4">
+      <c r="D6" s="29">
         <v>0.04</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4">
+      <c r="G6" s="36">
         <v>0.22</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="4">
+      <c r="J6" s="30">
         <v>0.04</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4">
+      <c r="M6" s="30">
         <v>0.06</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="5">
+      <c r="P6" s="44">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U6">
+        <v>0.17</v>
+      </c>
+      <c r="V6" s="23">
+        <v>0.06</v>
+      </c>
+      <c r="W6" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="X6">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="21">
+      <c r="D7" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E7" s="4"/>
@@ -822,37 +1060,55 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="4">
+      <c r="J7" s="33">
         <v>0.19</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4">
+      <c r="M7" s="33">
         <v>0.24</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="5">
+      <c r="P7" s="48">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S7" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7">
+        <v>0.23</v>
+      </c>
+      <c r="U7">
+        <v>0.3</v>
+      </c>
+      <c r="V7">
+        <v>0.5</v>
+      </c>
+      <c r="W7">
+        <v>0.27</v>
+      </c>
+      <c r="X7">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="21">
+      <c r="D8" s="36">
         <v>0.09</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4">
+      <c r="G8" s="29">
         <v>0.12</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="4">
+      <c r="J8" s="36">
         <v>0.12</v>
       </c>
       <c r="K8" s="4"/>
@@ -862,47 +1118,86 @@
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="5">
+      <c r="P8" s="47">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8">
+        <v>0.03</v>
+      </c>
+      <c r="U8">
+        <v>0.1</v>
+      </c>
+      <c r="V8">
+        <v>0.01</v>
+      </c>
+      <c r="W8">
+        <v>0.02</v>
+      </c>
+      <c r="X8">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="21">
+      <c r="D9" s="30">
         <v>0.05</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4">
+      <c r="G9" s="28">
         <v>0.1</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="4">
+      <c r="J9" s="32">
         <v>0.05</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4">
+      <c r="M9" s="32">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="5">
+      <c r="P9" s="42">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9">
+        <v>0.2</v>
+      </c>
+      <c r="U9">
+        <v>0.2</v>
+      </c>
+      <c r="V9">
+        <v>0.49</v>
+      </c>
+      <c r="W9">
+        <v>0.25</v>
+      </c>
+      <c r="X9">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="21">
+      <c r="D10" s="34">
         <v>0.15</v>
       </c>
       <c r="E10" s="4"/>
@@ -912,62 +1207,80 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="4">
+      <c r="J10" s="32">
         <v>0.05</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4">
+      <c r="M10" s="29">
         <v>0.03</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="5">
+      <c r="P10" s="42">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S10" t="s">
+        <v>51</v>
+      </c>
+      <c r="T10" s="24">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="U10" s="24">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="V10" s="26">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="W10" s="27">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="X10" s="23">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="21">
+      <c r="D11" s="15">
         <v>0.08</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="G11" s="37">
         <v>0.15</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="4">
+      <c r="J11" s="29">
         <v>0.03</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="M11" s="28">
         <v>0.02</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="5">
+      <c r="P11" s="43">
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="21">
+      <c r="D12" s="30">
         <v>0.05</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4">
+      <c r="G12" s="37">
         <v>0.15</v>
       </c>
       <c r="H12" s="4"/>
@@ -982,127 +1295,133 @@
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="5">
+      <c r="P12" s="47">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="21">
+      <c r="D13" s="38">
         <v>0.23</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4">
+      <c r="G13" s="34">
         <v>0.25</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4">
+      <c r="J13" s="28">
         <v>0.01</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4">
+      <c r="M13" s="29">
         <v>0.03</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="5">
+      <c r="P13" s="43">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="21">
+      <c r="D14" s="28">
         <v>0.03</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4">
+      <c r="G14" s="30">
         <v>0.13</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="4">
+      <c r="J14" s="35">
         <v>0.13</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4">
+      <c r="M14" s="38">
         <v>0.27</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="5">
+      <c r="P14" s="50">
         <v>0.13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="21">
+      <c r="D15" s="30">
         <v>0.05</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4">
+      <c r="G15" s="35">
         <v>0.23</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="4">
+      <c r="J15" s="36">
         <v>0.12</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4">
+      <c r="M15" s="35">
         <v>0.14000000000000001</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="5">
+      <c r="P15" s="49">
         <v>0.16</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="21">
+      <c r="D16" s="33">
         <v>0.17</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4">
+      <c r="G16" s="32">
         <v>0.14000000000000001</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="4">
+      <c r="J16" s="34">
         <v>0.18</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4">
+      <c r="M16" s="34">
         <v>0.18</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="5">
+      <c r="P16" s="51">
         <v>0.12</v>
       </c>
     </row>
@@ -1112,27 +1431,27 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="21">
+      <c r="D17" s="35">
         <v>0.1</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4">
+      <c r="G17" s="33">
         <v>0.27</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="4">
+      <c r="J17" s="37">
         <v>0.06</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4">
+      <c r="M17" s="36">
         <v>0.13</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="5">
+      <c r="P17" s="46">
         <v>0.09</v>
       </c>
     </row>
@@ -1142,17 +1461,17 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="21">
+      <c r="D18" s="32">
         <v>0.06</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4">
+      <c r="G18" s="38">
         <v>0.3</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="4">
+      <c r="J18" s="38">
         <v>0.5</v>
       </c>
       <c r="K18" s="4"/>
@@ -1162,7 +1481,7 @@
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="5">
+      <c r="P18" s="52">
         <v>0.11</v>
       </c>
     </row>
@@ -1172,12 +1491,12 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="21">
+      <c r="D19" s="35">
         <v>0.1</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4">
+      <c r="G19" s="40">
         <v>0.2</v>
       </c>
       <c r="H19" s="4"/>
@@ -1187,12 +1506,12 @@
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4">
+      <c r="M19" s="37">
         <v>0.08</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="5">
+      <c r="P19" s="42">
         <v>0.04</v>
       </c>
     </row>
@@ -1202,7 +1521,7 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="7">
+      <c r="D20" s="31">
         <v>0.05</v>
       </c>
       <c r="E20" s="7"/>
@@ -1212,112 +1531,112 @@
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="7">
+      <c r="J20" s="39">
         <v>0.03</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
-      <c r="M20" s="7">
+      <c r="M20" s="41">
         <v>0.08</v>
       </c>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
-      <c r="P20" s="8">
+      <c r="P20" s="45">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="21" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="15" t="s">
+      <c r="S22" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="15"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="15"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
+      <c r="Z22" s="21"/>
+      <c r="AA22" s="21"/>
+      <c r="AB22" s="21"/>
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="21"/>
+      <c r="AE22" s="21"/>
+      <c r="AF22" s="21"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16" t="s">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16" t="s">
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16" t="s">
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="16"/>
-      <c r="P23" s="17"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="20"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="16" t="s">
+      <c r="S23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16" t="s">
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16" t="s">
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="16"/>
-      <c r="AA23" s="16"/>
-      <c r="AB23" s="16" t="s">
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="16"/>
-      <c r="AD23" s="16"/>
-      <c r="AE23" s="16" t="s">
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="17"/>
+      <c r="AF23" s="19"/>
+      <c r="AG23" s="20"/>
     </row>
     <row r="24" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -2399,25 +2718,26 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="S22:AF22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AD23"/>
+    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="S22:AF22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AD23"/>
-    <mergeCell ref="AE23:AG23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2440,95 +2760,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16" t="s">
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="17"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="20"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16" t="s">
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16" t="s">
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16" t="s">
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16" t="s">
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="17"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="20"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -3297,95 +3617,95 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="18" t="s">
+      <c r="S22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
-      <c r="AB22" s="18"/>
-      <c r="AC22" s="18"/>
-      <c r="AD22" s="18"/>
-      <c r="AE22" s="18"/>
-      <c r="AF22" s="18"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="16"/>
+      <c r="AB22" s="16"/>
+      <c r="AC22" s="16"/>
+      <c r="AD22" s="16"/>
+      <c r="AE22" s="16"/>
+      <c r="AF22" s="16"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16" t="s">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16" t="s">
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16" t="s">
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="16"/>
+      <c r="O23" s="19"/>
       <c r="P23" s="5"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="16" t="s">
+      <c r="S23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16" t="s">
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16" t="s">
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="16"/>
-      <c r="AA23" s="16"/>
-      <c r="AB23" s="16" t="s">
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="16"/>
-      <c r="AD23" s="16"/>
-      <c r="AE23" s="16" t="s">
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="17"/>
+      <c r="AF23" s="19"/>
+      <c r="AG23" s="20"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -4152,95 +4472,95 @@
     <row r="42" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
       <c r="P43" s="2"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="15" t="s">
+      <c r="S43" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="15"/>
-      <c r="AA43" s="15"/>
-      <c r="AB43" s="15"/>
-      <c r="AC43" s="15"/>
-      <c r="AD43" s="15"/>
-      <c r="AE43" s="15"/>
-      <c r="AF43" s="15"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="21"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="21"/>
+      <c r="Z43" s="21"/>
+      <c r="AA43" s="21"/>
+      <c r="AB43" s="21"/>
+      <c r="AC43" s="21"/>
+      <c r="AD43" s="21"/>
+      <c r="AE43" s="21"/>
+      <c r="AF43" s="21"/>
       <c r="AG43" s="2"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16" t="s">
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16" t="s">
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16" t="s">
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
       <c r="N44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="O44" s="14"/>
       <c r="P44" s="5"/>
       <c r="R44" s="9"/>
-      <c r="S44" s="16" t="s">
+      <c r="S44" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="T44" s="16"/>
-      <c r="U44" s="16"/>
-      <c r="V44" s="16" t="s">
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="W44" s="16"/>
-      <c r="X44" s="16"/>
-      <c r="Y44" s="16" t="s">
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Z44" s="16"/>
-      <c r="AA44" s="16"/>
-      <c r="AB44" s="16" t="s">
+      <c r="Z44" s="19"/>
+      <c r="AA44" s="19"/>
+      <c r="AB44" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AC44" s="16"/>
-      <c r="AD44" s="16"/>
-      <c r="AE44" s="16" t="s">
+      <c r="AC44" s="19"/>
+      <c r="AD44" s="19"/>
+      <c r="AE44" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AF44" s="16"/>
-      <c r="AG44" s="17"/>
+      <c r="AF44" s="19"/>
+      <c r="AG44" s="20"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
@@ -5008,41 +5328,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="S43:AF43"/>
+    <mergeCell ref="S44:U44"/>
+    <mergeCell ref="V44:X44"/>
+    <mergeCell ref="Y44:AA44"/>
+    <mergeCell ref="AB44:AD44"/>
+    <mergeCell ref="AE44:AG44"/>
+    <mergeCell ref="S22:AF22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AD23"/>
+    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="S1:AF1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="B43:O43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:O23"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="B43:O43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="S1:AF1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="S22:AF22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AD23"/>
-    <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="S43:AF43"/>
-    <mergeCell ref="S44:U44"/>
-    <mergeCell ref="V44:X44"/>
-    <mergeCell ref="Y44:AA44"/>
-    <mergeCell ref="AB44:AD44"/>
-    <mergeCell ref="AE44:AG44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5064,95 +5384,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16" t="s">
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="17"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="20"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19" t="s">
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19" t="s">
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19" t="s">
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19" t="s">
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="20"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="18"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -5921,51 +6241,51 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16" t="s">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16" t="s">
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16" t="s">
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="16"/>
-      <c r="P23" s="17"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="20"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -6369,24 +6689,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="S1:AF1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="S1:AF1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More Results. NEXT: RGB, Lab and Color Mixtures.
</commit_message>
<xml_diff>
--- a/Analysis/First Study/centroids_allquestions.xlsx
+++ b/Analysis/First Study/centroids_allquestions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="62">
   <si>
     <t>Question 1</t>
   </si>
@@ -160,9 +160,6 @@
     <t>LCh</t>
   </si>
   <si>
-    <t>Laboratory Regular</t>
-  </si>
-  <si>
     <t>non</t>
   </si>
   <si>
@@ -183,12 +180,45 @@
   <si>
     <t>variancia</t>
   </si>
+  <si>
+    <t>Online (Regular)</t>
+  </si>
+  <si>
+    <t>Laboratory (Regular)</t>
+  </si>
+  <si>
+    <t>desv padrão</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Desvio-padrão</t>
+  </si>
+  <si>
+    <t>Variância</t>
+  </si>
+  <si>
+    <t>Online (Uncalibrated)</t>
+  </si>
+  <si>
+    <t>Expected C1 C2</t>
+  </si>
+  <si>
+    <t>Desvio-padrao</t>
+  </si>
+  <si>
+    <t>Variancia</t>
+  </si>
+  <si>
+    <t>Mediana</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,6 +245,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -376,8 +414,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -401,8 +490,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -419,27 +512,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -470,8 +542,63 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -483,6 +610,8 @@
     <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -494,6 +623,8 @@
     <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -769,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG41"/>
+  <dimension ref="A1:BC63"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,62 +913,69 @@
     <col min="19" max="33" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17" t="s">
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="17"/>
-      <c r="P2" s="18"/>
-      <c r="T2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
+      <c r="T2" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>28</v>
@@ -899,14 +1037,29 @@
       <c r="X3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="32">
+      <c r="D4" s="25">
         <v>0.06</v>
       </c>
       <c r="E4" s="4"/>
@@ -916,55 +1069,55 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="37">
+      <c r="J4" s="30">
         <v>0.06</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="37">
+      <c r="M4" s="30">
         <v>0.08</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="46">
+      <c r="P4" s="39">
         <v>0.09</v>
       </c>
       <c r="S4" t="s">
         <v>37</v>
       </c>
       <c r="T4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" t="s">
         <v>45</v>
       </c>
-      <c r="U4" t="s">
-        <v>46</v>
-      </c>
       <c r="V4" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X4" t="s">
         <v>45</v>
       </c>
-      <c r="W4" t="s">
-        <v>45</v>
-      </c>
-      <c r="X4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="36">
+      <c r="D5" s="29">
         <v>0.09</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="30">
+      <c r="G5" s="23">
         <v>0.13</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="37">
+      <c r="J5" s="30">
         <v>0.06</v>
       </c>
       <c r="K5" s="4"/>
@@ -974,7 +1127,7 @@
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="46">
+      <c r="P5" s="39">
         <v>0.09</v>
       </c>
       <c r="S5" t="s">
@@ -983,7 +1136,7 @@
       <c r="T5">
         <v>8.6499999999999994E-2</v>
       </c>
-      <c r="U5" s="26">
+      <c r="U5" s="19">
         <v>0.1812</v>
       </c>
       <c r="V5">
@@ -992,59 +1145,59 @@
       <c r="W5">
         <v>0.1047</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5" s="18">
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="29">
+      <c r="D6" s="22">
         <v>0.04</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="36">
+      <c r="G6" s="29">
         <v>0.22</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="30">
+      <c r="J6" s="23">
         <v>0.04</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="30">
+      <c r="M6" s="23">
         <v>0.06</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="44">
+      <c r="P6" s="37">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="S6" t="s">
         <v>39</v>
       </c>
-      <c r="T6" s="24">
+      <c r="T6" s="17">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="U6">
         <v>0.17</v>
       </c>
-      <c r="V6" s="23">
+      <c r="V6" s="16">
         <v>0.06</v>
       </c>
-      <c r="W6" s="25">
+      <c r="W6" s="18">
         <v>0.09</v>
       </c>
       <c r="X6">
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1060,17 +1213,17 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="33">
+      <c r="J7" s="26">
         <v>0.19</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="33">
+      <c r="M7" s="26">
         <v>0.24</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="48">
+      <c r="P7" s="41">
         <v>0.18</v>
       </c>
       <c r="S7" t="s">
@@ -1092,23 +1245,23 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="36">
+      <c r="D8" s="29">
         <v>0.09</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="29">
+      <c r="G8" s="22">
         <v>0.12</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="36">
+      <c r="J8" s="29">
         <v>0.12</v>
       </c>
       <c r="K8" s="4"/>
@@ -1118,7 +1271,7 @@
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="47">
+      <c r="P8" s="40">
         <v>0.1</v>
       </c>
       <c r="S8" t="s">
@@ -1140,40 +1293,40 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="30">
+      <c r="D9" s="23">
         <v>0.05</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="28">
+      <c r="G9" s="21">
         <v>0.1</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="32">
+      <c r="J9" s="25">
         <v>0.05</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="32">
+      <c r="M9" s="25">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="42">
+      <c r="P9" s="35">
         <v>0.04</v>
       </c>
       <c r="R9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T9">
         <v>0.2</v>
@@ -1191,13 +1344,13 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="34">
+      <c r="D10" s="27">
         <v>0.15</v>
       </c>
       <c r="E10" s="4"/>
@@ -1207,39 +1360,39 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="32">
+      <c r="J10" s="25">
         <v>0.05</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="29">
+      <c r="M10" s="22">
         <v>0.03</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="42">
+      <c r="P10" s="35">
         <v>0.04</v>
       </c>
       <c r="S10" t="s">
-        <v>51</v>
-      </c>
-      <c r="T10" s="24">
+        <v>50</v>
+      </c>
+      <c r="T10" s="17">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="U10" s="24">
+      <c r="U10" s="17">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="V10" s="26">
+      <c r="V10" s="19">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="W10" s="27">
+      <c r="W10" s="20">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="X10" s="23">
+      <c r="X10" s="16">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1250,37 +1403,55 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="37">
+      <c r="G11" s="30">
         <v>0.15</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="29">
+      <c r="J11" s="22">
         <v>0.03</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="28">
+      <c r="M11" s="21">
         <v>0.02</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="43">
+      <c r="P11" s="36">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>53</v>
+      </c>
+      <c r="T11">
+        <v>5.2670000000000002E-2</v>
+      </c>
+      <c r="U11">
+        <v>5.6329999999999998E-2</v>
+      </c>
+      <c r="V11">
+        <v>0.11402</v>
+      </c>
+      <c r="W11">
+        <v>6.9470000000000004E-2</v>
+      </c>
+      <c r="X11">
+        <v>4.1529999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="30">
+      <c r="D12" s="23">
         <v>0.05</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="37">
+      <c r="G12" s="30">
         <v>0.15</v>
       </c>
       <c r="H12" s="4"/>
@@ -1295,133 +1466,133 @@
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="47">
+      <c r="P12" s="40">
         <v>0.1</v>
       </c>
       <c r="R12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="38">
+      <c r="D13" s="31">
         <v>0.23</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="34">
+      <c r="G13" s="27">
         <v>0.25</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="28">
+      <c r="J13" s="21">
         <v>0.01</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="29">
+      <c r="M13" s="22">
         <v>0.03</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="43">
+      <c r="P13" s="36">
         <v>0.05</v>
       </c>
       <c r="R13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="28">
+      <c r="D14" s="21">
         <v>0.03</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="30">
+      <c r="G14" s="23">
         <v>0.13</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="35">
+      <c r="J14" s="28">
         <v>0.13</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="38">
+      <c r="M14" s="31">
         <v>0.27</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="50">
+      <c r="P14" s="43">
         <v>0.13</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="30">
+      <c r="D15" s="23">
         <v>0.05</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="35">
+      <c r="G15" s="28">
         <v>0.23</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="36">
+      <c r="J15" s="29">
         <v>0.12</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="35">
+      <c r="M15" s="28">
         <v>0.14000000000000001</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="49">
+      <c r="P15" s="42">
         <v>0.16</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="33">
+      <c r="D16" s="26">
         <v>0.17</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="32">
+      <c r="G16" s="25">
         <v>0.14000000000000001</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="34">
+      <c r="J16" s="27">
         <v>0.18</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="34">
+      <c r="M16" s="27">
         <v>0.18</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="51">
+      <c r="P16" s="44">
         <v>0.12</v>
       </c>
     </row>
@@ -1431,27 +1602,27 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="35">
+      <c r="D17" s="28">
         <v>0.1</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="33">
+      <c r="G17" s="26">
         <v>0.27</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="37">
+      <c r="J17" s="30">
         <v>0.06</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="36">
+      <c r="M17" s="29">
         <v>0.13</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="46">
+      <c r="P17" s="39">
         <v>0.09</v>
       </c>
     </row>
@@ -1461,17 +1632,17 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="32">
+      <c r="D18" s="25">
         <v>0.06</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="38">
+      <c r="G18" s="31">
         <v>0.3</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="38">
+      <c r="J18" s="31">
         <v>0.5</v>
       </c>
       <c r="K18" s="4"/>
@@ -1481,7 +1652,7 @@
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="52">
+      <c r="P18" s="45">
         <v>0.11</v>
       </c>
     </row>
@@ -1491,12 +1662,12 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="35">
+      <c r="D19" s="28">
         <v>0.1</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="40">
+      <c r="G19" s="33">
         <v>0.2</v>
       </c>
       <c r="H19" s="4"/>
@@ -1506,12 +1677,12 @@
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="37">
+      <c r="M19" s="30">
         <v>0.08</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="42">
+      <c r="P19" s="35">
         <v>0.04</v>
       </c>
     </row>
@@ -1521,7 +1692,7 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="31">
+      <c r="D20" s="24">
         <v>0.05</v>
       </c>
       <c r="E20" s="7"/>
@@ -1531,112 +1702,112 @@
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="39">
+      <c r="J20" s="32">
         <v>0.03</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
-      <c r="M20" s="41">
+      <c r="M20" s="34">
         <v>0.08</v>
       </c>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
-      <c r="P20" s="45">
+      <c r="P20" s="38">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="21" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="57"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="21" t="s">
+      <c r="S22" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="60"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="60"/>
+      <c r="AA22" s="60"/>
+      <c r="AB22" s="60"/>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="60"/>
+      <c r="AE22" s="60"/>
+      <c r="AF22" s="60"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19" t="s">
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19" t="s">
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19" t="s">
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="19"/>
-      <c r="P23" s="20"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="63"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="19" t="s">
+      <c r="S23" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19" t="s">
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19" t="s">
+      <c r="W23" s="62"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19" t="s">
+      <c r="Z23" s="62"/>
+      <c r="AA23" s="62"/>
+      <c r="AB23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19" t="s">
+      <c r="AC23" s="62"/>
+      <c r="AD23" s="62"/>
+      <c r="AE23" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="20"/>
+      <c r="AF23" s="62"/>
+      <c r="AG23" s="63"/>
     </row>
     <row r="24" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -2196,7 +2367,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>8</v>
       </c>
@@ -2254,7 +2425,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>9</v>
       </c>
@@ -2312,7 +2483,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>10</v>
       </c>
@@ -2370,7 +2541,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>11</v>
       </c>
@@ -2428,7 +2599,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>12</v>
       </c>
@@ -2486,7 +2657,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>13</v>
       </c>
@@ -2544,7 +2715,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>14</v>
       </c>
@@ -2601,7 +2772,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2659,7 +2830,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>16</v>
       </c>
@@ -2717,8 +2888,1970 @@
         <v>0.15</v>
       </c>
     </row>
+    <row r="42" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
+      <c r="L43" s="60"/>
+      <c r="M43" s="60"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="60"/>
+      <c r="P43" s="60"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="47"/>
+      <c r="T43" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="U43" s="60"/>
+      <c r="V43" s="60"/>
+      <c r="W43" s="60"/>
+      <c r="X43" s="60"/>
+      <c r="Y43" s="60"/>
+      <c r="Z43" s="60"/>
+      <c r="AA43" s="60"/>
+      <c r="AB43" s="60"/>
+      <c r="AC43" s="60"/>
+      <c r="AD43" s="60"/>
+      <c r="AE43" s="60"/>
+      <c r="AF43" s="60"/>
+      <c r="AG43" s="60"/>
+      <c r="AH43" s="60"/>
+      <c r="AI43" s="46"/>
+      <c r="AJ43" s="46"/>
+      <c r="AK43" s="47"/>
+      <c r="AL43" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM43" s="60"/>
+      <c r="AN43" s="60"/>
+      <c r="AO43" s="60"/>
+      <c r="AP43" s="60"/>
+      <c r="AQ43" s="60"/>
+      <c r="AR43" s="60"/>
+      <c r="AS43" s="60"/>
+      <c r="AT43" s="60"/>
+      <c r="AU43" s="60"/>
+      <c r="AV43" s="60"/>
+      <c r="AW43" s="60"/>
+      <c r="AX43" s="60"/>
+      <c r="AY43" s="60"/>
+      <c r="AZ43" s="60"/>
+      <c r="BA43" s="48"/>
+      <c r="BB43" s="48"/>
+      <c r="BC43" s="49"/>
+    </row>
+    <row r="44" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="62"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="O44" s="64"/>
+      <c r="P44" s="64"/>
+      <c r="Q44" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="R44" s="62"/>
+      <c r="S44" s="63"/>
+      <c r="T44" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="U44" s="58"/>
+      <c r="V44" s="58"/>
+      <c r="W44" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="X44" s="62"/>
+      <c r="Y44" s="62"/>
+      <c r="Z44" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA44" s="62"/>
+      <c r="AB44" s="62"/>
+      <c r="AC44" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD44" s="62"/>
+      <c r="AE44" s="62"/>
+      <c r="AF44" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG44" s="62"/>
+      <c r="AH44" s="62"/>
+      <c r="AI44" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ44" s="62"/>
+      <c r="AK44" s="63"/>
+      <c r="AL44" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM44" s="62"/>
+      <c r="AN44" s="62"/>
+      <c r="AO44" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP44" s="62"/>
+      <c r="AQ44" s="62"/>
+      <c r="AR44" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS44" s="62"/>
+      <c r="AT44" s="62"/>
+      <c r="AU44" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV44" s="62"/>
+      <c r="AW44" s="62"/>
+      <c r="AX44" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="AY44" s="62"/>
+      <c r="AZ44" s="62"/>
+      <c r="BA44" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB44" s="62"/>
+      <c r="BC44" s="63"/>
+    </row>
+    <row r="45" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="H45" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J45" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="K45" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="L45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M45" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="N45" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="P45" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T45" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="V45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="X45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y45" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB45" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE45" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH45" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK45" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL45" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM45" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN45" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO45" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR45" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AT45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU45" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX45" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA45" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC45" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="51">
+        <v>0.37680000000000002</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="D46" s="52">
+        <v>0.20283999999999999</v>
+      </c>
+      <c r="E46" s="54">
+        <v>0.1258</v>
+      </c>
+      <c r="F46" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G46" s="53">
+        <v>8.2750000000000004E-2</v>
+      </c>
+      <c r="H46" s="54">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="I46" s="15">
+        <v>0.18</v>
+      </c>
+      <c r="J46" s="71">
+        <v>6.4399999999999999E-2</v>
+      </c>
+      <c r="K46" s="54">
+        <v>9.2600000000000002E-2</v>
+      </c>
+      <c r="L46" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M46" s="53">
+        <v>6.1179999999999998E-2</v>
+      </c>
+      <c r="N46" s="54">
+        <v>0.1237</v>
+      </c>
+      <c r="O46" s="15">
+        <v>0.11</v>
+      </c>
+      <c r="P46" s="53">
+        <v>7.9250000000000001E-2</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>0.1232</v>
+      </c>
+      <c r="R46" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="S46" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="T46" s="3"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="4"/>
+      <c r="AF46" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="4"/>
+      <c r="AI46" s="4"/>
+      <c r="AJ46" s="4"/>
+      <c r="AK46" s="5"/>
+      <c r="AL46" s="9"/>
+      <c r="AM46" s="10"/>
+      <c r="AN46" s="10"/>
+      <c r="AO46" s="10"/>
+      <c r="AP46" s="10"/>
+      <c r="AQ46" s="10"/>
+      <c r="AR46" s="10"/>
+      <c r="AS46" s="10"/>
+      <c r="AT46" s="10"/>
+      <c r="AU46" s="10"/>
+      <c r="AV46" s="10"/>
+      <c r="AW46" s="10"/>
+      <c r="AX46" s="10"/>
+      <c r="AY46" s="10"/>
+      <c r="AZ46" s="10"/>
+      <c r="BA46" s="10"/>
+      <c r="BB46" s="10"/>
+      <c r="BC46" s="11"/>
+    </row>
+    <row r="47" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="51">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="D47" s="52">
+        <v>0.30142999999999998</v>
+      </c>
+      <c r="E47" s="54">
+        <v>0.21729999999999999</v>
+      </c>
+      <c r="F47" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="G47" s="53">
+        <v>0.13014000000000001</v>
+      </c>
+      <c r="H47" s="54">
+        <v>0.1573</v>
+      </c>
+      <c r="I47" s="15">
+        <v>0.16</v>
+      </c>
+      <c r="J47" s="53">
+        <v>9.4450000000000006E-2</v>
+      </c>
+      <c r="K47" s="54">
+        <v>0.106</v>
+      </c>
+      <c r="L47" s="15">
+        <v>0.12</v>
+      </c>
+      <c r="M47" s="53">
+        <v>5.6419999999999998E-2</v>
+      </c>
+      <c r="N47" s="54">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="O47" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P47" s="53">
+        <v>0.10521</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>0.156</v>
+      </c>
+      <c r="R47" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="S47" s="5">
+        <v>8.3989999999999995E-2</v>
+      </c>
+      <c r="T47" s="3"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
+      <c r="AC47" s="4"/>
+      <c r="AD47" s="4"/>
+      <c r="AE47" s="4"/>
+      <c r="AF47" s="4"/>
+      <c r="AG47" s="4"/>
+      <c r="AH47" s="4"/>
+      <c r="AI47" s="4"/>
+      <c r="AJ47" s="4"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="9"/>
+      <c r="AM47" s="10"/>
+      <c r="AN47" s="10"/>
+      <c r="AO47" s="10"/>
+      <c r="AP47" s="10"/>
+      <c r="AQ47" s="10"/>
+      <c r="AR47" s="10"/>
+      <c r="AS47" s="10"/>
+      <c r="AT47" s="10"/>
+      <c r="AU47" s="10"/>
+      <c r="AV47" s="10"/>
+      <c r="AW47" s="10"/>
+      <c r="AX47" s="10"/>
+      <c r="AY47" s="10"/>
+      <c r="AZ47" s="10"/>
+      <c r="BA47" s="10"/>
+      <c r="BB47" s="10"/>
+      <c r="BC47" s="11"/>
+    </row>
+    <row r="48" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="51">
+        <v>0.53910000000000002</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.59</v>
+      </c>
+      <c r="D48" s="52">
+        <v>0.15736</v>
+      </c>
+      <c r="E48" s="54">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="F48" s="15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G48" s="53">
+        <v>0.12307999999999999</v>
+      </c>
+      <c r="H48" s="54">
+        <v>0.23</v>
+      </c>
+      <c r="I48" s="15">
+        <v>0.215</v>
+      </c>
+      <c r="J48" s="71">
+        <v>5.8549999999999998E-2</v>
+      </c>
+      <c r="K48" s="54">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="L48" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="M48" s="53">
+        <v>3.3790000000000001E-2</v>
+      </c>
+      <c r="N48" s="54">
+        <v>0.1114</v>
+      </c>
+      <c r="O48" s="15">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="P48" s="53">
+        <v>6.0339999999999998E-2</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>0.1227</v>
+      </c>
+      <c r="R48" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="S48" s="5">
+        <v>3.918E-2</v>
+      </c>
+      <c r="T48" s="3"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="4"/>
+      <c r="AE48" s="4"/>
+      <c r="AF48" s="4"/>
+      <c r="AG48" s="4"/>
+      <c r="AH48" s="4"/>
+      <c r="AI48" s="4"/>
+      <c r="AJ48" s="4"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="9"/>
+      <c r="AM48" s="10"/>
+      <c r="AN48" s="10"/>
+      <c r="AO48" s="10"/>
+      <c r="AP48" s="10"/>
+      <c r="AQ48" s="10"/>
+      <c r="AR48" s="10"/>
+      <c r="AS48" s="10"/>
+      <c r="AT48" s="10"/>
+      <c r="AU48" s="10"/>
+      <c r="AV48" s="10"/>
+      <c r="AW48" s="10"/>
+      <c r="AX48" s="10"/>
+      <c r="AY48" s="10"/>
+      <c r="AZ48" s="10"/>
+      <c r="BA48" s="10"/>
+      <c r="BB48" s="10"/>
+      <c r="BC48" s="11"/>
+    </row>
+    <row r="49" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="51">
+        <v>0.53620000000000001</v>
+      </c>
+      <c r="C49" s="15">
+        <v>0.64</v>
+      </c>
+      <c r="D49" s="53">
+        <v>0.23433999999999999</v>
+      </c>
+      <c r="E49" s="54">
+        <v>0.1162</v>
+      </c>
+      <c r="F49" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G49" s="53">
+        <v>0.12975</v>
+      </c>
+      <c r="H49" s="54">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="I49" s="15">
+        <v>0.18</v>
+      </c>
+      <c r="J49" s="53">
+        <v>0.11768000000000001</v>
+      </c>
+      <c r="K49" s="54">
+        <v>0.1971</v>
+      </c>
+      <c r="L49" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="M49" s="53">
+        <v>7.3020000000000002E-2</v>
+      </c>
+      <c r="N49" s="54">
+        <v>0.25950000000000001</v>
+      </c>
+      <c r="O49" s="15">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P49" s="53">
+        <v>8.9749999999999996E-2</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>0.20050000000000001</v>
+      </c>
+      <c r="R49" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="S49" s="5">
+        <v>9.1730000000000006E-2</v>
+      </c>
+      <c r="T49" s="3"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4"/>
+      <c r="AE49" s="4"/>
+      <c r="AF49" s="4"/>
+      <c r="AG49" s="4"/>
+      <c r="AH49" s="4"/>
+      <c r="AI49" s="4"/>
+      <c r="AJ49" s="4"/>
+      <c r="AK49" s="5"/>
+      <c r="AL49" s="9"/>
+      <c r="AM49" s="10"/>
+      <c r="AN49" s="10"/>
+      <c r="AO49" s="10"/>
+      <c r="AP49" s="10"/>
+      <c r="AQ49" s="10"/>
+      <c r="AR49" s="10"/>
+      <c r="AS49" s="10"/>
+      <c r="AT49" s="10"/>
+      <c r="AU49" s="10"/>
+      <c r="AV49" s="10"/>
+      <c r="AW49" s="10"/>
+      <c r="AX49" s="10"/>
+      <c r="AY49" s="10"/>
+      <c r="AZ49" s="10"/>
+      <c r="BA49" s="10"/>
+      <c r="BB49" s="10"/>
+      <c r="BC49" s="11"/>
+    </row>
+    <row r="50" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="54">
+        <v>0.31830000000000003</v>
+      </c>
+      <c r="C50" s="15">
+        <v>0.31</v>
+      </c>
+      <c r="D50" s="53">
+        <v>0.18564</v>
+      </c>
+      <c r="E50" s="54">
+        <v>0.16830000000000001</v>
+      </c>
+      <c r="F50" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="G50" s="53">
+        <v>0.10113</v>
+      </c>
+      <c r="H50" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="I50" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="J50" s="53">
+        <v>0.08</v>
+      </c>
+      <c r="K50" s="54">
+        <v>0.13220000000000001</v>
+      </c>
+      <c r="L50" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M50" s="53">
+        <v>6.787E-2</v>
+      </c>
+      <c r="N50" s="54">
+        <v>0.1389</v>
+      </c>
+      <c r="O50" s="15">
+        <v>0.12</v>
+      </c>
+      <c r="P50" s="53">
+        <v>9.1060000000000002E-2</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="R50" s="4">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="S50" s="5">
+        <v>7.5789999999999996E-2</v>
+      </c>
+      <c r="T50" s="3"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="4"/>
+      <c r="AE50" s="4"/>
+      <c r="AF50" s="4"/>
+      <c r="AG50" s="4"/>
+      <c r="AH50" s="4"/>
+      <c r="AI50" s="4"/>
+      <c r="AJ50" s="4"/>
+      <c r="AK50" s="5"/>
+      <c r="AL50" s="9"/>
+      <c r="AM50" s="10"/>
+      <c r="AN50" s="10"/>
+      <c r="AO50" s="10"/>
+      <c r="AP50" s="10"/>
+      <c r="AQ50" s="10"/>
+      <c r="AR50" s="10"/>
+      <c r="AS50" s="10"/>
+      <c r="AT50" s="10"/>
+      <c r="AU50" s="10"/>
+      <c r="AV50" s="10"/>
+      <c r="AW50" s="10"/>
+      <c r="AX50" s="10"/>
+      <c r="AY50" s="10"/>
+      <c r="AZ50" s="10"/>
+      <c r="BA50" s="10"/>
+      <c r="BB50" s="10"/>
+      <c r="BC50" s="11"/>
+    </row>
+    <row r="51" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="54">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="C51" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="D51" s="53">
+        <v>0.2467</v>
+      </c>
+      <c r="E51" s="54">
+        <v>7.4099999999999999E-2</v>
+      </c>
+      <c r="F51" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G51" s="53">
+        <v>0.10417999999999999</v>
+      </c>
+      <c r="H51" s="54">
+        <v>0.13320000000000001</v>
+      </c>
+      <c r="I51" s="15">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="J51" s="53">
+        <v>8.6709999999999995E-2</v>
+      </c>
+      <c r="K51" s="54">
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="L51" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="M51" s="53">
+        <v>6.164E-2</v>
+      </c>
+      <c r="N51" s="54">
+        <v>7.7700000000000005E-2</v>
+      </c>
+      <c r="O51" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="P51" s="53">
+        <v>9.7299999999999998E-2</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>5.0900000000000001E-2</v>
+      </c>
+      <c r="R51" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="S51" s="5">
+        <v>7.374E-2</v>
+      </c>
+      <c r="T51" s="3"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="4"/>
+      <c r="AE51" s="4"/>
+      <c r="AF51" s="4"/>
+      <c r="AG51" s="4"/>
+      <c r="AH51" s="4"/>
+      <c r="AI51" s="4"/>
+      <c r="AJ51" s="4"/>
+      <c r="AK51" s="5"/>
+      <c r="AL51" s="9"/>
+      <c r="AM51" s="10"/>
+      <c r="AN51" s="10"/>
+      <c r="AO51" s="10"/>
+      <c r="AP51" s="10"/>
+      <c r="AQ51" s="10"/>
+      <c r="AR51" s="10"/>
+      <c r="AS51" s="10"/>
+      <c r="AT51" s="10"/>
+      <c r="AU51" s="10"/>
+      <c r="AV51" s="10"/>
+      <c r="AW51" s="10"/>
+      <c r="AX51" s="10"/>
+      <c r="AY51" s="10"/>
+      <c r="AZ51" s="10"/>
+      <c r="BA51" s="10"/>
+      <c r="BB51" s="10"/>
+      <c r="BC51" s="11"/>
+    </row>
+    <row r="52" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="54">
+        <v>0.4536</v>
+      </c>
+      <c r="C52" s="15">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="D52" s="53">
+        <v>0.11524</v>
+      </c>
+      <c r="E52" s="54">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="F52" s="15">
+        <v>0.06</v>
+      </c>
+      <c r="G52" s="53">
+        <v>0.20679</v>
+      </c>
+      <c r="H52" s="54">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="I52" s="15">
+        <v>0.27</v>
+      </c>
+      <c r="J52" s="53">
+        <v>0.10038</v>
+      </c>
+      <c r="K52" s="54">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="L52" s="15">
+        <v>0.06</v>
+      </c>
+      <c r="M52" s="53">
+        <v>7.5230000000000005E-2</v>
+      </c>
+      <c r="N52" s="54">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="O52" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="P52" s="53">
+        <v>0.12834999999999999</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>0.17050000000000001</v>
+      </c>
+      <c r="R52" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="S52" s="5">
+        <v>7.9250000000000001E-2</v>
+      </c>
+      <c r="T52" s="3"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4"/>
+      <c r="AA52" s="4"/>
+      <c r="AB52" s="4"/>
+      <c r="AC52" s="4"/>
+      <c r="AD52" s="4"/>
+      <c r="AE52" s="4"/>
+      <c r="AF52" s="4"/>
+      <c r="AG52" s="4"/>
+      <c r="AH52" s="4"/>
+      <c r="AI52" s="4"/>
+      <c r="AJ52" s="4"/>
+      <c r="AK52" s="5"/>
+      <c r="AL52" s="9"/>
+      <c r="AM52" s="10"/>
+      <c r="AN52" s="10"/>
+      <c r="AO52" s="10"/>
+      <c r="AP52" s="10"/>
+      <c r="AQ52" s="10"/>
+      <c r="AR52" s="10"/>
+      <c r="AS52" s="10"/>
+      <c r="AT52" s="10"/>
+      <c r="AU52" s="10"/>
+      <c r="AV52" s="10"/>
+      <c r="AW52" s="10"/>
+      <c r="AX52" s="10"/>
+      <c r="AY52" s="10"/>
+      <c r="AZ52" s="10"/>
+      <c r="BA52" s="10"/>
+      <c r="BB52" s="10"/>
+      <c r="BC52" s="11"/>
+    </row>
+    <row r="53" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="54">
+        <v>0.48770000000000002</v>
+      </c>
+      <c r="C53" s="15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D53" s="53">
+        <v>0.25331999999999999</v>
+      </c>
+      <c r="E53" s="54">
+        <v>9.5399999999999999E-2</v>
+      </c>
+      <c r="F53" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G53" s="53">
+        <v>0.16302</v>
+      </c>
+      <c r="H53" s="54">
+        <v>0.17</v>
+      </c>
+      <c r="I53" s="15">
+        <v>0.17</v>
+      </c>
+      <c r="J53" s="53">
+        <v>0.12845000000000001</v>
+      </c>
+      <c r="K53" s="54">
+        <v>0.1008</v>
+      </c>
+      <c r="L53" s="15">
+        <v>0.09</v>
+      </c>
+      <c r="M53" s="53">
+        <v>0.49740000000000001</v>
+      </c>
+      <c r="N53" s="54">
+        <v>0.12920000000000001</v>
+      </c>
+      <c r="O53" s="15">
+        <v>0.12</v>
+      </c>
+      <c r="P53" s="53">
+        <v>8.967E-2</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>0.12920000000000001</v>
+      </c>
+      <c r="R53" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S53" s="5">
+        <v>8.9859999999999995E-2</v>
+      </c>
+      <c r="T53" s="3"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4"/>
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="4"/>
+      <c r="AE53" s="4"/>
+      <c r="AF53" s="4"/>
+      <c r="AG53" s="4"/>
+      <c r="AH53" s="4"/>
+      <c r="AI53" s="4"/>
+      <c r="AJ53" s="4"/>
+      <c r="AK53" s="5"/>
+      <c r="AL53" s="9"/>
+      <c r="AM53" s="10"/>
+      <c r="AN53" s="10"/>
+      <c r="AO53" s="10"/>
+      <c r="AP53" s="10"/>
+      <c r="AQ53" s="10"/>
+      <c r="AR53" s="10"/>
+      <c r="AS53" s="10"/>
+      <c r="AT53" s="10"/>
+      <c r="AU53" s="10"/>
+      <c r="AV53" s="10"/>
+      <c r="AW53" s="10"/>
+      <c r="AX53" s="10"/>
+      <c r="AY53" s="10"/>
+      <c r="AZ53" s="10"/>
+      <c r="BA53" s="10"/>
+      <c r="BB53" s="10"/>
+      <c r="BC53" s="11"/>
+    </row>
+    <row r="54" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="54">
+        <v>0.4405</v>
+      </c>
+      <c r="C54" s="15">
+        <v>0.49</v>
+      </c>
+      <c r="D54" s="53">
+        <v>0.25394</v>
+      </c>
+      <c r="E54" s="54">
+        <v>0.1258</v>
+      </c>
+      <c r="F54" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="G54" s="53">
+        <v>9.8900000000000002E-2</v>
+      </c>
+      <c r="H54" s="54">
+        <v>0.16420000000000001</v>
+      </c>
+      <c r="I54" s="15">
+        <v>0.13</v>
+      </c>
+      <c r="J54" s="53">
+        <v>7.4630000000000002E-2</v>
+      </c>
+      <c r="K54" s="54">
+        <v>9.11E-2</v>
+      </c>
+      <c r="L54" s="15">
+        <v>0.09</v>
+      </c>
+      <c r="M54" s="53">
+        <v>4.6420000000000003E-2</v>
+      </c>
+      <c r="N54" s="54">
+        <v>0.10050000000000001</v>
+      </c>
+      <c r="O54" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="P54" s="53">
+        <v>7.5240000000000001E-2</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>0.1142</v>
+      </c>
+      <c r="R54" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="S54" s="5">
+        <v>6.694E-2</v>
+      </c>
+      <c r="T54" s="3"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4"/>
+      <c r="AB54" s="4"/>
+      <c r="AC54" s="4"/>
+      <c r="AD54" s="4"/>
+      <c r="AE54" s="4"/>
+      <c r="AF54" s="4"/>
+      <c r="AG54" s="4"/>
+      <c r="AH54" s="4"/>
+      <c r="AI54" s="4"/>
+      <c r="AJ54" s="4"/>
+      <c r="AK54" s="5"/>
+      <c r="AL54" s="9"/>
+      <c r="AM54" s="10"/>
+      <c r="AN54" s="10"/>
+      <c r="AO54" s="10"/>
+      <c r="AP54" s="10"/>
+      <c r="AQ54" s="10"/>
+      <c r="AR54" s="10"/>
+      <c r="AS54" s="10"/>
+      <c r="AT54" s="10"/>
+      <c r="AU54" s="10"/>
+      <c r="AV54" s="10"/>
+      <c r="AW54" s="10"/>
+      <c r="AX54" s="10"/>
+      <c r="AY54" s="10"/>
+      <c r="AZ54" s="10"/>
+      <c r="BA54" s="10"/>
+      <c r="BB54" s="10"/>
+      <c r="BC54" s="11"/>
+    </row>
+    <row r="55" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="51">
+        <v>0.56710000000000005</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="D55" s="52">
+        <v>0.15173</v>
+      </c>
+      <c r="E55" s="51">
+        <v>0.3</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="G55" s="52">
+        <v>0.15792</v>
+      </c>
+      <c r="H55" s="51">
+        <v>0.25569999999999998</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="J55" s="52">
+        <v>0.1164</v>
+      </c>
+      <c r="K55" s="51">
+        <v>0.13139999999999999</v>
+      </c>
+      <c r="L55" s="15">
+        <v>0.12</v>
+      </c>
+      <c r="M55" s="52">
+        <v>4.7690000000000003E-2</v>
+      </c>
+      <c r="N55" s="51">
+        <v>0.2107</v>
+      </c>
+      <c r="O55" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P55" s="52">
+        <v>6.4030000000000004E-2</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="R55" s="4">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="S55" s="5">
+        <v>9.5810000000000006E-2</v>
+      </c>
+      <c r="T55" s="3"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="4"/>
+      <c r="AA55" s="4"/>
+      <c r="AB55" s="4"/>
+      <c r="AC55" s="4"/>
+      <c r="AD55" s="4"/>
+      <c r="AE55" s="4"/>
+      <c r="AF55" s="4"/>
+      <c r="AG55" s="4"/>
+      <c r="AH55" s="4"/>
+      <c r="AI55" s="4"/>
+      <c r="AJ55" s="4"/>
+      <c r="AK55" s="5"/>
+      <c r="AL55" s="9"/>
+      <c r="AM55" s="10"/>
+      <c r="AN55" s="10"/>
+      <c r="AO55" s="10"/>
+      <c r="AP55" s="10"/>
+      <c r="AQ55" s="10"/>
+      <c r="AR55" s="10"/>
+      <c r="AS55" s="10"/>
+      <c r="AT55" s="10"/>
+      <c r="AU55" s="10"/>
+      <c r="AV55" s="10"/>
+      <c r="AW55" s="10"/>
+      <c r="AX55" s="10"/>
+      <c r="AY55" s="10"/>
+      <c r="AZ55" s="10"/>
+      <c r="BA55" s="10"/>
+      <c r="BB55" s="10"/>
+      <c r="BC55" s="11"/>
+    </row>
+    <row r="56" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="51">
+        <v>0.64480000000000004</v>
+      </c>
+      <c r="C56" s="15">
+        <v>0.73</v>
+      </c>
+      <c r="D56" s="52">
+        <v>0.13957</v>
+      </c>
+      <c r="E56" s="51">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="F56" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="G56" s="52">
+        <v>8.8279999999999997E-2</v>
+      </c>
+      <c r="H56" s="51">
+        <v>0.13739999999999999</v>
+      </c>
+      <c r="I56" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="J56" s="52">
+        <v>0.11752</v>
+      </c>
+      <c r="K56" s="51">
+        <v>0.13039999999999999</v>
+      </c>
+      <c r="L56" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M56" s="52">
+        <v>2.852E-2</v>
+      </c>
+      <c r="N56" s="51">
+        <v>0.18390000000000001</v>
+      </c>
+      <c r="O56" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="P56" s="52">
+        <v>3.986E-2</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>0.14430000000000001</v>
+      </c>
+      <c r="R56" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="S56" s="5">
+        <v>2.7269999999999999E-2</v>
+      </c>
+      <c r="T56" s="3"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4"/>
+      <c r="AB56" s="4"/>
+      <c r="AC56" s="4"/>
+      <c r="AD56" s="4"/>
+      <c r="AE56" s="4"/>
+      <c r="AF56" s="4"/>
+      <c r="AG56" s="4"/>
+      <c r="AH56" s="4"/>
+      <c r="AI56" s="4"/>
+      <c r="AJ56" s="4"/>
+      <c r="AK56" s="5"/>
+      <c r="AL56" s="9"/>
+      <c r="AM56" s="10"/>
+      <c r="AN56" s="10"/>
+      <c r="AO56" s="10"/>
+      <c r="AP56" s="10"/>
+      <c r="AQ56" s="10"/>
+      <c r="AR56" s="10"/>
+      <c r="AS56" s="10"/>
+      <c r="AT56" s="10"/>
+      <c r="AU56" s="10"/>
+      <c r="AV56" s="10"/>
+      <c r="AW56" s="10"/>
+      <c r="AX56" s="10"/>
+      <c r="AY56" s="10"/>
+      <c r="AZ56" s="10"/>
+      <c r="BA56" s="10"/>
+      <c r="BB56" s="10"/>
+      <c r="BC56" s="11"/>
+    </row>
+    <row r="57" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="51">
+        <v>0.4133</v>
+      </c>
+      <c r="C57" s="15">
+        <v>0.42</v>
+      </c>
+      <c r="D57" s="52">
+        <v>0.15060999999999999</v>
+      </c>
+      <c r="E57" s="51">
+        <v>0.1067</v>
+      </c>
+      <c r="F57" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="G57" s="52">
+        <v>0.12639</v>
+      </c>
+      <c r="H57" s="51">
+        <v>0.23430000000000001</v>
+      </c>
+      <c r="I57" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="J57" s="52">
+        <v>6.6379999999999995E-2</v>
+      </c>
+      <c r="K57" s="51">
+        <v>0.13139999999999999</v>
+      </c>
+      <c r="L57" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M57" s="52">
+        <v>3.9660000000000001E-2</v>
+      </c>
+      <c r="N57" s="51">
+        <v>0.151</v>
+      </c>
+      <c r="O57" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P57" s="52">
+        <v>7.7579999999999996E-2</v>
+      </c>
+      <c r="Q57" s="4">
+        <v>0.17430000000000001</v>
+      </c>
+      <c r="R57" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="S57" s="5">
+        <v>7.2840000000000002E-2</v>
+      </c>
+      <c r="T57" s="3"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+      <c r="AB57" s="4"/>
+      <c r="AC57" s="4"/>
+      <c r="AD57" s="4"/>
+      <c r="AE57" s="4"/>
+      <c r="AF57" s="4"/>
+      <c r="AG57" s="4"/>
+      <c r="AH57" s="4"/>
+      <c r="AI57" s="4"/>
+      <c r="AJ57" s="4"/>
+      <c r="AK57" s="5"/>
+      <c r="AL57" s="9"/>
+      <c r="AM57" s="10"/>
+      <c r="AN57" s="10"/>
+      <c r="AO57" s="10"/>
+      <c r="AP57" s="10"/>
+      <c r="AQ57" s="10"/>
+      <c r="AR57" s="10"/>
+      <c r="AS57" s="10"/>
+      <c r="AT57" s="10"/>
+      <c r="AU57" s="10"/>
+      <c r="AV57" s="10"/>
+      <c r="AW57" s="10"/>
+      <c r="AX57" s="10"/>
+      <c r="AY57" s="10"/>
+      <c r="AZ57" s="10"/>
+      <c r="BA57" s="10"/>
+      <c r="BB57" s="10"/>
+      <c r="BC57" s="11"/>
+    </row>
+    <row r="58" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="51">
+        <v>0.51690000000000003</v>
+      </c>
+      <c r="C58" s="15">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="D58" s="52">
+        <v>0.24789</v>
+      </c>
+      <c r="E58" s="51">
+        <v>0.27129999999999999</v>
+      </c>
+      <c r="F58" s="15">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G58" s="52">
+        <v>0.15606999999999999</v>
+      </c>
+      <c r="H58" s="51">
+        <v>0.1663</v>
+      </c>
+      <c r="I58" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J58" s="52">
+        <v>9.7009999999999999E-2</v>
+      </c>
+      <c r="K58" s="51">
+        <v>0.1875</v>
+      </c>
+      <c r="L58" s="15">
+        <v>0.215</v>
+      </c>
+      <c r="M58" s="52">
+        <v>0.13097</v>
+      </c>
+      <c r="N58" s="51">
+        <v>0.245</v>
+      </c>
+      <c r="O58" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="P58" s="52">
+        <v>0.15795000000000001</v>
+      </c>
+      <c r="Q58" s="4">
+        <v>0.22689999999999999</v>
+      </c>
+      <c r="R58" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="S58" s="5">
+        <v>0.12224</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
+      <c r="AA58" s="4"/>
+      <c r="AB58" s="4"/>
+      <c r="AC58" s="4"/>
+      <c r="AD58" s="4"/>
+      <c r="AE58" s="4"/>
+      <c r="AF58" s="4"/>
+      <c r="AG58" s="4"/>
+      <c r="AH58" s="4"/>
+      <c r="AI58" s="4"/>
+      <c r="AJ58" s="4"/>
+      <c r="AK58" s="5"/>
+      <c r="AL58" s="9"/>
+      <c r="AM58" s="10"/>
+      <c r="AN58" s="10"/>
+      <c r="AO58" s="10"/>
+      <c r="AP58" s="10"/>
+      <c r="AQ58" s="10"/>
+      <c r="AR58" s="10"/>
+      <c r="AS58" s="10"/>
+      <c r="AT58" s="10"/>
+      <c r="AU58" s="10"/>
+      <c r="AV58" s="10"/>
+      <c r="AW58" s="10"/>
+      <c r="AX58" s="10"/>
+      <c r="AY58" s="10"/>
+      <c r="AZ58" s="10"/>
+      <c r="BA58" s="10"/>
+      <c r="BB58" s="10"/>
+      <c r="BC58" s="11"/>
+    </row>
+    <row r="59" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="51">
+        <v>0.46089999999999998</v>
+      </c>
+      <c r="C59" s="15">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="D59" s="52">
+        <v>0.26694000000000001</v>
+      </c>
+      <c r="E59" s="51">
+        <v>0.1186</v>
+      </c>
+      <c r="F59" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="G59" s="52">
+        <v>1.4423E-2</v>
+      </c>
+      <c r="H59" s="51">
+        <v>0.29949999999999999</v>
+      </c>
+      <c r="I59" s="15">
+        <v>0.315</v>
+      </c>
+      <c r="J59" s="52">
+        <v>8.9359999999999995E-2</v>
+      </c>
+      <c r="K59" s="51">
+        <v>9.7299999999999998E-2</v>
+      </c>
+      <c r="L59" s="15">
+        <v>0.09</v>
+      </c>
+      <c r="M59" s="52">
+        <v>0.49009999999999998</v>
+      </c>
+      <c r="N59" s="51">
+        <v>0.13270000000000001</v>
+      </c>
+      <c r="O59" s="15">
+        <v>0.125</v>
+      </c>
+      <c r="P59" s="52">
+        <v>0.13406000000000001</v>
+      </c>
+      <c r="Q59" s="4">
+        <v>0.1336</v>
+      </c>
+      <c r="R59" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="S59" s="5">
+        <v>9.4439999999999996E-2</v>
+      </c>
+      <c r="T59" s="3"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+      <c r="W59" s="4"/>
+      <c r="X59" s="4"/>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="4"/>
+      <c r="AA59" s="4"/>
+      <c r="AB59" s="4"/>
+      <c r="AC59" s="4"/>
+      <c r="AD59" s="4"/>
+      <c r="AE59" s="4"/>
+      <c r="AF59" s="4"/>
+      <c r="AG59" s="4"/>
+      <c r="AH59" s="4"/>
+      <c r="AI59" s="4"/>
+      <c r="AJ59" s="4"/>
+      <c r="AK59" s="5"/>
+      <c r="AL59" s="9"/>
+      <c r="AM59" s="10"/>
+      <c r="AN59" s="10"/>
+      <c r="AO59" s="10"/>
+      <c r="AP59" s="10"/>
+      <c r="AQ59" s="10"/>
+      <c r="AR59" s="10"/>
+      <c r="AS59" s="10"/>
+      <c r="AT59" s="10"/>
+      <c r="AU59" s="10"/>
+      <c r="AV59" s="10"/>
+      <c r="AW59" s="10"/>
+      <c r="AX59" s="10"/>
+      <c r="AY59" s="10"/>
+      <c r="AZ59" s="10"/>
+      <c r="BA59" s="10"/>
+      <c r="BB59" s="10"/>
+      <c r="BC59" s="11"/>
+    </row>
+    <row r="60" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="51">
+        <v>0.68689999999999996</v>
+      </c>
+      <c r="C60" s="15">
+        <v>0.74</v>
+      </c>
+      <c r="D60" s="52">
+        <v>0.2787</v>
+      </c>
+      <c r="E60" s="51">
+        <v>0.09</v>
+      </c>
+      <c r="F60" s="15">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G60" s="52">
+        <v>3.5589999999999997E-2</v>
+      </c>
+      <c r="H60" s="51">
+        <v>0.30309999999999998</v>
+      </c>
+      <c r="I60" s="15">
+        <v>0.31</v>
+      </c>
+      <c r="J60" s="52">
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="K60" s="51">
+        <v>6.25E-2</v>
+      </c>
+      <c r="L60" s="15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="M60" s="52">
+        <v>2.6960000000000001E-2</v>
+      </c>
+      <c r="N60" s="51">
+        <v>0.11</v>
+      </c>
+      <c r="O60" s="15">
+        <v>0.11</v>
+      </c>
+      <c r="P60" s="52">
+        <v>4.7050000000000002E-2</v>
+      </c>
+      <c r="Q60" s="4">
+        <v>0.12559999999999999</v>
+      </c>
+      <c r="R60" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="S60" s="5">
+        <v>6.2289999999999998E-2</v>
+      </c>
+      <c r="T60" s="3"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
+      <c r="Z60" s="4"/>
+      <c r="AA60" s="4"/>
+      <c r="AB60" s="4"/>
+      <c r="AC60" s="4"/>
+      <c r="AD60" s="4"/>
+      <c r="AE60" s="4"/>
+      <c r="AF60" s="4"/>
+      <c r="AG60" s="4"/>
+      <c r="AH60" s="4"/>
+      <c r="AI60" s="4"/>
+      <c r="AJ60" s="4"/>
+      <c r="AK60" s="5"/>
+      <c r="AL60" s="9"/>
+      <c r="AM60" s="10"/>
+      <c r="AN60" s="10"/>
+      <c r="AO60" s="10"/>
+      <c r="AP60" s="10"/>
+      <c r="AQ60" s="10"/>
+      <c r="AR60" s="10"/>
+      <c r="AS60" s="10"/>
+      <c r="AT60" s="10"/>
+      <c r="AU60" s="10"/>
+      <c r="AV60" s="10"/>
+      <c r="AW60" s="10"/>
+      <c r="AX60" s="10"/>
+      <c r="AY60" s="10"/>
+      <c r="AZ60" s="10"/>
+      <c r="BA60" s="10"/>
+      <c r="BB60" s="10"/>
+      <c r="BC60" s="11"/>
+    </row>
+    <row r="61" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="51">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="C61" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="D61" s="52">
+        <v>0.22001000000000001</v>
+      </c>
+      <c r="E61" s="51">
+        <v>0.2087</v>
+      </c>
+      <c r="F61" s="15">
+        <v>0.23</v>
+      </c>
+      <c r="G61" s="52">
+        <v>0.10378</v>
+      </c>
+      <c r="H61" s="51">
+        <v>0.21870000000000001</v>
+      </c>
+      <c r="I61" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J61" s="52">
+        <v>0.12171</v>
+      </c>
+      <c r="K61" s="51">
+        <v>0.1033</v>
+      </c>
+      <c r="L61" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="M61" s="52">
+        <v>5.108E-2</v>
+      </c>
+      <c r="N61" s="51">
+        <v>0.1593</v>
+      </c>
+      <c r="O61" s="15">
+        <v>0.17</v>
+      </c>
+      <c r="P61" s="52">
+        <v>6.8290000000000003E-2</v>
+      </c>
+      <c r="Q61" s="4">
+        <v>0.124</v>
+      </c>
+      <c r="R61" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="S61" s="5">
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="T61" s="3"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="4"/>
+      <c r="Y61" s="4"/>
+      <c r="Z61" s="4"/>
+      <c r="AA61" s="4"/>
+      <c r="AB61" s="4"/>
+      <c r="AC61" s="4"/>
+      <c r="AD61" s="4"/>
+      <c r="AE61" s="4"/>
+      <c r="AF61" s="4"/>
+      <c r="AG61" s="4"/>
+      <c r="AH61" s="4"/>
+      <c r="AI61" s="4"/>
+      <c r="AJ61" s="4"/>
+      <c r="AK61" s="5"/>
+      <c r="AL61" s="9"/>
+      <c r="AM61" s="10"/>
+      <c r="AN61" s="10"/>
+      <c r="AO61" s="10"/>
+      <c r="AP61" s="10"/>
+      <c r="AQ61" s="10"/>
+      <c r="AR61" s="10"/>
+      <c r="AS61" s="10"/>
+      <c r="AT61" s="10"/>
+      <c r="AU61" s="10"/>
+      <c r="AV61" s="10"/>
+      <c r="AW61" s="10"/>
+      <c r="AX61" s="10"/>
+      <c r="AY61" s="10"/>
+      <c r="AZ61" s="10"/>
+      <c r="BA61" s="10"/>
+      <c r="BB61" s="10"/>
+      <c r="BC61" s="11"/>
+    </row>
+    <row r="62" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="55">
+        <v>0.49</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D62" s="56">
+        <v>0.18559</v>
+      </c>
+      <c r="E62" s="55">
+        <v>6.83E-2</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G62" s="56">
+        <v>0.10228</v>
+      </c>
+      <c r="H62" s="55">
+        <v>0.16259999999999999</v>
+      </c>
+      <c r="I62" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J62" s="72">
+        <v>5.9020000000000003E-2</v>
+      </c>
+      <c r="K62" s="55">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="L62" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="M62" s="56">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="N62" s="55">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="O62" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="P62" s="56">
+        <v>5.74E-2</v>
+      </c>
+      <c r="Q62" s="7">
+        <v>0.113</v>
+      </c>
+      <c r="R62" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="S62" s="8">
+        <v>5.1119999999999999E-2</v>
+      </c>
+      <c r="T62" s="6"/>
+      <c r="U62" s="7"/>
+      <c r="V62" s="7"/>
+      <c r="W62" s="7"/>
+      <c r="X62" s="7"/>
+      <c r="Y62" s="7"/>
+      <c r="Z62" s="7"/>
+      <c r="AA62" s="7"/>
+      <c r="AB62" s="7"/>
+      <c r="AC62" s="7"/>
+      <c r="AD62" s="7"/>
+      <c r="AE62" s="7"/>
+      <c r="AF62" s="7"/>
+      <c r="AG62" s="7"/>
+      <c r="AH62" s="7"/>
+      <c r="AI62" s="7"/>
+      <c r="AJ62" s="7"/>
+      <c r="AK62" s="8"/>
+      <c r="AL62" s="12"/>
+      <c r="AM62" s="13"/>
+      <c r="AN62" s="13"/>
+      <c r="AO62" s="13"/>
+      <c r="AP62" s="13"/>
+      <c r="AQ62" s="13"/>
+      <c r="AR62" s="13"/>
+      <c r="AS62" s="13"/>
+      <c r="AT62" s="13"/>
+      <c r="AU62" s="13"/>
+      <c r="AV62" s="13"/>
+      <c r="AW62" s="13"/>
+      <c r="AX62" s="13"/>
+      <c r="AY62" s="13"/>
+      <c r="AZ62" s="13"/>
+      <c r="BA62" s="13"/>
+      <c r="BB62" s="13"/>
+      <c r="BC62" s="50"/>
+    </row>
+    <row r="63" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="41">
+    <mergeCell ref="BA44:BC44"/>
+    <mergeCell ref="AF44:AH44"/>
+    <mergeCell ref="AI44:AK44"/>
+    <mergeCell ref="AL44:AN44"/>
+    <mergeCell ref="AO44:AQ44"/>
+    <mergeCell ref="AR44:AT44"/>
+    <mergeCell ref="AL43:AZ43"/>
+    <mergeCell ref="AU44:AW44"/>
+    <mergeCell ref="AX44:AZ44"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="T44:V44"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="Z44:AB44"/>
+    <mergeCell ref="AC44:AE44"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B43:P43"/>
     <mergeCell ref="T2:X2"/>
     <mergeCell ref="S22:AF22"/>
     <mergeCell ref="S23:U23"/>
@@ -2726,12 +4859,14 @@
     <mergeCell ref="Y23:AA23"/>
     <mergeCell ref="AB23:AD23"/>
     <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="Y2:AC2"/>
     <mergeCell ref="B22:O22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="N23:P23"/>
+    <mergeCell ref="T43:AH43"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
@@ -2760,95 +4895,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19" t="s">
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19" t="s">
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="20"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="63"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19" t="s">
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19" t="s">
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19" t="s">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19" t="s">
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="20"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="63"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -3617,95 +5752,95 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="16" t="s">
+      <c r="S22" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="16"/>
-      <c r="AB22" s="16"/>
-      <c r="AC22" s="16"/>
-      <c r="AD22" s="16"/>
-      <c r="AE22" s="16"/>
-      <c r="AF22" s="16"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="57"/>
+      <c r="Z22" s="57"/>
+      <c r="AA22" s="57"/>
+      <c r="AB22" s="57"/>
+      <c r="AC22" s="57"/>
+      <c r="AD22" s="57"/>
+      <c r="AE22" s="57"/>
+      <c r="AF22" s="57"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19" t="s">
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19" t="s">
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19" t="s">
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="19"/>
+      <c r="O23" s="62"/>
       <c r="P23" s="5"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="19" t="s">
+      <c r="S23" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19" t="s">
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19" t="s">
+      <c r="W23" s="62"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19" t="s">
+      <c r="Z23" s="62"/>
+      <c r="AA23" s="62"/>
+      <c r="AB23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19" t="s">
+      <c r="AC23" s="62"/>
+      <c r="AD23" s="62"/>
+      <c r="AE23" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="20"/>
+      <c r="AF23" s="62"/>
+      <c r="AG23" s="63"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -4472,95 +6607,95 @@
     <row r="42" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="21"/>
-      <c r="N43" s="21"/>
-      <c r="O43" s="21"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
+      <c r="L43" s="60"/>
+      <c r="M43" s="60"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="60"/>
       <c r="P43" s="2"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="21" t="s">
+      <c r="S43" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="T43" s="21"/>
-      <c r="U43" s="21"/>
-      <c r="V43" s="21"/>
-      <c r="W43" s="21"/>
-      <c r="X43" s="21"/>
-      <c r="Y43" s="21"/>
-      <c r="Z43" s="21"/>
-      <c r="AA43" s="21"/>
-      <c r="AB43" s="21"/>
-      <c r="AC43" s="21"/>
-      <c r="AD43" s="21"/>
-      <c r="AE43" s="21"/>
-      <c r="AF43" s="21"/>
+      <c r="T43" s="60"/>
+      <c r="U43" s="60"/>
+      <c r="V43" s="60"/>
+      <c r="W43" s="60"/>
+      <c r="X43" s="60"/>
+      <c r="Y43" s="60"/>
+      <c r="Z43" s="60"/>
+      <c r="AA43" s="60"/>
+      <c r="AB43" s="60"/>
+      <c r="AC43" s="60"/>
+      <c r="AD43" s="60"/>
+      <c r="AE43" s="60"/>
+      <c r="AF43" s="60"/>
       <c r="AG43" s="2"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19" t="s">
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19" t="s">
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19" t="s">
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
       <c r="N44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="O44" s="14"/>
       <c r="P44" s="5"/>
       <c r="R44" s="9"/>
-      <c r="S44" s="19" t="s">
+      <c r="S44" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19" t="s">
+      <c r="T44" s="62"/>
+      <c r="U44" s="62"/>
+      <c r="V44" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="19" t="s">
+      <c r="W44" s="62"/>
+      <c r="X44" s="62"/>
+      <c r="Y44" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="Z44" s="19"/>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="19" t="s">
+      <c r="Z44" s="62"/>
+      <c r="AA44" s="62"/>
+      <c r="AB44" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="AC44" s="19"/>
-      <c r="AD44" s="19"/>
-      <c r="AE44" s="19" t="s">
+      <c r="AC44" s="62"/>
+      <c r="AD44" s="62"/>
+      <c r="AE44" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="AF44" s="19"/>
-      <c r="AG44" s="20"/>
+      <c r="AF44" s="62"/>
+      <c r="AG44" s="63"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
@@ -5384,95 +7519,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="60"/>
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="60"/>
+      <c r="AF1" s="60"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19" t="s">
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19" t="s">
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="20"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="63"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17" t="s">
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17" t="s">
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17" t="s">
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="18"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="59"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -6241,51 +8376,51 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19" t="s">
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19" t="s">
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19" t="s">
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="19"/>
-      <c r="P23" s="20"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="63"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>

</xml_diff>

<commit_message>
More Question analysis. Generated infos for online and lab questions distances (mean, std dev).
</commit_message>
<xml_diff>
--- a/Analysis/First Study/centroids_allquestions.xlsx
+++ b/Analysis/First Study/centroids_allquestions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16360" windowHeight="15160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Laboratory &amp; Online" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="93">
   <si>
     <t>Question 1</t>
   </si>
@@ -304,6 +304,9 @@
   <si>
     <t>Medias distancias à resposta ideal</t>
   </si>
+  <si>
+    <t>Desvio Padrão distancias à resposta ideal</t>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -357,6 +360,25 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="15">
@@ -683,7 +705,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -932,19 +954,21 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -953,7 +977,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -968,91 +1004,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1088,22 +1058,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -1417,12 +1452,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC83"/>
+  <dimension ref="A1:BC82"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A56" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="118" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="N70" sqref="N70"/>
+      <selection pane="topRight" activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,65 +1468,65 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="130" t="s">
+      <c r="B1" s="139" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="130"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="139"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131" t="s">
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131" t="s">
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131" t="s">
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="131"/>
-      <c r="M2" s="131"/>
-      <c r="N2" s="131" t="s">
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="131"/>
-      <c r="P2" s="132"/>
-      <c r="T2" s="134" t="s">
+      <c r="O2" s="147"/>
+      <c r="P2" s="153"/>
+      <c r="T2" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="134"/>
-      <c r="V2" s="134"/>
-      <c r="W2" s="134"/>
-      <c r="X2" s="134"/>
-      <c r="Y2" s="134" t="s">
+      <c r="U2" s="152"/>
+      <c r="V2" s="152"/>
+      <c r="W2" s="152"/>
+      <c r="X2" s="152"/>
+      <c r="Y2" s="152" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="134"/>
-      <c r="AA2" s="134"/>
-      <c r="AB2" s="134"/>
-      <c r="AC2" s="134"/>
+      <c r="Z2" s="152"/>
+      <c r="AA2" s="152"/>
+      <c r="AB2" s="152"/>
+      <c r="AC2" s="152"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -2237,95 +2272,95 @@
     <row r="21" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="130" t="s">
+      <c r="B22" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="130"/>
-      <c r="D22" s="130"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
-      <c r="G22" s="130"/>
-      <c r="H22" s="130"/>
-      <c r="I22" s="130"/>
-      <c r="J22" s="130"/>
-      <c r="K22" s="130"/>
-      <c r="L22" s="130"/>
-      <c r="M22" s="130"/>
-      <c r="N22" s="130"/>
-      <c r="O22" s="130"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="139"/>
+      <c r="J22" s="139"/>
+      <c r="K22" s="139"/>
+      <c r="L22" s="139"/>
+      <c r="M22" s="139"/>
+      <c r="N22" s="139"/>
+      <c r="O22" s="139"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="133" t="s">
+      <c r="S22" s="145" t="s">
         <v>60</v>
       </c>
-      <c r="T22" s="133"/>
-      <c r="U22" s="133"/>
-      <c r="V22" s="133"/>
-      <c r="W22" s="133"/>
-      <c r="X22" s="133"/>
-      <c r="Y22" s="133"/>
-      <c r="Z22" s="133"/>
-      <c r="AA22" s="133"/>
-      <c r="AB22" s="133"/>
-      <c r="AC22" s="133"/>
-      <c r="AD22" s="133"/>
-      <c r="AE22" s="133"/>
-      <c r="AF22" s="133"/>
+      <c r="T22" s="145"/>
+      <c r="U22" s="145"/>
+      <c r="V22" s="145"/>
+      <c r="W22" s="145"/>
+      <c r="X22" s="145"/>
+      <c r="Y22" s="145"/>
+      <c r="Z22" s="145"/>
+      <c r="AA22" s="145"/>
+      <c r="AB22" s="145"/>
+      <c r="AC22" s="145"/>
+      <c r="AD22" s="145"/>
+      <c r="AE22" s="145"/>
+      <c r="AF22" s="145"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="135"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="135" t="s">
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="135"/>
-      <c r="G23" s="135"/>
-      <c r="H23" s="135" t="s">
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="135"/>
-      <c r="J23" s="135"/>
-      <c r="K23" s="135" t="s">
+      <c r="I23" s="141"/>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="135"/>
-      <c r="M23" s="135"/>
-      <c r="N23" s="135" t="s">
+      <c r="L23" s="141"/>
+      <c r="M23" s="141"/>
+      <c r="N23" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="135"/>
-      <c r="P23" s="136"/>
+      <c r="O23" s="141"/>
+      <c r="P23" s="142"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="135" t="s">
+      <c r="S23" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="135"/>
-      <c r="U23" s="135"/>
-      <c r="V23" s="135" t="s">
+      <c r="T23" s="141"/>
+      <c r="U23" s="141"/>
+      <c r="V23" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="135"/>
-      <c r="X23" s="135"/>
-      <c r="Y23" s="135" t="s">
+      <c r="W23" s="141"/>
+      <c r="X23" s="141"/>
+      <c r="Y23" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="135"/>
-      <c r="AA23" s="135"/>
-      <c r="AB23" s="135" t="s">
+      <c r="Z23" s="141"/>
+      <c r="AA23" s="141"/>
+      <c r="AB23" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="135"/>
-      <c r="AD23" s="135"/>
-      <c r="AE23" s="135" t="s">
+      <c r="AC23" s="141"/>
+      <c r="AD23" s="141"/>
+      <c r="AE23" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="135"/>
-      <c r="AG23" s="136"/>
+      <c r="AF23" s="141"/>
+      <c r="AG23" s="142"/>
     </row>
     <row r="24" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -3409,159 +3444,159 @@
     <row r="42" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="133"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="133"/>
-      <c r="F43" s="133"/>
-      <c r="G43" s="133"/>
-      <c r="H43" s="133"/>
-      <c r="I43" s="133"/>
-      <c r="J43" s="133"/>
-      <c r="K43" s="133"/>
-      <c r="L43" s="133"/>
-      <c r="M43" s="133"/>
-      <c r="N43" s="133"/>
-      <c r="O43" s="133"/>
-      <c r="P43" s="133"/>
+      <c r="C43" s="145"/>
+      <c r="D43" s="145"/>
+      <c r="E43" s="145"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="145"/>
+      <c r="I43" s="145"/>
+      <c r="J43" s="145"/>
+      <c r="K43" s="145"/>
+      <c r="L43" s="145"/>
+      <c r="M43" s="145"/>
+      <c r="N43" s="145"/>
+      <c r="O43" s="145"/>
+      <c r="P43" s="145"/>
       <c r="Q43" s="46"/>
       <c r="R43" s="46"/>
       <c r="S43" s="47"/>
-      <c r="T43" s="137" t="s">
+      <c r="T43" s="144" t="s">
         <v>62</v>
       </c>
-      <c r="U43" s="133"/>
-      <c r="V43" s="133"/>
-      <c r="W43" s="133"/>
-      <c r="X43" s="133"/>
-      <c r="Y43" s="133"/>
-      <c r="Z43" s="133"/>
-      <c r="AA43" s="133"/>
-      <c r="AB43" s="133"/>
-      <c r="AC43" s="133"/>
-      <c r="AD43" s="133"/>
-      <c r="AE43" s="133"/>
-      <c r="AF43" s="133"/>
-      <c r="AG43" s="133"/>
-      <c r="AH43" s="133"/>
+      <c r="U43" s="145"/>
+      <c r="V43" s="145"/>
+      <c r="W43" s="145"/>
+      <c r="X43" s="145"/>
+      <c r="Y43" s="145"/>
+      <c r="Z43" s="145"/>
+      <c r="AA43" s="145"/>
+      <c r="AB43" s="145"/>
+      <c r="AC43" s="145"/>
+      <c r="AD43" s="145"/>
+      <c r="AE43" s="145"/>
+      <c r="AF43" s="145"/>
+      <c r="AG43" s="145"/>
+      <c r="AH43" s="145"/>
       <c r="AI43" s="46"/>
       <c r="AJ43" s="46"/>
       <c r="AK43" s="47"/>
-      <c r="AL43" s="137" t="s">
+      <c r="AL43" s="144" t="s">
         <v>63</v>
       </c>
-      <c r="AM43" s="133"/>
-      <c r="AN43" s="133"/>
-      <c r="AO43" s="133"/>
-      <c r="AP43" s="133"/>
-      <c r="AQ43" s="133"/>
-      <c r="AR43" s="133"/>
-      <c r="AS43" s="133"/>
-      <c r="AT43" s="133"/>
-      <c r="AU43" s="133"/>
-      <c r="AV43" s="133"/>
-      <c r="AW43" s="133"/>
-      <c r="AX43" s="133"/>
-      <c r="AY43" s="133"/>
-      <c r="AZ43" s="133"/>
+      <c r="AM43" s="145"/>
+      <c r="AN43" s="145"/>
+      <c r="AO43" s="145"/>
+      <c r="AP43" s="145"/>
+      <c r="AQ43" s="145"/>
+      <c r="AR43" s="145"/>
+      <c r="AS43" s="145"/>
+      <c r="AT43" s="145"/>
+      <c r="AU43" s="145"/>
+      <c r="AV43" s="145"/>
+      <c r="AW43" s="145"/>
+      <c r="AX43" s="145"/>
+      <c r="AY43" s="145"/>
+      <c r="AZ43" s="145"/>
       <c r="BA43" s="48"/>
       <c r="BB43" s="48"/>
       <c r="BC43" s="49"/>
     </row>
     <row r="44" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
-      <c r="B44" s="141" t="s">
+      <c r="B44" s="151" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="141"/>
-      <c r="D44" s="141"/>
-      <c r="E44" s="138" t="s">
+      <c r="C44" s="151"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="138"/>
-      <c r="G44" s="138"/>
-      <c r="H44" s="138" t="s">
+      <c r="F44" s="148"/>
+      <c r="G44" s="148"/>
+      <c r="H44" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="I44" s="138"/>
-      <c r="J44" s="138"/>
-      <c r="K44" s="139" t="s">
+      <c r="I44" s="148"/>
+      <c r="J44" s="148"/>
+      <c r="K44" s="149" t="s">
         <v>19</v>
       </c>
-      <c r="L44" s="135"/>
-      <c r="M44" s="140"/>
-      <c r="N44" s="138" t="s">
+      <c r="L44" s="141"/>
+      <c r="M44" s="150"/>
+      <c r="N44" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="O44" s="138"/>
-      <c r="P44" s="138"/>
-      <c r="Q44" s="135" t="s">
+      <c r="O44" s="148"/>
+      <c r="P44" s="148"/>
+      <c r="Q44" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="R44" s="135"/>
-      <c r="S44" s="136"/>
-      <c r="T44" s="142" t="s">
+      <c r="R44" s="141"/>
+      <c r="S44" s="142"/>
+      <c r="T44" s="146" t="s">
         <v>54</v>
       </c>
-      <c r="U44" s="131"/>
-      <c r="V44" s="131"/>
-      <c r="W44" s="135" t="s">
+      <c r="U44" s="147"/>
+      <c r="V44" s="147"/>
+      <c r="W44" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="X44" s="135"/>
-      <c r="Y44" s="135"/>
-      <c r="Z44" s="135" t="s">
+      <c r="X44" s="141"/>
+      <c r="Y44" s="141"/>
+      <c r="Z44" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="AA44" s="135"/>
-      <c r="AB44" s="135"/>
-      <c r="AC44" s="135" t="s">
+      <c r="AA44" s="141"/>
+      <c r="AB44" s="141"/>
+      <c r="AC44" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="AD44" s="135"/>
-      <c r="AE44" s="135"/>
-      <c r="AF44" s="135" t="s">
+      <c r="AD44" s="141"/>
+      <c r="AE44" s="141"/>
+      <c r="AF44" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AG44" s="135"/>
-      <c r="AH44" s="135"/>
-      <c r="AI44" s="135" t="s">
+      <c r="AG44" s="141"/>
+      <c r="AH44" s="141"/>
+      <c r="AI44" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="AJ44" s="135"/>
-      <c r="AK44" s="136"/>
+      <c r="AJ44" s="141"/>
+      <c r="AK44" s="142"/>
       <c r="AL44" s="143" t="s">
         <v>54</v>
       </c>
-      <c r="AM44" s="135"/>
-      <c r="AN44" s="135"/>
-      <c r="AO44" s="135" t="s">
+      <c r="AM44" s="141"/>
+      <c r="AN44" s="141"/>
+      <c r="AO44" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="AP44" s="135"/>
-      <c r="AQ44" s="135"/>
-      <c r="AR44" s="135" t="s">
+      <c r="AP44" s="141"/>
+      <c r="AQ44" s="141"/>
+      <c r="AR44" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="AS44" s="135"/>
-      <c r="AT44" s="135"/>
-      <c r="AU44" s="135" t="s">
+      <c r="AS44" s="141"/>
+      <c r="AT44" s="141"/>
+      <c r="AU44" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="AV44" s="135"/>
-      <c r="AW44" s="135"/>
-      <c r="AX44" s="135" t="s">
+      <c r="AV44" s="141"/>
+      <c r="AW44" s="141"/>
+      <c r="AX44" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AY44" s="135"/>
-      <c r="AZ44" s="135"/>
-      <c r="BA44" s="135" t="s">
+      <c r="AY44" s="141"/>
+      <c r="AZ44" s="141"/>
+      <c r="BA44" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="BB44" s="135"/>
-      <c r="BC44" s="136"/>
+      <c r="BB44" s="141"/>
+      <c r="BC44" s="142"/>
     </row>
     <row r="45" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
@@ -5350,37 +5385,63 @@
     </row>
     <row r="64" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="130" t="s">
+      <c r="B64" s="139" t="s">
         <v>91</v>
       </c>
-      <c r="C64" s="130"/>
-      <c r="D64" s="130"/>
-      <c r="E64" s="130"/>
-      <c r="F64" s="130"/>
-      <c r="G64" s="130"/>
-      <c r="H64" s="130"/>
-      <c r="I64" s="130"/>
-      <c r="J64" s="130"/>
-      <c r="K64" s="182"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C64" s="139"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="139"/>
+      <c r="F64" s="139"/>
+      <c r="G64" s="139"/>
+      <c r="H64" s="139"/>
+      <c r="I64" s="139"/>
+      <c r="J64" s="139"/>
+      <c r="K64" s="140"/>
+      <c r="L64" s="139" t="s">
+        <v>92</v>
+      </c>
+      <c r="M64" s="139"/>
+      <c r="N64" s="139"/>
+      <c r="O64" s="139"/>
+      <c r="P64" s="139"/>
+      <c r="Q64" s="139"/>
+      <c r="R64" s="139"/>
+      <c r="S64" s="139"/>
+      <c r="T64" s="139"/>
+      <c r="U64" s="140"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-      <c r="B65" s="186" t="s">
+      <c r="B65" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="130"/>
-      <c r="D65" s="130"/>
-      <c r="E65" s="130"/>
-      <c r="F65" s="182"/>
-      <c r="G65" s="186" t="s">
+      <c r="C65" s="139"/>
+      <c r="D65" s="139"/>
+      <c r="E65" s="139"/>
+      <c r="F65" s="140"/>
+      <c r="G65" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="H65" s="130"/>
-      <c r="I65" s="130"/>
-      <c r="J65" s="130"/>
-      <c r="K65" s="182"/>
-    </row>
-    <row r="66" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="139"/>
+      <c r="I65" s="139"/>
+      <c r="J65" s="139"/>
+      <c r="K65" s="140"/>
+      <c r="L65" s="139" t="s">
+        <v>89</v>
+      </c>
+      <c r="M65" s="139"/>
+      <c r="N65" s="139"/>
+      <c r="O65" s="139"/>
+      <c r="P65" s="140"/>
+      <c r="Q65" s="139" t="s">
+        <v>90</v>
+      </c>
+      <c r="R65" s="139"/>
+      <c r="S65" s="139"/>
+      <c r="T65" s="139"/>
+      <c r="U65" s="140"/>
+    </row>
+    <row r="66" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
         <v>17</v>
@@ -5397,7 +5458,7 @@
       <c r="F66" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G66" s="6" t="s">
+      <c r="G66" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H66" s="7" t="s">
@@ -5412,646 +5473,990 @@
       <c r="K66" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="184" t="s">
+      <c r="L66" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M66" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N66" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O66" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P66" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q66" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R66" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S66" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T66" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U66" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A67" s="130" t="s">
         <v>0</v>
       </c>
       <c r="B67" s="1">
         <v>0.13</v>
       </c>
-      <c r="C67" s="187">
+      <c r="C67" s="131">
         <v>0.2</v>
       </c>
-      <c r="D67" s="193">
+      <c r="D67" s="137">
         <v>0.09</v>
       </c>
-      <c r="E67" s="188">
+      <c r="E67" s="132">
         <v>0.12</v>
       </c>
       <c r="F67" s="2">
         <v>0.12</v>
       </c>
-      <c r="G67" s="183">
-        <f>AVERAGE(G14:G66)</f>
-        <v>0.15279202439024392</v>
-      </c>
-      <c r="H67" s="183">
-        <f t="shared" ref="H67:K67" si="0">AVERAGE(H14:H66)</f>
-        <v>0.20163529411764708</v>
-      </c>
-      <c r="I67" s="183">
-        <f t="shared" si="0"/>
-        <v>0.19058823529411764</v>
-      </c>
-      <c r="J67" s="183">
-        <f t="shared" si="0"/>
-        <v>0.10881390243902438</v>
-      </c>
-      <c r="K67" s="183">
-        <f t="shared" si="0"/>
-        <v>0.10741176470588235</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" s="184" t="s">
+      <c r="G67" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H67" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="I67" s="199">
+        <v>0.06</v>
+      </c>
+      <c r="J67" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K67" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L67" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="M67" s="205">
+        <v>0.06</v>
+      </c>
+      <c r="N67" s="205">
+        <v>0.06</v>
+      </c>
+      <c r="O67" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="P67" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="Q67" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="R67" s="193">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S67" s="198">
+        <v>0.06</v>
+      </c>
+      <c r="T67" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="U67" s="194">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A68" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="B68" s="3">
-        <f>MEDIAN(B53:B67)</f>
-        <v>0.49</v>
-      </c>
-      <c r="C68" s="4">
-        <f t="shared" ref="C68:F68" si="1">MEDIAN(C53:C67)</f>
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="D68" s="4">
-        <f t="shared" si="1"/>
-        <v>0.22001000000000001</v>
-      </c>
-      <c r="E68" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1186</v>
-      </c>
-      <c r="F68" s="5">
-        <f t="shared" si="1"/>
+      <c r="B68" s="192">
+        <v>0.22</v>
+      </c>
+      <c r="C68" s="193">
+        <v>0.16</v>
+      </c>
+      <c r="D68" s="198">
+        <v>0.11</v>
+      </c>
+      <c r="E68" s="193">
+        <v>0.17</v>
+      </c>
+      <c r="F68" s="194">
+        <v>0.16</v>
+      </c>
+      <c r="G68" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="H68" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="I68" s="199">
+        <v>0.08</v>
+      </c>
+      <c r="J68" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="K68" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="L68" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="M68" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="N68" s="198">
+        <v>0.06</v>
+      </c>
+      <c r="O68" s="193">
+        <v>0.11</v>
+      </c>
+      <c r="P68" s="194">
+        <v>0.08</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="R68" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="S68" s="199">
+        <v>0.04</v>
+      </c>
+      <c r="T68" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="U68" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A69" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="200">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0.215</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E69" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G68" s="10">
+      <c r="F69" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="G69" s="199">
+        <v>0.04</v>
+      </c>
+      <c r="H69" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="I69" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="J69" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="K69" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="L69" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="M69" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="N69" s="199">
+        <v>0.03</v>
+      </c>
+      <c r="O69" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="P69" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="Q69" s="193">
         <v>0.09</v>
       </c>
-      <c r="H68" s="10">
+      <c r="R69" s="193">
+        <v>0.06</v>
+      </c>
+      <c r="S69" s="198">
+        <v>0.03</v>
+      </c>
+      <c r="T69" s="193">
+        <v>0.06</v>
+      </c>
+      <c r="U69" s="194">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A70" s="130" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="C70" s="133"/>
+      <c r="D70" s="133"/>
+      <c r="E70" s="133"/>
+      <c r="F70" s="134"/>
+      <c r="G70" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="H70" s="135"/>
+      <c r="I70" s="135"/>
+      <c r="J70" s="135"/>
+      <c r="K70" s="136"/>
+      <c r="L70" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="M70" s="133"/>
+      <c r="N70" s="133"/>
+      <c r="O70" s="133"/>
+      <c r="P70" s="134"/>
+      <c r="Q70" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="R70" s="135"/>
+      <c r="S70" s="135"/>
+      <c r="T70" s="135"/>
+      <c r="U70" s="136"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A71" s="130" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="3">
         <v>0.17</v>
       </c>
-      <c r="I68" s="10">
+      <c r="C71" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D71" s="199">
+        <v>0.13</v>
+      </c>
+      <c r="E71" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F71" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G71" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="H71" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="I71" s="199">
+        <v>0.13</v>
+      </c>
+      <c r="J71" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K71" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="L71" s="193">
+        <v>0.1</v>
+      </c>
+      <c r="M71" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="N71" s="198">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J68" s="10">
+      <c r="O71" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="P71" s="194">
+        <v>0.08</v>
+      </c>
+      <c r="Q71" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="R71" s="193">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S71" s="198">
+        <v>0.06</v>
+      </c>
+      <c r="T71" s="193">
         <v>0.1</v>
       </c>
-      <c r="K68" s="11">
+      <c r="U71" s="194">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A72" s="130" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="195">
+        <v>7.4090909090909096E-2</v>
+      </c>
+      <c r="C72" s="196">
+        <v>0.13318181818181818</v>
+      </c>
+      <c r="D72" s="196">
+        <v>5.7727272727272738E-2</v>
+      </c>
+      <c r="E72" s="196">
+        <v>7.7727272727272756E-2</v>
+      </c>
+      <c r="F72" s="201">
+        <v>5.0909090909090911E-2</v>
+      </c>
+      <c r="G72" s="196">
+        <v>3.0136986301369861E-2</v>
+      </c>
+      <c r="H72" s="196">
+        <v>0.13643835616438363</v>
+      </c>
+      <c r="I72" s="196">
+        <v>3.3150684931506844E-2</v>
+      </c>
+      <c r="J72" s="196">
+        <v>3.9863013698630129E-2</v>
+      </c>
+      <c r="K72" s="201">
+        <v>2.3561643835616451E-2</v>
+      </c>
+      <c r="L72" s="193">
+        <v>0.1</v>
+      </c>
+      <c r="M72" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="N72" s="198">
+        <v>0.06</v>
+      </c>
+      <c r="O72" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="P72" s="194">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q72" s="193">
+        <v>0.05</v>
+      </c>
+      <c r="R72" s="193">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S72" s="198">
+        <v>0.03</v>
+      </c>
+      <c r="T72" s="193">
+        <v>0.05</v>
+      </c>
+      <c r="U72" s="206">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A73" s="130" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="195">
+        <v>0.15772727272727274</v>
+      </c>
+      <c r="C73" s="196">
+        <v>0.23227272727272724</v>
+      </c>
+      <c r="D73" s="202">
+        <v>9.8636363636363647E-2</v>
+      </c>
+      <c r="E73" s="196">
+        <v>0.14545454545454548</v>
+      </c>
+      <c r="F73" s="197">
+        <v>0.17045454545454544</v>
+      </c>
+      <c r="G73" s="196">
+        <v>0.12815789473684203</v>
+      </c>
+      <c r="H73" s="196">
+        <v>0.18447368421052621</v>
+      </c>
+      <c r="I73" s="202">
+        <v>0.11473684210526321</v>
+      </c>
+      <c r="J73" s="196">
+        <v>0.16723684210526321</v>
+      </c>
+      <c r="K73" s="197">
+        <v>0.2152631578947368</v>
+      </c>
+      <c r="L73" s="193">
+        <v>0.21</v>
+      </c>
+      <c r="M73" s="193">
+        <v>0.1</v>
+      </c>
+      <c r="N73" s="198">
+        <v>0.08</v>
+      </c>
+      <c r="O73" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="P73" s="206">
+        <v>0.08</v>
+      </c>
+      <c r="Q73" s="193">
+        <v>0.21</v>
+      </c>
+      <c r="R73" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="S73" s="198">
+        <v>0.06</v>
+      </c>
+      <c r="T73" s="193">
+        <v>0.11</v>
+      </c>
+      <c r="U73" s="194">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A74" s="130" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="203">
+        <v>9.5384615384615401E-2</v>
+      </c>
+      <c r="C74" s="196">
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="D74" s="202">
+        <v>0.10076923076923078</v>
+      </c>
+      <c r="E74" s="196">
+        <v>0.12923076923076923</v>
+      </c>
+      <c r="F74" s="197">
+        <v>0.12923076923076923</v>
+      </c>
+      <c r="G74" s="196">
+        <v>0.1009677419354838</v>
+      </c>
+      <c r="H74" s="202">
+        <v>9.0806451612903211E-2</v>
+      </c>
+      <c r="I74" s="196">
+        <v>0.11838709677419348</v>
+      </c>
+      <c r="J74" s="196">
+        <v>0.14338709677419362</v>
+      </c>
+      <c r="K74" s="197">
+        <v>0.16387096774193544</v>
+      </c>
+      <c r="L74" s="193">
+        <v>0.16</v>
+      </c>
+      <c r="M74" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="N74" s="198">
+        <v>0.05</v>
+      </c>
+      <c r="O74" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="P74" s="194">
+        <v>0.09</v>
+      </c>
+      <c r="Q74" s="196">
+        <v>0.16936438239584437</v>
+      </c>
+      <c r="R74" s="196">
+        <v>0.1198400352805981</v>
+      </c>
+      <c r="S74" s="202">
+        <v>4.8727867557271667E-2</v>
+      </c>
+      <c r="T74" s="196">
+        <v>7.0430608761031466E-2</v>
+      </c>
+      <c r="U74" s="197">
+        <v>6.7831876028940266E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A75" s="130" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="195">
+        <v>0.12578947368421051</v>
+      </c>
+      <c r="C75" s="196">
+        <v>0.16421052631578945</v>
+      </c>
+      <c r="D75" s="202">
+        <v>9.1052631578947399E-2</v>
+      </c>
+      <c r="E75" s="196">
+        <v>0.1005263157894737</v>
+      </c>
+      <c r="F75" s="197">
+        <v>0.11421052631578947</v>
+      </c>
+      <c r="G75" s="196">
+        <v>0.10831168831168823</v>
+      </c>
+      <c r="H75" s="196">
+        <v>0.12740259740259738</v>
+      </c>
+      <c r="I75" s="202">
+        <v>0.10103896103896103</v>
+      </c>
+      <c r="J75" s="202">
+        <v>9.9480519480519419E-2</v>
+      </c>
+      <c r="K75" s="197">
+        <v>0.1109090909090909</v>
+      </c>
+      <c r="L75" s="193">
+        <v>0.1</v>
+      </c>
+      <c r="M75" s="193">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N75" s="198">
+        <v>0.05</v>
+      </c>
+      <c r="O75" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="P75" s="194">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q75" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="R75" s="193">
+        <v>0.06</v>
+      </c>
+      <c r="S75" s="198">
+        <v>0.04</v>
+      </c>
+      <c r="T75" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="U75" s="194">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A76" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="195">
+        <v>0.3</v>
+      </c>
+      <c r="C76" s="196">
+        <v>0.25571428571428573</v>
+      </c>
+      <c r="D76" s="202">
+        <v>0.13142857142857142</v>
+      </c>
+      <c r="E76" s="196">
+        <v>0.21071428571428569</v>
+      </c>
+      <c r="F76" s="197">
+        <v>0.20428571428571424</v>
+      </c>
+      <c r="G76" s="196">
+        <v>0.16923076923076918</v>
+      </c>
+      <c r="H76" s="196">
+        <v>0.26846153846153853</v>
+      </c>
+      <c r="I76" s="202">
+        <v>0.13326923076923075</v>
+      </c>
+      <c r="J76" s="196">
+        <v>0.2046153846153847</v>
+      </c>
+      <c r="K76" s="197">
+        <v>0.21846153846153843</v>
+      </c>
+      <c r="L76" s="193">
+        <v>0.16</v>
+      </c>
+      <c r="M76" s="193">
+        <v>0.12</v>
+      </c>
+      <c r="N76" s="198">
+        <v>0.05</v>
+      </c>
+      <c r="O76" s="193">
+        <v>0.06</v>
+      </c>
+      <c r="P76" s="194">
+        <v>0.1</v>
+      </c>
+      <c r="Q76" s="193">
+        <v>0.17</v>
+      </c>
+      <c r="R76" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="S76" s="198">
+        <v>0.04</v>
+      </c>
+      <c r="T76" s="198">
+        <v>0.04</v>
+      </c>
+      <c r="U76" s="194">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A77" s="130" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="204">
+        <v>0.06</v>
+      </c>
+      <c r="C77" s="135"/>
+      <c r="D77" s="135"/>
+      <c r="E77" s="135"/>
+      <c r="F77" s="136"/>
+      <c r="G77" s="205">
+        <v>0.04</v>
+      </c>
+      <c r="H77" s="135"/>
+      <c r="I77" s="135"/>
+      <c r="J77" s="135"/>
+      <c r="K77" s="136"/>
+      <c r="L77" s="205">
+        <v>0.09</v>
+      </c>
+      <c r="M77" s="135"/>
+      <c r="N77" s="135"/>
+      <c r="O77" s="135"/>
+      <c r="P77" s="136"/>
+      <c r="Q77" s="205">
+        <v>0.06</v>
+      </c>
+      <c r="R77" s="135"/>
+      <c r="S77" s="135"/>
+      <c r="T77" s="135"/>
+      <c r="U77" s="136"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A78" s="130" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" s="203">
+        <v>0.10666666666666667</v>
+      </c>
+      <c r="C78" s="196">
+        <v>0.23428571428571432</v>
+      </c>
+      <c r="D78" s="196">
+        <v>0.13142857142857145</v>
+      </c>
+      <c r="E78" s="196">
+        <v>0.15095238095238095</v>
+      </c>
+      <c r="F78" s="197">
+        <v>0.17428571428571429</v>
+      </c>
+      <c r="G78" s="202">
+        <v>7.6478873239436612E-2</v>
+      </c>
+      <c r="H78" s="196">
+        <v>0.24436619718309871</v>
+      </c>
+      <c r="I78" s="196">
+        <v>0.11619718309859157</v>
+      </c>
+      <c r="J78" s="196">
+        <v>0.12929577464788722</v>
+      </c>
+      <c r="K78" s="197">
+        <v>0.14845070422535211</v>
+      </c>
+      <c r="L78" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="M78" s="193">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N78" s="198">
+        <v>0.04</v>
+      </c>
+      <c r="O78" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="P78" s="194">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q78" s="193">
+        <v>0.11</v>
+      </c>
+      <c r="R78" s="193">
+        <v>0.06</v>
+      </c>
+      <c r="S78" s="198">
+        <v>0.05</v>
+      </c>
+      <c r="T78" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="U78" s="194">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A79" s="130" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="195">
+        <v>0.27124999999999999</v>
+      </c>
+      <c r="C79" s="202">
+        <v>0.16625000000000004</v>
+      </c>
+      <c r="D79" s="196">
+        <v>0.18749999999999997</v>
+      </c>
+      <c r="E79" s="196">
+        <v>0.245</v>
+      </c>
+      <c r="F79" s="197">
+        <v>0.22687500000000002</v>
+      </c>
+      <c r="G79" s="196">
+        <v>0.1443396226415094</v>
+      </c>
+      <c r="H79" s="196">
+        <v>0.19867924528301883</v>
+      </c>
+      <c r="I79" s="196">
+        <v>0.13962264150943396</v>
+      </c>
+      <c r="J79" s="202">
+        <v>0.12773584905660376</v>
+      </c>
+      <c r="K79" s="197">
+        <v>0.14471698113207548</v>
+      </c>
+      <c r="L79" s="193">
+        <v>0.16</v>
+      </c>
+      <c r="M79" s="198">
+        <v>0.1</v>
+      </c>
+      <c r="N79" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="O79" s="193">
+        <v>0.16</v>
+      </c>
+      <c r="P79" s="194">
+        <v>0.12</v>
+      </c>
+      <c r="Q79" s="193">
+        <v>0.16</v>
+      </c>
+      <c r="R79" s="198">
+        <v>0.09</v>
+      </c>
+      <c r="S79" s="193">
+        <v>0.11</v>
+      </c>
+      <c r="T79" s="193">
+        <v>0.15</v>
+      </c>
+      <c r="U79" s="194">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A80" s="130" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" s="195">
+        <v>0.11863636363636361</v>
+      </c>
+      <c r="C80" s="196">
+        <v>0.2995454545454545</v>
+      </c>
+      <c r="D80" s="202">
+        <v>9.7272727272727302E-2</v>
+      </c>
+      <c r="E80" s="196">
+        <v>0.13272727272727269</v>
+      </c>
+      <c r="F80" s="197">
+        <v>0.13363636363636364</v>
+      </c>
+      <c r="G80" s="196">
+        <v>9.9506172839506066E-2</v>
+      </c>
+      <c r="H80" s="196">
+        <v>0.29185185185185197</v>
+      </c>
+      <c r="I80" s="202">
+        <v>9.3580246913580231E-2</v>
+      </c>
+      <c r="J80" s="196">
+        <v>0.11481481481481479</v>
+      </c>
+      <c r="K80" s="197">
+        <v>0.12333333333333327</v>
+      </c>
+      <c r="L80" s="193">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="184" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" s="3">
-        <f>MEDIAN(B47:B68)</f>
-        <v>0.49</v>
-      </c>
-      <c r="C69" s="4">
-        <f t="shared" ref="C69:E69" si="2">MEDIAN(C47:C68)</f>
-        <v>0.53750000000000009</v>
-      </c>
-      <c r="D69" s="4">
-        <f t="shared" si="2"/>
-        <v>0.22001000000000001</v>
-      </c>
-      <c r="E69" s="4">
-        <f t="shared" si="2"/>
-        <v>0.1186</v>
-      </c>
-      <c r="F69" s="5">
-        <f>MEDIAN(F47:F68)</f>
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="G69" s="10">
+      <c r="M80" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="N80" s="198">
+        <v>0.05</v>
+      </c>
+      <c r="O80" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="P80" s="194">
+        <v>0.09</v>
+      </c>
+      <c r="Q80" s="193">
+        <v>0.12</v>
+      </c>
+      <c r="R80" s="193">
+        <v>0.13</v>
+      </c>
+      <c r="S80" s="198">
+        <v>0.05</v>
+      </c>
+      <c r="T80" s="193">
+        <v>0.12</v>
+      </c>
+      <c r="U80" s="194">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A81" s="130" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81" s="195">
+        <v>9.0000000000000024E-2</v>
+      </c>
+      <c r="C81" s="196">
+        <v>0.30312500000000003</v>
+      </c>
+      <c r="D81" s="202">
+        <v>6.2500000000000014E-2</v>
+      </c>
+      <c r="E81" s="196">
+        <v>0.11000000000000003</v>
+      </c>
+      <c r="F81" s="197">
+        <v>0.12562500000000001</v>
+      </c>
+      <c r="G81" s="196">
+        <v>0.11291666666666662</v>
+      </c>
+      <c r="H81" s="196">
+        <v>0.30402777777777779</v>
+      </c>
+      <c r="I81" s="202">
+        <v>6.2083333333333331E-2</v>
+      </c>
+      <c r="J81" s="196">
+        <v>0.11222222222222222</v>
+      </c>
+      <c r="K81" s="197">
+        <v>0.12527777777777777</v>
+      </c>
+      <c r="L81" s="193">
         <v>0.04</v>
       </c>
-      <c r="H69" s="10">
+      <c r="M81" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="N81" s="198">
+        <v>0.03</v>
+      </c>
+      <c r="O81" s="193">
+        <v>0.05</v>
+      </c>
+      <c r="P81" s="194">
+        <v>0.06</v>
+      </c>
+      <c r="Q81" s="193">
+        <v>0.08</v>
+      </c>
+      <c r="R81" s="193">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S81" s="198">
+        <v>0.03</v>
+      </c>
+      <c r="T81" s="193">
+        <v>0.04</v>
+      </c>
+      <c r="U81" s="194">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A82" s="130" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82" s="9">
         <v>0.21</v>
       </c>
-      <c r="I69" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="J69" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="K69" s="11">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="184" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="3">
-        <f>MEDIAN(B49:B69)</f>
-        <v>0.49</v>
-      </c>
-      <c r="C70" s="189">
-        <f t="shared" ref="C70:F70" si="3">MEDIAN(C49:C69)</f>
-        <v>0.53750000000000009</v>
-      </c>
-      <c r="D70" s="189">
-        <f t="shared" si="3"/>
-        <v>0.22001000000000001</v>
-      </c>
-      <c r="E70" s="189">
-        <f t="shared" si="3"/>
-        <v>0.1186</v>
-      </c>
-      <c r="F70" s="190">
-        <f t="shared" si="3"/>
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="G70" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="H70" s="191">
-        <v>0.18</v>
-      </c>
-      <c r="I70" s="191">
-        <v>0.215</v>
-      </c>
-      <c r="J70" s="191">
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="K70" s="192">
-        <v>0.22500000000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="C71" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D71" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E71" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="F71" s="11">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="G71" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H71" s="10">
-        <v>0.16</v>
-      </c>
-      <c r="I71" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J71" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="K71" s="11">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="184" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72" s="9">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C72" s="10">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="D72" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="E72" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="F72" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="G72" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="H72" s="10">
-        <v>0.09</v>
-      </c>
-      <c r="I72" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="J72" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="K72" s="11">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="184" t="s">
-        <v>6</v>
-      </c>
-      <c r="B73" s="9">
-        <v>0.06</v>
-      </c>
-      <c r="C73" s="10">
-        <v>0.27</v>
-      </c>
-      <c r="D73" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="E73" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="F73" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="G73" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H73" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="I73" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="J73" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="K73" s="11">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="184" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="C74" s="10">
-        <v>0.17</v>
-      </c>
-      <c r="D74" s="10">
-        <v>0.09</v>
-      </c>
-      <c r="E74" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="F74" s="11">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G74" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H74" s="10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I74" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J74" s="10">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="K74" s="11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="184" t="s">
-        <v>8</v>
-      </c>
-      <c r="B75" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="C75" s="10">
-        <v>0.13</v>
-      </c>
-      <c r="D75" s="10">
-        <v>0.09</v>
-      </c>
-      <c r="E75" s="10">
-        <v>0.08</v>
-      </c>
-      <c r="F75" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="G75" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="H75" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="I75" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="J75" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K75" s="11">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="184" t="s">
-        <v>9</v>
-      </c>
-      <c r="B76" s="9">
-        <v>0.39500000000000002</v>
-      </c>
-      <c r="C76" s="10">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="D76" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="E76" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="F76" s="11">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="G76" s="10">
-        <v>0.09</v>
-      </c>
-      <c r="H76" s="10">
-        <v>0.27</v>
-      </c>
-      <c r="I76" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J76" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="K76" s="11">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="184" t="s">
-        <v>10</v>
-      </c>
-      <c r="B77" s="9">
-        <v>0.03</v>
-      </c>
-      <c r="C77" s="191">
-        <v>0.05</v>
-      </c>
-      <c r="D77" s="191">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E77" s="191">
-        <v>0.2</v>
-      </c>
-      <c r="F77" s="192">
-        <v>0.15</v>
-      </c>
-      <c r="G77" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="H77" s="191">
-        <v>0.06</v>
-      </c>
-      <c r="I77" s="191">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J77" s="191">
-        <v>0.19</v>
-      </c>
-      <c r="K77" s="192">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="184" t="s">
-        <v>11</v>
-      </c>
-      <c r="B78" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="C78" s="10">
-        <v>0.22</v>
-      </c>
-      <c r="D78" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E78" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F78" s="11">
-        <v>0.18</v>
-      </c>
-      <c r="G78" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="H78" s="10">
-        <v>0.22</v>
-      </c>
-      <c r="I78" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="J78" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="K78" s="11">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="184" t="s">
-        <v>12</v>
-      </c>
-      <c r="B79" s="9">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="C79" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D79" s="10">
-        <v>0.215</v>
-      </c>
-      <c r="E79" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="F79" s="11">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="G79" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="H79" s="10">
-        <v>0.17</v>
-      </c>
-      <c r="I79" s="10">
-        <v>0.08</v>
-      </c>
-      <c r="J79" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="K79" s="11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="184" t="s">
-        <v>13</v>
-      </c>
-      <c r="B80" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="C80" s="10">
-        <v>0.315</v>
-      </c>
-      <c r="D80" s="10">
-        <v>0.09</v>
-      </c>
-      <c r="E80" s="10">
-        <v>0.125</v>
-      </c>
-      <c r="F80" s="11">
-        <v>0.13</v>
-      </c>
-      <c r="G80" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="H80" s="10">
-        <v>0.36</v>
-      </c>
-      <c r="I80" s="10">
-        <v>0.09</v>
-      </c>
-      <c r="J80" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="K80" s="11">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="184" t="s">
-        <v>14</v>
-      </c>
-      <c r="B81" s="9">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="C81" s="10">
-        <v>0.31</v>
-      </c>
-      <c r="D81" s="10">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="E81" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="F81" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G81" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="H81" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="I81" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="J81" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="K81" s="11">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="184" t="s">
-        <v>15</v>
-      </c>
-      <c r="B82" s="9">
-        <v>0.23</v>
-      </c>
-      <c r="C82" s="191">
-        <v>0.25</v>
-      </c>
-      <c r="D82" s="191">
-        <v>0.1</v>
-      </c>
-      <c r="E82" s="191">
-        <v>0.17</v>
-      </c>
-      <c r="F82" s="192">
-        <v>0.11</v>
-      </c>
+      <c r="C82" s="135"/>
+      <c r="D82" s="135"/>
+      <c r="E82" s="135"/>
+      <c r="F82" s="136"/>
       <c r="G82" s="10">
         <v>0.19</v>
       </c>
-      <c r="H82" s="191">
-        <v>0.15</v>
-      </c>
-      <c r="I82" s="191">
+      <c r="H82" s="135"/>
+      <c r="I82" s="135"/>
+      <c r="J82" s="135"/>
+      <c r="K82" s="136"/>
+      <c r="L82" s="10">
         <v>0.1</v>
       </c>
-      <c r="J82" s="191">
-        <v>0.17</v>
-      </c>
-      <c r="K82" s="192">
+      <c r="M82" s="135"/>
+      <c r="N82" s="135"/>
+      <c r="O82" s="135"/>
+      <c r="P82" s="136"/>
+      <c r="Q82" s="10">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="185" t="s">
-        <v>16</v>
-      </c>
-      <c r="B83" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="C83" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D83" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="E83" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="F83" s="50">
-        <v>0.11</v>
-      </c>
-      <c r="G83" s="13">
-        <v>0.02</v>
-      </c>
-      <c r="H83" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I83" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="J83" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="K83" s="50">
-        <v>0.12</v>
-      </c>
+      <c r="R82" s="135"/>
+      <c r="S82" s="135"/>
+      <c r="T82" s="135"/>
+      <c r="U82" s="136"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="G65:K65"/>
-    <mergeCell ref="B64:K64"/>
-    <mergeCell ref="BA44:BC44"/>
-    <mergeCell ref="AF44:AH44"/>
-    <mergeCell ref="AI44:AK44"/>
-    <mergeCell ref="AL44:AN44"/>
-    <mergeCell ref="AO44:AQ44"/>
-    <mergeCell ref="AR44:AT44"/>
-    <mergeCell ref="AL43:AZ43"/>
-    <mergeCell ref="AU44:AW44"/>
-    <mergeCell ref="AX44:AZ44"/>
-    <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="T44:V44"/>
-    <mergeCell ref="W44:Y44"/>
-    <mergeCell ref="Z44:AB44"/>
-    <mergeCell ref="AC44:AE44"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B44:D44"/>
+  <mergeCells count="47">
+    <mergeCell ref="L64:U64"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="B43:P43"/>
     <mergeCell ref="T2:X2"/>
     <mergeCell ref="S22:AF22"/>
@@ -6068,12 +6473,30 @@
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="N23:P23"/>
     <mergeCell ref="T43:AH43"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="AL43:AZ43"/>
+    <mergeCell ref="AU44:AW44"/>
+    <mergeCell ref="AX44:AZ44"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="T44:V44"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="Z44:AB44"/>
+    <mergeCell ref="AC44:AE44"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="G65:K65"/>
+    <mergeCell ref="B64:K64"/>
+    <mergeCell ref="BA44:BC44"/>
+    <mergeCell ref="AF44:AH44"/>
+    <mergeCell ref="AI44:AK44"/>
+    <mergeCell ref="AL44:AN44"/>
+    <mergeCell ref="AO44:AQ44"/>
+    <mergeCell ref="AR44:AT44"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="L65:P65"/>
+    <mergeCell ref="Q65:U65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6116,48 +6539,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="155" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="169"/>
-      <c r="H1" s="169"/>
-      <c r="I1" s="169"/>
-      <c r="J1" s="169"/>
-      <c r="K1" s="170"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="157"/>
       <c r="L1" s="65"/>
-      <c r="M1" s="148" t="s">
+      <c r="M1" s="155" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
-      <c r="P1" s="149"/>
-      <c r="Q1" s="149"/>
-      <c r="R1" s="149"/>
-      <c r="S1" s="149"/>
-      <c r="T1" s="149"/>
-      <c r="U1" s="149"/>
-      <c r="V1" s="149"/>
-      <c r="W1" s="149"/>
-      <c r="X1" s="149"/>
-      <c r="Y1" s="149"/>
-      <c r="Z1" s="149"/>
-      <c r="AA1" s="149"/>
-      <c r="AB1" s="149"/>
-      <c r="AC1" s="149"/>
-      <c r="AD1" s="149"/>
-      <c r="AE1" s="149"/>
-      <c r="AF1" s="149"/>
-      <c r="AG1" s="149"/>
-      <c r="AH1" s="149"/>
-      <c r="AI1" s="149"/>
-      <c r="AJ1" s="149"/>
-      <c r="AK1" s="149"/>
-      <c r="AL1" s="150"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
+      <c r="AD1" s="179"/>
+      <c r="AE1" s="179"/>
+      <c r="AF1" s="179"/>
+      <c r="AG1" s="179"/>
+      <c r="AH1" s="179"/>
+      <c r="AI1" s="179"/>
+      <c r="AJ1" s="179"/>
+      <c r="AK1" s="179"/>
+      <c r="AL1" s="180"/>
       <c r="AM1" s="71"/>
       <c r="AN1" s="71"/>
       <c r="AO1" s="71"/>
@@ -6173,44 +6596,44 @@
       <c r="AY1" s="72"/>
     </row>
     <row r="2" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151"/>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
-      <c r="I2" s="171"/>
-      <c r="J2" s="171"/>
-      <c r="K2" s="172"/>
+      <c r="A2" s="158"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="160"/>
       <c r="L2" s="74"/>
-      <c r="M2" s="151"/>
-      <c r="N2" s="152"/>
-      <c r="O2" s="152"/>
-      <c r="P2" s="152"/>
-      <c r="Q2" s="152"/>
-      <c r="R2" s="152"/>
-      <c r="S2" s="152"/>
-      <c r="T2" s="152"/>
-      <c r="U2" s="152"/>
-      <c r="V2" s="152"/>
-      <c r="W2" s="152"/>
-      <c r="X2" s="152"/>
-      <c r="Y2" s="152"/>
-      <c r="Z2" s="152"/>
-      <c r="AA2" s="152"/>
-      <c r="AB2" s="152"/>
-      <c r="AC2" s="152"/>
-      <c r="AD2" s="152"/>
-      <c r="AE2" s="152"/>
-      <c r="AF2" s="152"/>
-      <c r="AG2" s="152"/>
-      <c r="AH2" s="152"/>
-      <c r="AI2" s="152"/>
-      <c r="AJ2" s="152"/>
-      <c r="AK2" s="152"/>
-      <c r="AL2" s="153"/>
+      <c r="M2" s="158"/>
+      <c r="N2" s="181"/>
+      <c r="O2" s="181"/>
+      <c r="P2" s="181"/>
+      <c r="Q2" s="181"/>
+      <c r="R2" s="181"/>
+      <c r="S2" s="181"/>
+      <c r="T2" s="181"/>
+      <c r="U2" s="181"/>
+      <c r="V2" s="181"/>
+      <c r="W2" s="181"/>
+      <c r="X2" s="181"/>
+      <c r="Y2" s="181"/>
+      <c r="Z2" s="181"/>
+      <c r="AA2" s="181"/>
+      <c r="AB2" s="181"/>
+      <c r="AC2" s="181"/>
+      <c r="AD2" s="181"/>
+      <c r="AE2" s="181"/>
+      <c r="AF2" s="181"/>
+      <c r="AG2" s="181"/>
+      <c r="AH2" s="181"/>
+      <c r="AI2" s="181"/>
+      <c r="AJ2" s="181"/>
+      <c r="AK2" s="181"/>
+      <c r="AL2" s="182"/>
       <c r="AM2" s="66"/>
       <c r="AN2" s="66"/>
       <c r="AO2" s="66"/>
@@ -6226,7 +6649,7 @@
       <c r="AY2" s="73"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A3" s="179"/>
+      <c r="A3" s="167"/>
       <c r="B3" s="93" t="s">
         <v>76</v>
       </c>
@@ -6245,57 +6668,57 @@
       <c r="G3" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="164" t="s">
+      <c r="H3" s="172" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="162" t="s">
+      <c r="I3" s="175" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="162" t="s">
+      <c r="J3" s="175" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="163" t="s">
+      <c r="K3" s="176" t="s">
         <v>70</v>
       </c>
       <c r="L3" s="77"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="174"/>
-      <c r="O3" s="161" t="s">
+      <c r="M3" s="161"/>
+      <c r="N3" s="162"/>
+      <c r="O3" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="162"/>
-      <c r="Q3" s="162"/>
-      <c r="R3" s="163"/>
-      <c r="S3" s="162" t="s">
+      <c r="P3" s="175"/>
+      <c r="Q3" s="175"/>
+      <c r="R3" s="176"/>
+      <c r="S3" s="175" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="162"/>
-      <c r="U3" s="162"/>
-      <c r="V3" s="163"/>
-      <c r="W3" s="144" t="s">
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="176"/>
+      <c r="W3" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="X3" s="144"/>
-      <c r="Y3" s="144"/>
-      <c r="Z3" s="145"/>
-      <c r="AA3" s="144" t="s">
+      <c r="X3" s="188"/>
+      <c r="Y3" s="188"/>
+      <c r="Z3" s="189"/>
+      <c r="AA3" s="188" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="144"/>
-      <c r="AC3" s="144"/>
-      <c r="AD3" s="145"/>
-      <c r="AE3" s="144" t="s">
+      <c r="AB3" s="188"/>
+      <c r="AC3" s="188"/>
+      <c r="AD3" s="189"/>
+      <c r="AE3" s="188" t="s">
         <v>20</v>
       </c>
-      <c r="AF3" s="144"/>
-      <c r="AG3" s="144"/>
-      <c r="AH3" s="145"/>
-      <c r="AI3" s="144" t="s">
+      <c r="AF3" s="188"/>
+      <c r="AG3" s="188"/>
+      <c r="AH3" s="189"/>
+      <c r="AI3" s="188" t="s">
         <v>21</v>
       </c>
-      <c r="AJ3" s="144"/>
-      <c r="AK3" s="144"/>
-      <c r="AL3" s="145"/>
+      <c r="AJ3" s="188"/>
+      <c r="AK3" s="188"/>
+      <c r="AL3" s="189"/>
       <c r="AM3" s="68"/>
       <c r="AN3" s="68"/>
       <c r="AO3" s="68"/>
@@ -6311,80 +6734,80 @@
       <c r="AY3" s="68"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A4" s="180"/>
-      <c r="B4" s="154" t="s">
+      <c r="A4" s="168"/>
+      <c r="B4" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="156" t="s">
+      <c r="D4" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="156" t="s">
+      <c r="E4" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="156" t="s">
+      <c r="F4" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="158" t="s">
+      <c r="G4" s="185" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="165"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="160"/>
+      <c r="H4" s="173"/>
+      <c r="I4" s="170"/>
+      <c r="J4" s="170"/>
+      <c r="K4" s="177"/>
       <c r="L4" s="77"/>
-      <c r="M4" s="175"/>
-      <c r="N4" s="176"/>
-      <c r="O4" s="154" t="s">
+      <c r="M4" s="163"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="P4" s="156"/>
-      <c r="Q4" s="156" t="s">
+      <c r="P4" s="170"/>
+      <c r="Q4" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="160"/>
-      <c r="S4" s="156" t="s">
+      <c r="R4" s="177"/>
+      <c r="S4" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="T4" s="156"/>
-      <c r="U4" s="156" t="s">
+      <c r="T4" s="170"/>
+      <c r="U4" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="146" t="s">
+      <c r="V4" s="177"/>
+      <c r="W4" s="190" t="s">
         <v>74</v>
       </c>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="146" t="s">
+      <c r="X4" s="190"/>
+      <c r="Y4" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="Z4" s="147"/>
-      <c r="AA4" s="146" t="s">
+      <c r="Z4" s="191"/>
+      <c r="AA4" s="190" t="s">
         <v>74</v>
       </c>
-      <c r="AB4" s="146"/>
-      <c r="AC4" s="146" t="s">
+      <c r="AB4" s="190"/>
+      <c r="AC4" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="AD4" s="147"/>
-      <c r="AE4" s="146" t="s">
+      <c r="AD4" s="191"/>
+      <c r="AE4" s="190" t="s">
         <v>74</v>
       </c>
-      <c r="AF4" s="146"/>
-      <c r="AG4" s="146" t="s">
+      <c r="AF4" s="190"/>
+      <c r="AG4" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="AH4" s="147"/>
-      <c r="AI4" s="146" t="s">
+      <c r="AH4" s="191"/>
+      <c r="AI4" s="190" t="s">
         <v>74</v>
       </c>
-      <c r="AJ4" s="146"/>
-      <c r="AK4" s="146" t="s">
+      <c r="AJ4" s="190"/>
+      <c r="AK4" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="AL4" s="147"/>
+      <c r="AL4" s="191"/>
       <c r="AM4" s="68"/>
       <c r="AN4" s="68"/>
       <c r="AO4" s="68"/>
@@ -6400,20 +6823,20 @@
       <c r="AY4" s="68"/>
     </row>
     <row r="5" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="181"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="166"/>
-      <c r="I5" s="157"/>
-      <c r="J5" s="157"/>
-      <c r="K5" s="167"/>
+      <c r="A5" s="169"/>
+      <c r="B5" s="184"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="186"/>
+      <c r="H5" s="174"/>
+      <c r="I5" s="171"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="178"/>
       <c r="L5" s="78"/>
-      <c r="M5" s="177"/>
-      <c r="N5" s="178"/>
+      <c r="M5" s="165"/>
+      <c r="N5" s="166"/>
       <c r="O5" s="95" t="s">
         <v>73</v>
       </c>
@@ -7834,29 +8257,29 @@
     </row>
     <row r="24" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="148" t="s">
+      <c r="A25" s="155" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="169"/>
-      <c r="C25" s="169"/>
-      <c r="D25" s="169"/>
-      <c r="E25" s="169"/>
-      <c r="F25" s="169"/>
-      <c r="G25" s="169"/>
-      <c r="H25" s="169"/>
-      <c r="I25" s="169"/>
-      <c r="J25" s="169"/>
-      <c r="K25" s="169"/>
-      <c r="L25" s="169"/>
-      <c r="M25" s="169"/>
-      <c r="N25" s="169"/>
-      <c r="O25" s="169"/>
-      <c r="P25" s="169"/>
-      <c r="Q25" s="169"/>
-      <c r="R25" s="169"/>
-      <c r="S25" s="169"/>
-      <c r="T25" s="169"/>
-      <c r="U25" s="170"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="156"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="156"/>
+      <c r="K25" s="156"/>
+      <c r="L25" s="156"/>
+      <c r="M25" s="156"/>
+      <c r="N25" s="156"/>
+      <c r="O25" s="156"/>
+      <c r="P25" s="156"/>
+      <c r="Q25" s="156"/>
+      <c r="R25" s="156"/>
+      <c r="S25" s="156"/>
+      <c r="T25" s="156"/>
+      <c r="U25" s="157"/>
       <c r="Z25" s="4"/>
       <c r="AA25" s="66"/>
       <c r="AB25" s="66"/>
@@ -7885,27 +8308,27 @@
       <c r="AY25" s="66"/>
     </row>
     <row r="26" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="151"/>
-      <c r="B26" s="171"/>
-      <c r="C26" s="171"/>
-      <c r="D26" s="171"/>
-      <c r="E26" s="171"/>
-      <c r="F26" s="171"/>
-      <c r="G26" s="171"/>
-      <c r="H26" s="171"/>
-      <c r="I26" s="171"/>
-      <c r="J26" s="171"/>
-      <c r="K26" s="171"/>
-      <c r="L26" s="171"/>
-      <c r="M26" s="171"/>
-      <c r="N26" s="171"/>
-      <c r="O26" s="171"/>
-      <c r="P26" s="171"/>
-      <c r="Q26" s="171"/>
-      <c r="R26" s="171"/>
-      <c r="S26" s="171"/>
-      <c r="T26" s="171"/>
-      <c r="U26" s="172"/>
+      <c r="A26" s="158"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
+      <c r="H26" s="159"/>
+      <c r="I26" s="159"/>
+      <c r="J26" s="159"/>
+      <c r="K26" s="159"/>
+      <c r="L26" s="159"/>
+      <c r="M26" s="159"/>
+      <c r="N26" s="159"/>
+      <c r="O26" s="159"/>
+      <c r="P26" s="159"/>
+      <c r="Q26" s="159"/>
+      <c r="R26" s="159"/>
+      <c r="S26" s="159"/>
+      <c r="T26" s="159"/>
+      <c r="U26" s="160"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="66"/>
       <c r="AB26" s="66"/>
@@ -7935,46 +8358,46 @@
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" s="75"/>
-      <c r="B27" s="130" t="s">
+      <c r="B27" s="139" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="182"/>
-      <c r="D27" s="130" t="s">
+      <c r="C27" s="140"/>
+      <c r="D27" s="139" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="182"/>
-      <c r="F27" s="133" t="s">
+      <c r="E27" s="140"/>
+      <c r="F27" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="168"/>
-      <c r="H27" s="137" t="s">
+      <c r="G27" s="154"/>
+      <c r="H27" s="144" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="168"/>
-      <c r="J27" s="133" t="s">
+      <c r="I27" s="154"/>
+      <c r="J27" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="K27" s="168"/>
-      <c r="L27" s="133" t="s">
+      <c r="K27" s="154"/>
+      <c r="L27" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="M27" s="168"/>
-      <c r="N27" s="133" t="s">
+      <c r="M27" s="154"/>
+      <c r="N27" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="O27" s="168"/>
-      <c r="P27" s="133" t="s">
+      <c r="O27" s="154"/>
+      <c r="P27" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="Q27" s="168"/>
-      <c r="R27" s="133" t="s">
+      <c r="Q27" s="154"/>
+      <c r="R27" s="145" t="s">
         <v>86</v>
       </c>
-      <c r="S27" s="168"/>
-      <c r="T27" s="133" t="s">
+      <c r="S27" s="154"/>
+      <c r="T27" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="U27" s="168"/>
+      <c r="U27" s="154"/>
     </row>
     <row r="28" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="76"/>
@@ -8916,6 +9339,33 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="AE3:AH3"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="M1:AL2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
     <mergeCell ref="P27:Q27"/>
     <mergeCell ref="R27:S27"/>
     <mergeCell ref="T27:U27"/>
@@ -8932,33 +9382,6 @@
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="M1:AL2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE3:AH3"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AL4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8980,95 +9403,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="145" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="133"/>
-      <c r="N1" s="133"/>
-      <c r="O1" s="133"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="130" t="s">
+      <c r="S1" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="130"/>
-      <c r="U1" s="130"/>
-      <c r="V1" s="130"/>
-      <c r="W1" s="130"/>
-      <c r="X1" s="130"/>
-      <c r="Y1" s="130"/>
-      <c r="Z1" s="130"/>
-      <c r="AA1" s="130"/>
-      <c r="AB1" s="130"/>
-      <c r="AC1" s="130"/>
-      <c r="AD1" s="130"/>
-      <c r="AE1" s="130"/>
-      <c r="AF1" s="130"/>
+      <c r="T1" s="139"/>
+      <c r="U1" s="139"/>
+      <c r="V1" s="139"/>
+      <c r="W1" s="139"/>
+      <c r="X1" s="139"/>
+      <c r="Y1" s="139"/>
+      <c r="Z1" s="139"/>
+      <c r="AA1" s="139"/>
+      <c r="AB1" s="139"/>
+      <c r="AC1" s="139"/>
+      <c r="AD1" s="139"/>
+      <c r="AE1" s="139"/>
+      <c r="AF1" s="139"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135" t="s">
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135" t="s">
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135" t="s">
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
-      <c r="N2" s="135" t="s">
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
+      <c r="N2" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="135"/>
-      <c r="P2" s="136"/>
+      <c r="O2" s="141"/>
+      <c r="P2" s="142"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="135" t="s">
+      <c r="S2" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="135"/>
-      <c r="U2" s="135"/>
-      <c r="V2" s="135" t="s">
+      <c r="T2" s="141"/>
+      <c r="U2" s="141"/>
+      <c r="V2" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="135"/>
-      <c r="X2" s="135"/>
-      <c r="Y2" s="135" t="s">
+      <c r="W2" s="141"/>
+      <c r="X2" s="141"/>
+      <c r="Y2" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="135"/>
-      <c r="AA2" s="135"/>
-      <c r="AB2" s="135" t="s">
+      <c r="Z2" s="141"/>
+      <c r="AA2" s="141"/>
+      <c r="AB2" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="135"/>
-      <c r="AD2" s="135"/>
-      <c r="AE2" s="135" t="s">
+      <c r="AC2" s="141"/>
+      <c r="AD2" s="141"/>
+      <c r="AE2" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="135"/>
-      <c r="AG2" s="136"/>
+      <c r="AF2" s="141"/>
+      <c r="AG2" s="142"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -9837,95 +10260,95 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="133" t="s">
+      <c r="B22" s="145" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="133"/>
-      <c r="K22" s="133"/>
-      <c r="L22" s="133"/>
-      <c r="M22" s="133"/>
-      <c r="N22" s="133"/>
-      <c r="O22" s="133"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="145"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="145"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="145"/>
+      <c r="J22" s="145"/>
+      <c r="K22" s="145"/>
+      <c r="L22" s="145"/>
+      <c r="M22" s="145"/>
+      <c r="N22" s="145"/>
+      <c r="O22" s="145"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="130" t="s">
+      <c r="S22" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="T22" s="130"/>
-      <c r="U22" s="130"/>
-      <c r="V22" s="130"/>
-      <c r="W22" s="130"/>
-      <c r="X22" s="130"/>
-      <c r="Y22" s="130"/>
-      <c r="Z22" s="130"/>
-      <c r="AA22" s="130"/>
-      <c r="AB22" s="130"/>
-      <c r="AC22" s="130"/>
-      <c r="AD22" s="130"/>
-      <c r="AE22" s="130"/>
-      <c r="AF22" s="130"/>
+      <c r="T22" s="139"/>
+      <c r="U22" s="139"/>
+      <c r="V22" s="139"/>
+      <c r="W22" s="139"/>
+      <c r="X22" s="139"/>
+      <c r="Y22" s="139"/>
+      <c r="Z22" s="139"/>
+      <c r="AA22" s="139"/>
+      <c r="AB22" s="139"/>
+      <c r="AC22" s="139"/>
+      <c r="AD22" s="139"/>
+      <c r="AE22" s="139"/>
+      <c r="AF22" s="139"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="135"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="135" t="s">
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="135"/>
-      <c r="G23" s="135"/>
-      <c r="H23" s="135" t="s">
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="135"/>
-      <c r="J23" s="135"/>
-      <c r="K23" s="135" t="s">
+      <c r="I23" s="141"/>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="135"/>
-      <c r="M23" s="135"/>
-      <c r="N23" s="135" t="s">
+      <c r="L23" s="141"/>
+      <c r="M23" s="141"/>
+      <c r="N23" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="135"/>
+      <c r="O23" s="141"/>
       <c r="P23" s="5"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="135" t="s">
+      <c r="S23" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="135"/>
-      <c r="U23" s="135"/>
-      <c r="V23" s="135" t="s">
+      <c r="T23" s="141"/>
+      <c r="U23" s="141"/>
+      <c r="V23" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="135"/>
-      <c r="X23" s="135"/>
-      <c r="Y23" s="135" t="s">
+      <c r="W23" s="141"/>
+      <c r="X23" s="141"/>
+      <c r="Y23" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="135"/>
-      <c r="AA23" s="135"/>
-      <c r="AB23" s="135" t="s">
+      <c r="Z23" s="141"/>
+      <c r="AA23" s="141"/>
+      <c r="AB23" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="135"/>
-      <c r="AD23" s="135"/>
-      <c r="AE23" s="135" t="s">
+      <c r="AC23" s="141"/>
+      <c r="AD23" s="141"/>
+      <c r="AE23" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="135"/>
-      <c r="AG23" s="136"/>
+      <c r="AF23" s="141"/>
+      <c r="AG23" s="142"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -10692,95 +11115,95 @@
     <row r="42" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="145" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="133"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="133"/>
-      <c r="F43" s="133"/>
-      <c r="G43" s="133"/>
-      <c r="H43" s="133"/>
-      <c r="I43" s="133"/>
-      <c r="J43" s="133"/>
-      <c r="K43" s="133"/>
-      <c r="L43" s="133"/>
-      <c r="M43" s="133"/>
-      <c r="N43" s="133"/>
-      <c r="O43" s="133"/>
+      <c r="C43" s="145"/>
+      <c r="D43" s="145"/>
+      <c r="E43" s="145"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="145"/>
+      <c r="I43" s="145"/>
+      <c r="J43" s="145"/>
+      <c r="K43" s="145"/>
+      <c r="L43" s="145"/>
+      <c r="M43" s="145"/>
+      <c r="N43" s="145"/>
+      <c r="O43" s="145"/>
       <c r="P43" s="2"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="133" t="s">
+      <c r="S43" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="T43" s="133"/>
-      <c r="U43" s="133"/>
-      <c r="V43" s="133"/>
-      <c r="W43" s="133"/>
-      <c r="X43" s="133"/>
-      <c r="Y43" s="133"/>
-      <c r="Z43" s="133"/>
-      <c r="AA43" s="133"/>
-      <c r="AB43" s="133"/>
-      <c r="AC43" s="133"/>
-      <c r="AD43" s="133"/>
-      <c r="AE43" s="133"/>
-      <c r="AF43" s="133"/>
+      <c r="T43" s="145"/>
+      <c r="U43" s="145"/>
+      <c r="V43" s="145"/>
+      <c r="W43" s="145"/>
+      <c r="X43" s="145"/>
+      <c r="Y43" s="145"/>
+      <c r="Z43" s="145"/>
+      <c r="AA43" s="145"/>
+      <c r="AB43" s="145"/>
+      <c r="AC43" s="145"/>
+      <c r="AD43" s="145"/>
+      <c r="AE43" s="145"/>
+      <c r="AF43" s="145"/>
       <c r="AG43" s="2"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="135" t="s">
+      <c r="B44" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="135"/>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135" t="s">
+      <c r="C44" s="141"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="135"/>
-      <c r="G44" s="135"/>
-      <c r="H44" s="135" t="s">
+      <c r="F44" s="141"/>
+      <c r="G44" s="141"/>
+      <c r="H44" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="135"/>
-      <c r="J44" s="135"/>
-      <c r="K44" s="135" t="s">
+      <c r="I44" s="141"/>
+      <c r="J44" s="141"/>
+      <c r="K44" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="L44" s="135"/>
-      <c r="M44" s="135"/>
+      <c r="L44" s="141"/>
+      <c r="M44" s="141"/>
       <c r="N44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="O44" s="14"/>
       <c r="P44" s="5"/>
       <c r="R44" s="9"/>
-      <c r="S44" s="135" t="s">
+      <c r="S44" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="T44" s="135"/>
-      <c r="U44" s="135"/>
-      <c r="V44" s="135" t="s">
+      <c r="T44" s="141"/>
+      <c r="U44" s="141"/>
+      <c r="V44" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="W44" s="135"/>
-      <c r="X44" s="135"/>
-      <c r="Y44" s="135" t="s">
+      <c r="W44" s="141"/>
+      <c r="X44" s="141"/>
+      <c r="Y44" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="Z44" s="135"/>
-      <c r="AA44" s="135"/>
-      <c r="AB44" s="135" t="s">
+      <c r="Z44" s="141"/>
+      <c r="AA44" s="141"/>
+      <c r="AB44" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AC44" s="135"/>
-      <c r="AD44" s="135"/>
-      <c r="AE44" s="135" t="s">
+      <c r="AC44" s="141"/>
+      <c r="AD44" s="141"/>
+      <c r="AE44" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="AF44" s="135"/>
-      <c r="AG44" s="136"/>
+      <c r="AF44" s="141"/>
+      <c r="AG44" s="142"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
@@ -11548,41 +11971,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="B43:O43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="S1:AF1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="S22:AF22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AD23"/>
+    <mergeCell ref="AE23:AG23"/>
     <mergeCell ref="S43:AF43"/>
     <mergeCell ref="S44:U44"/>
     <mergeCell ref="V44:X44"/>
     <mergeCell ref="Y44:AA44"/>
     <mergeCell ref="AB44:AD44"/>
     <mergeCell ref="AE44:AG44"/>
-    <mergeCell ref="S22:AF22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AD23"/>
-    <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="S1:AF1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="B43:O43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11604,95 +12027,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="133"/>
-      <c r="N1" s="133"/>
-      <c r="O1" s="133"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="133" t="s">
+      <c r="S1" s="145" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="133"/>
-      <c r="U1" s="133"/>
-      <c r="V1" s="133"/>
-      <c r="W1" s="133"/>
-      <c r="X1" s="133"/>
-      <c r="Y1" s="133"/>
-      <c r="Z1" s="133"/>
-      <c r="AA1" s="133"/>
-      <c r="AB1" s="133"/>
-      <c r="AC1" s="133"/>
-      <c r="AD1" s="133"/>
-      <c r="AE1" s="133"/>
-      <c r="AF1" s="133"/>
+      <c r="T1" s="145"/>
+      <c r="U1" s="145"/>
+      <c r="V1" s="145"/>
+      <c r="W1" s="145"/>
+      <c r="X1" s="145"/>
+      <c r="Y1" s="145"/>
+      <c r="Z1" s="145"/>
+      <c r="AA1" s="145"/>
+      <c r="AB1" s="145"/>
+      <c r="AC1" s="145"/>
+      <c r="AD1" s="145"/>
+      <c r="AE1" s="145"/>
+      <c r="AF1" s="145"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135" t="s">
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135" t="s">
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135" t="s">
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
-      <c r="N2" s="135" t="s">
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
+      <c r="N2" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="135"/>
-      <c r="P2" s="136"/>
+      <c r="O2" s="141"/>
+      <c r="P2" s="142"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="131" t="s">
+      <c r="S2" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="131"/>
-      <c r="U2" s="131"/>
-      <c r="V2" s="131" t="s">
+      <c r="T2" s="147"/>
+      <c r="U2" s="147"/>
+      <c r="V2" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="131"/>
-      <c r="X2" s="131"/>
-      <c r="Y2" s="131" t="s">
+      <c r="W2" s="147"/>
+      <c r="X2" s="147"/>
+      <c r="Y2" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="131"/>
-      <c r="AA2" s="131"/>
-      <c r="AB2" s="131" t="s">
+      <c r="Z2" s="147"/>
+      <c r="AA2" s="147"/>
+      <c r="AB2" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="131"/>
-      <c r="AD2" s="131"/>
-      <c r="AE2" s="131" t="s">
+      <c r="AC2" s="147"/>
+      <c r="AD2" s="147"/>
+      <c r="AE2" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="131"/>
-      <c r="AG2" s="132"/>
+      <c r="AF2" s="147"/>
+      <c r="AG2" s="153"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -12461,51 +12884,51 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="133" t="s">
+      <c r="B22" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="133"/>
-      <c r="K22" s="133"/>
-      <c r="L22" s="133"/>
-      <c r="M22" s="133"/>
-      <c r="N22" s="133"/>
-      <c r="O22" s="133"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="145"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="145"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="145"/>
+      <c r="J22" s="145"/>
+      <c r="K22" s="145"/>
+      <c r="L22" s="145"/>
+      <c r="M22" s="145"/>
+      <c r="N22" s="145"/>
+      <c r="O22" s="145"/>
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="135"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="135" t="s">
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="135"/>
-      <c r="G23" s="135"/>
-      <c r="H23" s="135" t="s">
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="135"/>
-      <c r="J23" s="135"/>
-      <c r="K23" s="135" t="s">
+      <c r="I23" s="141"/>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="135"/>
-      <c r="M23" s="135"/>
-      <c r="N23" s="135" t="s">
+      <c r="L23" s="141"/>
+      <c r="M23" s="141"/>
+      <c r="N23" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="135"/>
-      <c r="P23" s="136"/>
+      <c r="O23" s="141"/>
+      <c r="P23" s="142"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -12909,24 +13332,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
     <mergeCell ref="S1:AF1"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="V2:X2"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Color Models. NEXT: Color Mixtures.
</commit_message>
<xml_diff>
--- a/Analysis/First Study/centroids_allquestions.xlsx
+++ b/Analysis/First Study/centroids_allquestions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="113">
   <si>
     <t>Question 1</t>
   </si>
@@ -311,9 +311,6 @@
     <t>Centroides</t>
   </si>
   <si>
-    <t>Distâncias</t>
-  </si>
-  <si>
     <t>Question 18</t>
   </si>
   <si>
@@ -364,6 +361,12 @@
   <si>
     <t>HSV_2</t>
   </si>
+  <si>
+    <t>Distâncias - objTwoColors</t>
+  </si>
+  <si>
+    <t>Distâncias - twoColorsObj</t>
+  </si>
 </sst>
 </file>
 
@@ -372,7 +375,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,6 +438,18 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -524,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -795,8 +810,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -890,8 +931,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1187,7 +1256,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1214,9 +1323,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1232,19 +1338,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1361,15 +1461,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="121">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1416,6 +1509,20 @@
     <cellStyle name="Hiperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1462,6 +1569,20 @@
     <cellStyle name="Hiperlink Visitado" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1737,12 +1858,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC101"/>
+  <dimension ref="A1:BC102"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A75" zoomScale="118" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="L88" sqref="L88:P88"/>
+      <selection pane="topRight" activeCell="AH93" sqref="AH93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1753,78 +1874,78 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="181" t="s">
+      <c r="B1" s="203" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-      <c r="G1" s="181"/>
-      <c r="H1" s="181"/>
-      <c r="I1" s="181"/>
-      <c r="J1" s="181"/>
-      <c r="K1" s="181"/>
-      <c r="L1" s="181"/>
-      <c r="M1" s="181"/>
-      <c r="N1" s="181"/>
-      <c r="O1" s="181"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
+      <c r="I1" s="203"/>
+      <c r="J1" s="203"/>
+      <c r="K1" s="203"/>
+      <c r="L1" s="203"/>
+      <c r="M1" s="203"/>
+      <c r="N1" s="203"/>
+      <c r="O1" s="203"/>
       <c r="P1" s="2"/>
-      <c r="S1" s="177" t="s">
+      <c r="S1" s="195" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
+      <c r="T1" s="195"/>
+      <c r="U1" s="195"/>
+      <c r="V1" s="195"/>
+      <c r="W1" s="195"/>
+      <c r="X1" s="195"/>
+      <c r="Y1" s="195"/>
+      <c r="Z1" s="195"/>
+      <c r="AA1" s="195"/>
+      <c r="AB1" s="195"/>
+      <c r="AC1" s="195"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184" t="s">
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184" t="s">
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184" t="s">
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="184"/>
-      <c r="M2" s="184"/>
-      <c r="N2" s="184" t="s">
+      <c r="L2" s="206"/>
+      <c r="M2" s="206"/>
+      <c r="N2" s="206" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="184"/>
-      <c r="P2" s="196"/>
-      <c r="T2" s="177" t="s">
+      <c r="O2" s="206"/>
+      <c r="P2" s="194"/>
+      <c r="T2" s="195" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="177"/>
-      <c r="V2" s="177"/>
-      <c r="W2" s="177"/>
-      <c r="X2" s="177"/>
-      <c r="Y2" s="177" t="s">
+      <c r="U2" s="195"/>
+      <c r="V2" s="195"/>
+      <c r="W2" s="195"/>
+      <c r="X2" s="195"/>
+      <c r="Y2" s="195" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="177"/>
-      <c r="AA2" s="177"/>
-      <c r="AB2" s="177"/>
-      <c r="AC2" s="177"/>
+      <c r="Z2" s="195"/>
+      <c r="AA2" s="195"/>
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="195"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -2570,95 +2691,95 @@
     <row r="21" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="181" t="s">
+      <c r="B22" s="203" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="181"/>
-      <c r="D22" s="181"/>
-      <c r="E22" s="181"/>
-      <c r="F22" s="181"/>
-      <c r="G22" s="181"/>
-      <c r="H22" s="181"/>
-      <c r="I22" s="181"/>
-      <c r="J22" s="181"/>
-      <c r="K22" s="181"/>
-      <c r="L22" s="181"/>
-      <c r="M22" s="181"/>
-      <c r="N22" s="181"/>
-      <c r="O22" s="181"/>
+      <c r="C22" s="203"/>
+      <c r="D22" s="203"/>
+      <c r="E22" s="203"/>
+      <c r="F22" s="203"/>
+      <c r="G22" s="203"/>
+      <c r="H22" s="203"/>
+      <c r="I22" s="203"/>
+      <c r="J22" s="203"/>
+      <c r="K22" s="203"/>
+      <c r="L22" s="203"/>
+      <c r="M22" s="203"/>
+      <c r="N22" s="203"/>
+      <c r="O22" s="203"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="178" t="s">
+      <c r="S22" s="200" t="s">
         <v>60</v>
       </c>
-      <c r="T22" s="178"/>
-      <c r="U22" s="178"/>
-      <c r="V22" s="178"/>
-      <c r="W22" s="178"/>
-      <c r="X22" s="178"/>
-      <c r="Y22" s="178"/>
-      <c r="Z22" s="178"/>
-      <c r="AA22" s="178"/>
-      <c r="AB22" s="178"/>
-      <c r="AC22" s="178"/>
-      <c r="AD22" s="178"/>
-      <c r="AE22" s="178"/>
-      <c r="AF22" s="178"/>
+      <c r="T22" s="200"/>
+      <c r="U22" s="200"/>
+      <c r="V22" s="200"/>
+      <c r="W22" s="200"/>
+      <c r="X22" s="200"/>
+      <c r="Y22" s="200"/>
+      <c r="Z22" s="200"/>
+      <c r="AA22" s="200"/>
+      <c r="AB22" s="200"/>
+      <c r="AC22" s="200"/>
+      <c r="AD22" s="200"/>
+      <c r="AE22" s="200"/>
+      <c r="AF22" s="200"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="179" t="s">
+      <c r="B23" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="179"/>
-      <c r="D23" s="179"/>
-      <c r="E23" s="179" t="s">
+      <c r="C23" s="201"/>
+      <c r="D23" s="201"/>
+      <c r="E23" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="179"/>
-      <c r="G23" s="179"/>
-      <c r="H23" s="179" t="s">
+      <c r="F23" s="201"/>
+      <c r="G23" s="201"/>
+      <c r="H23" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="179"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="179" t="s">
+      <c r="I23" s="201"/>
+      <c r="J23" s="201"/>
+      <c r="K23" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="179"/>
-      <c r="M23" s="179"/>
-      <c r="N23" s="179" t="s">
+      <c r="L23" s="201"/>
+      <c r="M23" s="201"/>
+      <c r="N23" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="179"/>
-      <c r="P23" s="180"/>
+      <c r="O23" s="201"/>
+      <c r="P23" s="202"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="179" t="s">
+      <c r="S23" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="179"/>
-      <c r="U23" s="179"/>
-      <c r="V23" s="179" t="s">
+      <c r="T23" s="201"/>
+      <c r="U23" s="201"/>
+      <c r="V23" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="179"/>
-      <c r="X23" s="179"/>
-      <c r="Y23" s="179" t="s">
+      <c r="W23" s="201"/>
+      <c r="X23" s="201"/>
+      <c r="Y23" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="179"/>
-      <c r="AA23" s="179"/>
-      <c r="AB23" s="179" t="s">
+      <c r="Z23" s="201"/>
+      <c r="AA23" s="201"/>
+      <c r="AB23" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="179"/>
-      <c r="AD23" s="179"/>
-      <c r="AE23" s="179" t="s">
+      <c r="AC23" s="201"/>
+      <c r="AD23" s="201"/>
+      <c r="AE23" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="179"/>
-      <c r="AG23" s="180"/>
+      <c r="AF23" s="201"/>
+      <c r="AG23" s="202"/>
     </row>
     <row r="24" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -3742,159 +3863,159 @@
     <row r="42" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="178" t="s">
+      <c r="B43" s="200" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="178"/>
-      <c r="F43" s="178"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="178"/>
-      <c r="K43" s="178"/>
-      <c r="L43" s="178"/>
-      <c r="M43" s="178"/>
-      <c r="N43" s="178"/>
-      <c r="O43" s="178"/>
-      <c r="P43" s="178"/>
+      <c r="C43" s="200"/>
+      <c r="D43" s="200"/>
+      <c r="E43" s="200"/>
+      <c r="F43" s="200"/>
+      <c r="G43" s="200"/>
+      <c r="H43" s="200"/>
+      <c r="I43" s="200"/>
+      <c r="J43" s="200"/>
+      <c r="K43" s="200"/>
+      <c r="L43" s="200"/>
+      <c r="M43" s="200"/>
+      <c r="N43" s="200"/>
+      <c r="O43" s="200"/>
+      <c r="P43" s="200"/>
       <c r="Q43" s="46"/>
       <c r="R43" s="46"/>
       <c r="S43" s="47"/>
-      <c r="T43" s="182" t="s">
+      <c r="T43" s="204" t="s">
         <v>62</v>
       </c>
-      <c r="U43" s="178"/>
-      <c r="V43" s="178"/>
-      <c r="W43" s="178"/>
-      <c r="X43" s="178"/>
-      <c r="Y43" s="178"/>
-      <c r="Z43" s="178"/>
-      <c r="AA43" s="178"/>
-      <c r="AB43" s="178"/>
-      <c r="AC43" s="178"/>
-      <c r="AD43" s="178"/>
-      <c r="AE43" s="178"/>
-      <c r="AF43" s="178"/>
-      <c r="AG43" s="178"/>
-      <c r="AH43" s="178"/>
+      <c r="U43" s="200"/>
+      <c r="V43" s="200"/>
+      <c r="W43" s="200"/>
+      <c r="X43" s="200"/>
+      <c r="Y43" s="200"/>
+      <c r="Z43" s="200"/>
+      <c r="AA43" s="200"/>
+      <c r="AB43" s="200"/>
+      <c r="AC43" s="200"/>
+      <c r="AD43" s="200"/>
+      <c r="AE43" s="200"/>
+      <c r="AF43" s="200"/>
+      <c r="AG43" s="200"/>
+      <c r="AH43" s="200"/>
       <c r="AI43" s="46"/>
       <c r="AJ43" s="46"/>
       <c r="AK43" s="47"/>
-      <c r="AL43" s="182" t="s">
+      <c r="AL43" s="204" t="s">
         <v>63</v>
       </c>
-      <c r="AM43" s="178"/>
-      <c r="AN43" s="178"/>
-      <c r="AO43" s="178"/>
-      <c r="AP43" s="178"/>
-      <c r="AQ43" s="178"/>
-      <c r="AR43" s="178"/>
-      <c r="AS43" s="178"/>
-      <c r="AT43" s="178"/>
-      <c r="AU43" s="178"/>
-      <c r="AV43" s="178"/>
-      <c r="AW43" s="178"/>
-      <c r="AX43" s="178"/>
-      <c r="AY43" s="178"/>
-      <c r="AZ43" s="178"/>
+      <c r="AM43" s="200"/>
+      <c r="AN43" s="200"/>
+      <c r="AO43" s="200"/>
+      <c r="AP43" s="200"/>
+      <c r="AQ43" s="200"/>
+      <c r="AR43" s="200"/>
+      <c r="AS43" s="200"/>
+      <c r="AT43" s="200"/>
+      <c r="AU43" s="200"/>
+      <c r="AV43" s="200"/>
+      <c r="AW43" s="200"/>
+      <c r="AX43" s="200"/>
+      <c r="AY43" s="200"/>
+      <c r="AZ43" s="200"/>
       <c r="BA43" s="48"/>
       <c r="BB43" s="48"/>
       <c r="BC43" s="49"/>
     </row>
     <row r="44" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
-      <c r="B44" s="191" t="s">
+      <c r="B44" s="212" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="191"/>
-      <c r="D44" s="191"/>
-      <c r="E44" s="188" t="s">
+      <c r="C44" s="212"/>
+      <c r="D44" s="212"/>
+      <c r="E44" s="209" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="188"/>
-      <c r="G44" s="188"/>
-      <c r="H44" s="188" t="s">
+      <c r="F44" s="209"/>
+      <c r="G44" s="209"/>
+      <c r="H44" s="209" t="s">
         <v>18</v>
       </c>
-      <c r="I44" s="188"/>
-      <c r="J44" s="188"/>
-      <c r="K44" s="189" t="s">
+      <c r="I44" s="209"/>
+      <c r="J44" s="209"/>
+      <c r="K44" s="210" t="s">
         <v>19</v>
       </c>
-      <c r="L44" s="179"/>
-      <c r="M44" s="190"/>
-      <c r="N44" s="188" t="s">
+      <c r="L44" s="201"/>
+      <c r="M44" s="211"/>
+      <c r="N44" s="209" t="s">
         <v>20</v>
       </c>
-      <c r="O44" s="188"/>
-      <c r="P44" s="188"/>
-      <c r="Q44" s="179" t="s">
+      <c r="O44" s="209"/>
+      <c r="P44" s="209"/>
+      <c r="Q44" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="R44" s="179"/>
-      <c r="S44" s="180"/>
-      <c r="T44" s="183" t="s">
+      <c r="R44" s="201"/>
+      <c r="S44" s="202"/>
+      <c r="T44" s="205" t="s">
         <v>54</v>
       </c>
-      <c r="U44" s="184"/>
-      <c r="V44" s="184"/>
-      <c r="W44" s="179" t="s">
+      <c r="U44" s="206"/>
+      <c r="V44" s="206"/>
+      <c r="W44" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="X44" s="179"/>
-      <c r="Y44" s="179"/>
-      <c r="Z44" s="179" t="s">
+      <c r="X44" s="201"/>
+      <c r="Y44" s="201"/>
+      <c r="Z44" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="AA44" s="179"/>
-      <c r="AB44" s="179"/>
-      <c r="AC44" s="179" t="s">
+      <c r="AA44" s="201"/>
+      <c r="AB44" s="201"/>
+      <c r="AC44" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="AD44" s="179"/>
-      <c r="AE44" s="179"/>
-      <c r="AF44" s="179" t="s">
+      <c r="AD44" s="201"/>
+      <c r="AE44" s="201"/>
+      <c r="AF44" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="AG44" s="179"/>
-      <c r="AH44" s="179"/>
-      <c r="AI44" s="179" t="s">
+      <c r="AG44" s="201"/>
+      <c r="AH44" s="201"/>
+      <c r="AI44" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="AJ44" s="179"/>
-      <c r="AK44" s="180"/>
-      <c r="AL44" s="187" t="s">
+      <c r="AJ44" s="201"/>
+      <c r="AK44" s="202"/>
+      <c r="AL44" s="208" t="s">
         <v>54</v>
       </c>
-      <c r="AM44" s="179"/>
-      <c r="AN44" s="179"/>
-      <c r="AO44" s="179" t="s">
+      <c r="AM44" s="201"/>
+      <c r="AN44" s="201"/>
+      <c r="AO44" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="AP44" s="179"/>
-      <c r="AQ44" s="179"/>
-      <c r="AR44" s="179" t="s">
+      <c r="AP44" s="201"/>
+      <c r="AQ44" s="201"/>
+      <c r="AR44" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="AS44" s="179"/>
-      <c r="AT44" s="179"/>
-      <c r="AU44" s="179" t="s">
+      <c r="AS44" s="201"/>
+      <c r="AT44" s="201"/>
+      <c r="AU44" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="AV44" s="179"/>
-      <c r="AW44" s="179"/>
-      <c r="AX44" s="179" t="s">
+      <c r="AV44" s="201"/>
+      <c r="AW44" s="201"/>
+      <c r="AX44" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="AY44" s="179"/>
-      <c r="AZ44" s="179"/>
-      <c r="BA44" s="179" t="s">
+      <c r="AY44" s="201"/>
+      <c r="AZ44" s="201"/>
+      <c r="BA44" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="BB44" s="179"/>
-      <c r="BC44" s="180"/>
+      <c r="BB44" s="201"/>
+      <c r="BC44" s="202"/>
     </row>
     <row r="45" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
@@ -5683,61 +5804,61 @@
     </row>
     <row r="64" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="181" t="s">
+      <c r="B64" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="C64" s="181"/>
-      <c r="D64" s="181"/>
-      <c r="E64" s="181"/>
-      <c r="F64" s="181"/>
-      <c r="G64" s="181"/>
-      <c r="H64" s="181"/>
-      <c r="I64" s="181"/>
-      <c r="J64" s="181"/>
-      <c r="K64" s="186"/>
-      <c r="L64" s="181" t="s">
+      <c r="C64" s="203"/>
+      <c r="D64" s="203"/>
+      <c r="E64" s="203"/>
+      <c r="F64" s="203"/>
+      <c r="G64" s="203"/>
+      <c r="H64" s="203"/>
+      <c r="I64" s="203"/>
+      <c r="J64" s="203"/>
+      <c r="K64" s="193"/>
+      <c r="L64" s="203" t="s">
         <v>92</v>
       </c>
-      <c r="M64" s="181"/>
-      <c r="N64" s="181"/>
-      <c r="O64" s="181"/>
-      <c r="P64" s="181"/>
-      <c r="Q64" s="181"/>
-      <c r="R64" s="181"/>
-      <c r="S64" s="181"/>
-      <c r="T64" s="181"/>
-      <c r="U64" s="186"/>
+      <c r="M64" s="203"/>
+      <c r="N64" s="203"/>
+      <c r="O64" s="203"/>
+      <c r="P64" s="203"/>
+      <c r="Q64" s="203"/>
+      <c r="R64" s="203"/>
+      <c r="S64" s="203"/>
+      <c r="T64" s="203"/>
+      <c r="U64" s="193"/>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-      <c r="B65" s="185" t="s">
+      <c r="B65" s="207" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="181"/>
-      <c r="D65" s="181"/>
-      <c r="E65" s="181"/>
-      <c r="F65" s="186"/>
-      <c r="G65" s="181" t="s">
+      <c r="C65" s="203"/>
+      <c r="D65" s="203"/>
+      <c r="E65" s="203"/>
+      <c r="F65" s="193"/>
+      <c r="G65" s="203" t="s">
         <v>90</v>
       </c>
-      <c r="H65" s="181"/>
-      <c r="I65" s="181"/>
-      <c r="J65" s="181"/>
-      <c r="K65" s="186"/>
-      <c r="L65" s="181" t="s">
+      <c r="H65" s="203"/>
+      <c r="I65" s="203"/>
+      <c r="J65" s="203"/>
+      <c r="K65" s="193"/>
+      <c r="L65" s="203" t="s">
         <v>89</v>
       </c>
-      <c r="M65" s="181"/>
-      <c r="N65" s="181"/>
-      <c r="O65" s="181"/>
-      <c r="P65" s="186"/>
-      <c r="Q65" s="181" t="s">
+      <c r="M65" s="203"/>
+      <c r="N65" s="203"/>
+      <c r="O65" s="203"/>
+      <c r="P65" s="193"/>
+      <c r="Q65" s="203" t="s">
         <v>90</v>
       </c>
-      <c r="R65" s="181"/>
-      <c r="S65" s="181"/>
-      <c r="T65" s="181"/>
-      <c r="U65" s="186"/>
+      <c r="R65" s="203"/>
+      <c r="S65" s="203"/>
+      <c r="T65" s="203"/>
+      <c r="U65" s="193"/>
     </row>
     <row r="66" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
@@ -5866,19 +5987,19 @@
       <c r="U67" s="140">
         <v>0.08</v>
       </c>
-      <c r="X67" s="177" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y67" s="177"/>
-      <c r="Z67" s="177"/>
-      <c r="AA67" s="177"/>
-      <c r="AB67" s="177"/>
-      <c r="AC67" s="177"/>
-      <c r="AD67" s="177"/>
-      <c r="AE67" s="177"/>
-      <c r="AF67" s="177"/>
-      <c r="AG67" s="177"/>
-      <c r="AH67" s="177"/>
+      <c r="X67" s="195" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y67" s="195"/>
+      <c r="Z67" s="195"/>
+      <c r="AA67" s="195"/>
+      <c r="AB67" s="195"/>
+      <c r="AC67" s="195"/>
+      <c r="AD67" s="195"/>
+      <c r="AE67" s="195"/>
+      <c r="AF67" s="195"/>
+      <c r="AG67" s="195"/>
+      <c r="AH67" s="195"/>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68" s="130" t="s">
@@ -5944,20 +6065,20 @@
       <c r="U68" s="5">
         <v>0.05</v>
       </c>
-      <c r="Y68" s="192" t="s">
+      <c r="Y68" s="196" t="s">
         <v>49</v>
       </c>
-      <c r="Z68" s="193"/>
-      <c r="AA68" s="193"/>
-      <c r="AB68" s="193"/>
-      <c r="AC68" s="194"/>
-      <c r="AD68" s="193" t="s">
+      <c r="Z68" s="197"/>
+      <c r="AA68" s="197"/>
+      <c r="AB68" s="197"/>
+      <c r="AC68" s="198"/>
+      <c r="AD68" s="197" t="s">
         <v>48</v>
       </c>
-      <c r="AE68" s="193"/>
-      <c r="AF68" s="193"/>
-      <c r="AG68" s="193"/>
-      <c r="AH68" s="194"/>
+      <c r="AE68" s="197"/>
+      <c r="AF68" s="197"/>
+      <c r="AG68" s="197"/>
+      <c r="AH68" s="198"/>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" s="130" t="s">
@@ -6086,10 +6207,10 @@
       <c r="S70" s="135"/>
       <c r="T70" s="135"/>
       <c r="U70" s="136"/>
-      <c r="W70" s="177" t="s">
+      <c r="W70" s="195" t="s">
         <v>34</v>
       </c>
-      <c r="X70" s="195"/>
+      <c r="X70" s="199"/>
       <c r="Y70" s="54"/>
       <c r="Z70" s="15"/>
       <c r="AA70" s="15"/>
@@ -6165,10 +6286,10 @@
       <c r="U71" s="140">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W71" s="177" t="s">
+      <c r="W71" s="195" t="s">
         <v>35</v>
       </c>
-      <c r="X71" s="195"/>
+      <c r="X71" s="199"/>
       <c r="Y71" s="159">
         <v>0.14179</v>
       </c>
@@ -6264,10 +6385,10 @@
       <c r="U72" s="151">
         <v>0.03</v>
       </c>
-      <c r="W72" s="177" t="s">
+      <c r="W72" s="195" t="s">
         <v>36</v>
       </c>
-      <c r="X72" s="195"/>
+      <c r="X72" s="199"/>
       <c r="Y72" s="159">
         <v>0.125</v>
       </c>
@@ -6363,10 +6484,10 @@
       <c r="U73" s="140">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W73" s="177" t="s">
+      <c r="W73" s="195" t="s">
         <v>37</v>
       </c>
-      <c r="X73" s="195"/>
+      <c r="X73" s="199"/>
       <c r="Y73" s="159">
         <v>0.3</v>
       </c>
@@ -6462,10 +6583,10 @@
       <c r="U74" s="143">
         <v>6.7831876028940266E-2</v>
       </c>
-      <c r="W74" s="177" t="s">
+      <c r="W74" s="195" t="s">
         <v>38</v>
       </c>
-      <c r="X74" s="195"/>
+      <c r="X74" s="199"/>
       <c r="Y74" s="159">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -6561,10 +6682,10 @@
       <c r="U75" s="140">
         <v>0.06</v>
       </c>
-      <c r="W75" s="177" t="s">
+      <c r="W75" s="195" t="s">
         <v>45</v>
       </c>
-      <c r="X75" s="195"/>
+      <c r="X75" s="199"/>
       <c r="Y75" s="159">
         <v>0.255</v>
       </c>
@@ -6660,10 +6781,10 @@
       <c r="U76" s="140">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W76" s="177" t="s">
+      <c r="W76" s="195" t="s">
         <v>47</v>
       </c>
-      <c r="X76" s="195"/>
+      <c r="X76" s="199"/>
       <c r="Y76" s="170">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -6727,10 +6848,10 @@
       <c r="S77" s="135"/>
       <c r="T77" s="135"/>
       <c r="U77" s="136"/>
-      <c r="W77" s="177" t="s">
+      <c r="W77" s="195" t="s">
         <v>50</v>
       </c>
-      <c r="X77" s="195"/>
+      <c r="X77" s="199"/>
       <c r="Y77" s="165">
         <v>7.5743000000000005E-2</v>
       </c>
@@ -6957,7 +7078,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81" s="130" t="s">
         <v>14</v>
       </c>
@@ -7022,7 +7143,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82" s="130" t="s">
         <v>15</v>
       </c>
@@ -7055,7 +7176,7 @@
       <c r="T82" s="135"/>
       <c r="U82" s="136"/>
     </row>
-    <row r="83" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="152" t="s">
         <v>16</v>
       </c>
@@ -7120,742 +7241,1538 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="238" t="s">
+    <row r="84" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="213" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="238"/>
-      <c r="D84" s="238"/>
-      <c r="E84" s="238"/>
-      <c r="F84" s="238"/>
-      <c r="G84" s="238" t="s">
+      <c r="C84" s="214"/>
+      <c r="D84" s="214"/>
+      <c r="E84" s="214"/>
+      <c r="F84" s="215"/>
+      <c r="G84" s="214" t="s">
         <v>90</v>
       </c>
-      <c r="H84" s="238"/>
-      <c r="I84" s="238"/>
-      <c r="J84" s="238"/>
-      <c r="K84" s="238"/>
-      <c r="L84" s="238" t="s">
+      <c r="H84" s="214"/>
+      <c r="I84" s="214"/>
+      <c r="J84" s="214"/>
+      <c r="K84" s="215"/>
+      <c r="L84" s="214" t="s">
         <v>89</v>
       </c>
-      <c r="M84" s="238"/>
-      <c r="N84" s="238"/>
-      <c r="O84" s="238"/>
-      <c r="P84" s="238"/>
-      <c r="Q84" s="238" t="s">
+      <c r="M84" s="214"/>
+      <c r="N84" s="214"/>
+      <c r="O84" s="214"/>
+      <c r="P84" s="215"/>
+      <c r="Q84" s="214" t="s">
         <v>90</v>
       </c>
-      <c r="R84" s="238"/>
-      <c r="S84" s="238"/>
-      <c r="T84" s="238"/>
-      <c r="U84" s="238"/>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A85" s="235" t="s">
+      <c r="R84" s="214"/>
+      <c r="S84" s="214"/>
+      <c r="T84" s="214"/>
+      <c r="U84" s="215"/>
+    </row>
+    <row r="85" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="177" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" s="178" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" s="178" t="s">
+        <v>19</v>
+      </c>
+      <c r="E85" s="178" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" s="179" t="s">
+        <v>39</v>
+      </c>
+      <c r="G85" s="178" t="s">
+        <v>17</v>
+      </c>
+      <c r="H85" s="178" t="s">
+        <v>40</v>
+      </c>
+      <c r="I85" s="178" t="s">
+        <v>19</v>
+      </c>
+      <c r="J85" s="178" t="s">
+        <v>20</v>
+      </c>
+      <c r="K85" s="179" t="s">
+        <v>39</v>
+      </c>
+      <c r="L85" s="178" t="s">
+        <v>17</v>
+      </c>
+      <c r="M85" s="178" t="s">
+        <v>40</v>
+      </c>
+      <c r="N85" s="178" t="s">
+        <v>19</v>
+      </c>
+      <c r="O85" s="178" t="s">
+        <v>20</v>
+      </c>
+      <c r="P85" s="179" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q85" s="178" t="s">
+        <v>17</v>
+      </c>
+      <c r="R85" s="178" t="s">
+        <v>40</v>
+      </c>
+      <c r="S85" s="178" t="s">
+        <v>19</v>
+      </c>
+      <c r="T85" s="178" t="s">
+        <v>20</v>
+      </c>
+      <c r="U85" s="179" t="s">
+        <v>39</v>
+      </c>
+      <c r="X85" s="195" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y85" s="195"/>
+      <c r="Z85" s="195"/>
+      <c r="AA85" s="195"/>
+      <c r="AB85" s="195"/>
+      <c r="AC85" s="195"/>
+      <c r="AD85" s="195"/>
+      <c r="AE85" s="195"/>
+      <c r="AF85" s="195"/>
+      <c r="AG85" s="195"/>
+      <c r="AH85" s="195"/>
+    </row>
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A86" s="181" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="141">
+        <v>0.1406896551724138</v>
+      </c>
+      <c r="C86" s="142">
+        <v>0.14241379310344823</v>
+      </c>
+      <c r="D86" s="147">
+        <v>0.10931034482758623</v>
+      </c>
+      <c r="E86" s="142">
+        <v>0.14551724137931038</v>
+      </c>
+      <c r="F86" s="143">
+        <v>0.13965517241379308</v>
+      </c>
+      <c r="G86" s="142">
+        <v>0.11752380952380966</v>
+      </c>
+      <c r="H86" s="142">
+        <v>0.11523809523809531</v>
+      </c>
+      <c r="I86" s="147">
+        <v>8.2380952380952222E-2</v>
+      </c>
+      <c r="J86" s="142">
+        <v>0.12228571428571439</v>
+      </c>
+      <c r="K86" s="143">
+        <v>0.11361904761904773</v>
+      </c>
+      <c r="L86" s="144">
+        <v>0.1</v>
+      </c>
+      <c r="M86" s="144">
+        <v>0.1</v>
+      </c>
+      <c r="N86" s="144">
+        <v>0.1</v>
+      </c>
+      <c r="O86" s="139">
+        <v>0.11</v>
+      </c>
+      <c r="P86" s="140">
+        <v>0.11</v>
+      </c>
+      <c r="Q86" s="147">
+        <v>9.2941058166131518E-2</v>
+      </c>
+      <c r="R86" s="142">
+        <v>9.6696345071482087E-2</v>
+      </c>
+      <c r="S86" s="142">
+        <v>9.5257987849231063E-2</v>
+      </c>
+      <c r="T86" s="147">
+        <v>9.3420648587009741E-2</v>
+      </c>
+      <c r="U86" s="143">
+        <v>9.7044040453526839E-2</v>
+      </c>
+      <c r="Y86" s="196" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z86" s="197"/>
+      <c r="AA86" s="197"/>
+      <c r="AB86" s="197"/>
+      <c r="AC86" s="198"/>
+      <c r="AD86" s="197" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE86" s="197"/>
+      <c r="AF86" s="197"/>
+      <c r="AG86" s="197"/>
+      <c r="AH86" s="198"/>
+    </row>
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A87" s="130" t="s">
         <v>95</v>
       </c>
-      <c r="B85" s="1"/>
-      <c r="C85" s="131"/>
-      <c r="D85" s="131"/>
-      <c r="E85" s="131"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="131"/>
-      <c r="H85" s="131"/>
-      <c r="I85" s="131"/>
-      <c r="J85" s="131"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="131"/>
-      <c r="M85" s="131"/>
-      <c r="N85" s="131"/>
-      <c r="O85" s="131"/>
-      <c r="P85" s="2"/>
-      <c r="Q85" s="131"/>
-      <c r="R85" s="131"/>
-      <c r="S85" s="131"/>
-      <c r="T85" s="131"/>
-      <c r="U85" s="2"/>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A86" s="236" t="s">
+      <c r="B87" s="148">
+        <v>0.16035714285714281</v>
+      </c>
+      <c r="C87" s="142">
+        <v>0.23071428571428568</v>
+      </c>
+      <c r="D87" s="142">
+        <v>0.17357142857142857</v>
+      </c>
+      <c r="E87" s="147">
+        <v>0.16035714285714286</v>
+      </c>
+      <c r="F87" s="143">
+        <v>0.1867857142857143</v>
+      </c>
+      <c r="G87" s="147">
+        <v>0.13451923076923064</v>
+      </c>
+      <c r="H87" s="142">
+        <v>0.24451923076923107</v>
+      </c>
+      <c r="I87" s="142">
+        <v>0.18749999999999997</v>
+      </c>
+      <c r="J87" s="142">
+        <v>0.13788461538461541</v>
+      </c>
+      <c r="K87" s="143">
+        <v>0.19173076923076937</v>
+      </c>
+      <c r="L87" s="144">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M87" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="N87" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="O87" s="144">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P87" s="151">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q87" s="142">
+        <v>6.8462728967336794E-2</v>
+      </c>
+      <c r="R87" s="142">
+        <v>5.648059736771547E-2</v>
+      </c>
+      <c r="S87" s="142">
+        <v>5.573428639187604E-2</v>
+      </c>
+      <c r="T87" s="142">
+        <v>6.6356979233947289E-2</v>
+      </c>
+      <c r="U87" s="146">
+        <v>5.0481993477099467E-2</v>
+      </c>
+      <c r="Y87" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z87" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA87" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC87" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD87" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE87" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF87" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH87" s="52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A88" s="130" t="s">
         <v>96</v>
       </c>
-      <c r="B86" s="3"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="5"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="5"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
-      <c r="S86" s="4"/>
-      <c r="T86" s="4"/>
-      <c r="U86" s="5"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A87" s="236" t="s">
-        <v>97</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-      <c r="K87" s="5"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-      <c r="P87" s="5"/>
-      <c r="Q87" s="4"/>
-      <c r="R87" s="4"/>
-      <c r="S87" s="4"/>
-      <c r="T87" s="4"/>
-      <c r="U87" s="5"/>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A88" s="236" t="s">
+      <c r="B88" s="141">
+        <v>0.12535714285714286</v>
+      </c>
+      <c r="C88" s="142">
+        <v>0.16750000000000001</v>
+      </c>
+      <c r="D88" s="142">
+        <v>0.13500000000000004</v>
+      </c>
+      <c r="E88" s="142">
+        <v>0.12535714285714286</v>
+      </c>
+      <c r="F88" s="146">
+        <v>0.10785714285714286</v>
+      </c>
+      <c r="G88" s="142">
+        <v>0.1170999999999999</v>
+      </c>
+      <c r="H88" s="142">
+        <v>0.16799999999999979</v>
+      </c>
+      <c r="I88" s="142">
+        <v>0.13090000000000004</v>
+      </c>
+      <c r="J88" s="142">
+        <v>0.1170999999999999</v>
+      </c>
+      <c r="K88" s="146">
+        <v>0.10159999999999995</v>
+      </c>
+      <c r="L88" s="142">
+        <v>6.4203504165192923E-2</v>
+      </c>
+      <c r="M88" s="142">
+        <v>8.9178348144478253E-2</v>
+      </c>
+      <c r="N88" s="142">
+        <v>7.6279214197043921E-2</v>
+      </c>
+      <c r="O88" s="142">
+        <v>6.4203504165192923E-2</v>
+      </c>
+      <c r="P88" s="146">
+        <v>5.4931414668296284E-2</v>
+      </c>
+      <c r="Q88" s="144">
+        <v>0.06</v>
+      </c>
+      <c r="R88" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="S88" s="139">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T88" s="144">
+        <v>0.06</v>
+      </c>
+      <c r="U88" s="151">
+        <v>0.06</v>
+      </c>
+      <c r="W88" s="195" t="s">
+        <v>34</v>
+      </c>
+      <c r="X88" s="199"/>
+      <c r="Y88" s="54"/>
+      <c r="Z88" s="15"/>
+      <c r="AA88" s="15"/>
+      <c r="AB88" s="15"/>
+      <c r="AC88" s="53"/>
+      <c r="AD88" s="4"/>
+      <c r="AE88" s="4"/>
+      <c r="AF88" s="4"/>
+      <c r="AG88" s="4"/>
+      <c r="AH88" s="52"/>
+    </row>
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A89" s="130" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="148">
+        <v>0.1767857142857143</v>
+      </c>
+      <c r="C89" s="142">
+        <v>0.20392857142857143</v>
+      </c>
+      <c r="D89" s="142">
+        <v>0.24571428571428564</v>
+      </c>
+      <c r="E89" s="142">
+        <v>0.20535714285714282</v>
+      </c>
+      <c r="F89" s="143">
+        <v>0.19571428571428576</v>
+      </c>
+      <c r="G89" s="147">
+        <v>0.14267857142857149</v>
+      </c>
+      <c r="H89" s="142">
+        <v>0.16223214285714291</v>
+      </c>
+      <c r="I89" s="142">
+        <v>0.20053571428571421</v>
+      </c>
+      <c r="J89" s="142">
+        <v>0.16553571428571442</v>
+      </c>
+      <c r="K89" s="143">
+        <v>0.15571428571428567</v>
+      </c>
+      <c r="L89" s="147">
+        <v>8.027976874556414E-2</v>
+      </c>
+      <c r="M89" s="142">
+        <v>8.7911541639531895E-2</v>
+      </c>
+      <c r="N89" s="142">
+        <v>9.3508905158361161E-2</v>
+      </c>
+      <c r="O89" s="142">
+        <v>8.7833265564264143E-2</v>
+      </c>
+      <c r="P89" s="143">
+        <v>8.6213712556670541E-2</v>
+      </c>
+      <c r="Q89" s="144">
+        <v>0.08</v>
+      </c>
+      <c r="R89" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="S89" s="139">
+        <v>0.1</v>
+      </c>
+      <c r="T89" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="U89" s="140">
+        <v>0.09</v>
+      </c>
+      <c r="W89" s="195" t="s">
+        <v>35</v>
+      </c>
+      <c r="X89" s="199"/>
+      <c r="Y89" s="159">
+        <v>0.17732999999999999</v>
+      </c>
+      <c r="Z89" s="160">
+        <v>0.17133000000000001</v>
+      </c>
+      <c r="AA89" s="160">
+        <v>0.12933</v>
+      </c>
+      <c r="AB89" s="160">
+        <v>0.14066999999999999</v>
+      </c>
+      <c r="AC89" s="161">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="AD89" s="162">
+        <v>0.16667000000000001</v>
+      </c>
+      <c r="AE89" s="162">
+        <v>0.15332999999999999</v>
+      </c>
+      <c r="AF89" s="162">
+        <v>0.11466999999999999</v>
+      </c>
+      <c r="AG89" s="162">
+        <v>0.12533</v>
+      </c>
+      <c r="AH89" s="163">
+        <v>0.11667</v>
+      </c>
+    </row>
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A90" s="130" t="s">
         <v>99</v>
       </c>
-      <c r="B88" s="175">
-        <v>0.1767857142857143</v>
-      </c>
-      <c r="C88" s="175">
-        <v>0.20392857142857143</v>
-      </c>
-      <c r="D88" s="175">
-        <v>0.24571428571428564</v>
-      </c>
-      <c r="E88" s="175">
-        <v>0.20535714285714282</v>
-      </c>
-      <c r="F88" s="175">
-        <v>0.19571428571428576</v>
-      </c>
-      <c r="G88" s="175">
-        <v>0.14267857142857149</v>
-      </c>
-      <c r="H88" s="175">
-        <v>0.16223214285714291</v>
-      </c>
-      <c r="I88" s="175">
-        <v>0.20053571428571421</v>
-      </c>
-      <c r="J88" s="175">
-        <v>0.16553571428571442</v>
-      </c>
-      <c r="K88" s="175">
-        <v>0.15571428571428567</v>
-      </c>
-      <c r="L88" s="175">
-        <v>8.027976874556414E-2</v>
-      </c>
-      <c r="M88" s="175">
-        <v>8.7911541639531895E-2</v>
-      </c>
-      <c r="N88" s="175">
-        <v>9.3508905158361161E-2</v>
-      </c>
-      <c r="O88" s="175">
-        <v>8.7833265564264143E-2</v>
-      </c>
-      <c r="P88" s="175">
-        <v>8.6213712556670541E-2</v>
-      </c>
-      <c r="Q88" s="239">
+      <c r="B90" s="148">
+        <v>0.16444444444444445</v>
+      </c>
+      <c r="C90" s="147">
+        <v>0.15777777777777777</v>
+      </c>
+      <c r="D90" s="147">
+        <v>0.15814814814814809</v>
+      </c>
+      <c r="E90" s="142">
+        <v>0.17518518518518522</v>
+      </c>
+      <c r="F90" s="146">
+        <v>0.15703703703703706</v>
+      </c>
+      <c r="G90" s="142">
+        <v>8.5142857142857117E-2</v>
+      </c>
+      <c r="H90" s="147">
+        <v>8.2666666666666735E-2</v>
+      </c>
+      <c r="I90" s="147">
+        <v>7.8761904761904672E-2</v>
+      </c>
+      <c r="J90" s="142">
+        <v>9.6476190476190521E-2</v>
+      </c>
+      <c r="K90" s="146">
+        <v>7.9333333333333311E-2</v>
+      </c>
+      <c r="L90" s="144">
+        <v>0.1</v>
+      </c>
+      <c r="M90" s="144">
+        <v>0.1</v>
+      </c>
+      <c r="N90" s="144">
+        <v>0.1</v>
+      </c>
+      <c r="O90" s="144">
+        <v>0.1</v>
+      </c>
+      <c r="P90" s="151">
+        <v>0.1</v>
+      </c>
+      <c r="Q90" s="144">
+        <v>0.05</v>
+      </c>
+      <c r="R90" s="144">
+        <v>0.05</v>
+      </c>
+      <c r="S90" s="144">
+        <v>0.05</v>
+      </c>
+      <c r="T90" s="139">
+        <v>0.06</v>
+      </c>
+      <c r="U90" s="151">
+        <v>0.05</v>
+      </c>
+      <c r="W90" s="195" t="s">
+        <v>36</v>
+      </c>
+      <c r="X90" s="199"/>
+      <c r="Y90" s="159">
+        <v>0.16</v>
+      </c>
+      <c r="Z90" s="160">
+        <v>0.17</v>
+      </c>
+      <c r="AA90" s="160">
+        <v>0.12</v>
+      </c>
+      <c r="AB90" s="162">
+        <v>0.13</v>
+      </c>
+      <c r="AC90" s="164">
+        <v>0.13</v>
+      </c>
+      <c r="AD90" s="160">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AE90" s="160">
+        <v>0.13</v>
+      </c>
+      <c r="AF90" s="160">
+        <v>0.12</v>
+      </c>
+      <c r="AG90" s="160">
+        <v>0.13</v>
+      </c>
+      <c r="AH90" s="163">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A91" s="130" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" s="141">
+        <v>0.26964285714285713</v>
+      </c>
+      <c r="C91" s="142">
+        <v>0.11535714285714291</v>
+      </c>
+      <c r="D91" s="147">
+        <v>8.3928571428571436E-2</v>
+      </c>
+      <c r="E91" s="142">
+        <v>0.115</v>
+      </c>
+      <c r="F91" s="146">
+        <v>8.4642857142857131E-2</v>
+      </c>
+      <c r="G91" s="142">
+        <v>0.27780952380952373</v>
+      </c>
+      <c r="H91" s="142">
+        <v>0.11476190476190475</v>
+      </c>
+      <c r="I91" s="147">
+        <v>8.7809523809523796E-2</v>
+      </c>
+      <c r="J91" s="142">
+        <v>0.12628571428571433</v>
+      </c>
+      <c r="K91" s="146">
+        <v>8.9904761904761848E-2</v>
+      </c>
+      <c r="L91" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="M91" s="139">
+        <v>0.06</v>
+      </c>
+      <c r="N91" s="144">
+        <v>0.05</v>
+      </c>
+      <c r="O91" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="P91" s="151">
+        <v>0.05</v>
+      </c>
+      <c r="Q91" s="142">
+        <v>9.4492378125484652E-2</v>
+      </c>
+      <c r="R91" s="142">
+        <v>6.3474635123246664E-2</v>
+      </c>
+      <c r="S91" s="147">
+        <v>5.2311584104305496E-2</v>
+      </c>
+      <c r="T91" s="142">
+        <v>8.9499217259760899E-2</v>
+      </c>
+      <c r="U91" s="146">
+        <v>5.2339410766781939E-2</v>
+      </c>
+      <c r="W91" s="195" t="s">
+        <v>37</v>
+      </c>
+      <c r="X91" s="199"/>
+      <c r="Y91" s="159">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Z91" s="160">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA91" s="160">
+        <v>0.25</v>
+      </c>
+      <c r="AB91" s="160">
+        <v>0.21</v>
+      </c>
+      <c r="AC91" s="164">
+        <v>0.2</v>
+      </c>
+      <c r="AD91" s="160">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AE91" s="160">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AF91" s="160">
+        <v>0.2</v>
+      </c>
+      <c r="AG91" s="160">
+        <v>0.17</v>
+      </c>
+      <c r="AH91" s="163">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A92" s="130" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92" s="141">
+        <v>0.2688888888888889</v>
+      </c>
+      <c r="C92" s="142">
+        <v>0.17629629629629626</v>
+      </c>
+      <c r="D92" s="142">
+        <v>0.1159259259259259</v>
+      </c>
+      <c r="E92" s="142">
+        <v>0.12777777777777774</v>
+      </c>
+      <c r="F92" s="146">
+        <v>0.10074074074074073</v>
+      </c>
+      <c r="G92" s="142">
+        <v>0.21163636363636373</v>
+      </c>
+      <c r="H92" s="142">
+        <v>0.11772727272727271</v>
+      </c>
+      <c r="I92" s="142">
+        <v>6.981818181818171E-2</v>
+      </c>
+      <c r="J92" s="142">
+        <v>7.3272727272727184E-2</v>
+      </c>
+      <c r="K92" s="146">
+        <v>6.4454545454545403E-2</v>
+      </c>
+      <c r="L92" s="139">
         <v>0.08</v>
       </c>
-      <c r="R88" s="239">
+      <c r="M92" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="N92" s="139">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O92" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="P92" s="151">
+        <v>0.05</v>
+      </c>
+      <c r="Q92" s="142">
+        <v>6.758653675073352E-2</v>
+      </c>
+      <c r="R92" s="142">
+        <v>6.8344232468876248E-2</v>
+      </c>
+      <c r="S92" s="142">
+        <v>5.7660534866297977E-2</v>
+      </c>
+      <c r="T92" s="142">
+        <v>6.0972381940237824E-2</v>
+      </c>
+      <c r="U92" s="146">
+        <v>4.5787429941166059E-2</v>
+      </c>
+      <c r="W92" s="195" t="s">
+        <v>38</v>
+      </c>
+      <c r="X92" s="199"/>
+      <c r="Y92" s="159">
+        <v>0.11</v>
+      </c>
+      <c r="Z92" s="160">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA92" s="160">
+        <v>0.08</v>
+      </c>
+      <c r="AB92" s="160">
         <v>0.09</v>
       </c>
-      <c r="S88" s="239">
+      <c r="AC92" s="164">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AD92" s="160">
+        <v>0.09</v>
+      </c>
+      <c r="AE92" s="160">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AF92" s="160">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AG92" s="160">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH92" s="163">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A93" s="130" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93" s="141">
+        <v>0.11642857142857144</v>
+      </c>
+      <c r="C93" s="147">
+        <v>9.857142857142856E-2</v>
+      </c>
+      <c r="D93" s="147">
+        <v>0.10142857142857145</v>
+      </c>
+      <c r="E93" s="142">
+        <v>0.1357142857142857</v>
+      </c>
+      <c r="F93" s="143">
+        <v>0.11214285714285717</v>
+      </c>
+      <c r="G93" s="142">
+        <v>0.12141509433962275</v>
+      </c>
+      <c r="H93" s="147">
+        <v>0.10830188679245289</v>
+      </c>
+      <c r="I93" s="142">
+        <v>0.1218867924528301</v>
+      </c>
+      <c r="J93" s="142">
+        <v>0.1379245283018867</v>
+      </c>
+      <c r="K93" s="143">
+        <v>0.11632075471698125</v>
+      </c>
+      <c r="L93" s="142">
+        <v>4.5233082429033691E-2</v>
+      </c>
+      <c r="M93" s="147">
+        <v>4.300855089090367E-2</v>
+      </c>
+      <c r="N93" s="142">
+        <v>5.6089497644672665E-2</v>
+      </c>
+      <c r="O93" s="142">
+        <v>4.7409060817728187E-2</v>
+      </c>
+      <c r="P93" s="146">
+        <v>4.4998530252306324E-2</v>
+      </c>
+      <c r="Q93" s="142">
+        <v>6.4843234830815694E-2</v>
+      </c>
+      <c r="R93" s="142">
+        <v>6.074884593241571E-2</v>
+      </c>
+      <c r="S93" s="147">
+        <v>4.6987601354423716E-2</v>
+      </c>
+      <c r="T93" s="142">
+        <v>6.8239312522804144E-2</v>
+      </c>
+      <c r="U93" s="143">
+        <v>6.72497190179734E-2</v>
+      </c>
+      <c r="W93" s="195" t="s">
+        <v>45</v>
+      </c>
+      <c r="X93" s="199"/>
+      <c r="Y93" s="159">
+        <v>0.17</v>
+      </c>
+      <c r="Z93" s="160">
+        <v>0.22</v>
+      </c>
+      <c r="AA93" s="160">
+        <v>0.17</v>
+      </c>
+      <c r="AB93" s="160">
+        <v>0.12</v>
+      </c>
+      <c r="AC93" s="164">
+        <v>0.13</v>
+      </c>
+      <c r="AD93" s="160">
+        <v>0.2</v>
+      </c>
+      <c r="AE93" s="160">
+        <v>0.22</v>
+      </c>
+      <c r="AF93" s="160">
+        <v>0.13</v>
+      </c>
+      <c r="AG93" s="160">
         <v>0.1</v>
       </c>
-      <c r="T88" s="239">
+      <c r="AH93" s="163">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A94" s="130" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="141">
+        <v>0.1867857142857143</v>
+      </c>
+      <c r="C94" s="142">
+        <v>0.17107142857142857</v>
+      </c>
+      <c r="D94" s="147">
+        <v>0.1467857142857143</v>
+      </c>
+      <c r="E94" s="142">
+        <v>0.18392857142857141</v>
+      </c>
+      <c r="F94" s="143">
+        <v>0.17178571428571429</v>
+      </c>
+      <c r="G94" s="142">
+        <v>0.16836363636363627</v>
+      </c>
+      <c r="H94" s="142">
+        <v>0.14645454545454548</v>
+      </c>
+      <c r="I94" s="147">
+        <v>0.11900000000000008</v>
+      </c>
+      <c r="J94" s="142">
+        <v>0.16209090909090906</v>
+      </c>
+      <c r="K94" s="143">
+        <v>0.14663636363636365</v>
+      </c>
+      <c r="L94" s="144">
+        <v>0.08</v>
+      </c>
+      <c r="M94" s="139">
         <v>0.09</v>
       </c>
-      <c r="U88" s="239">
+      <c r="N94" s="139">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A89" s="236" t="s">
-        <v>100</v>
-      </c>
-      <c r="B89" s="175">
-        <v>0.16444444444444445</v>
-      </c>
-      <c r="C89" s="175">
-        <v>0.15777777777777777</v>
-      </c>
-      <c r="D89" s="175">
-        <v>0.15814814814814809</v>
-      </c>
-      <c r="E89" s="175">
-        <v>0.17518518518518522</v>
-      </c>
-      <c r="F89" s="175">
-        <v>0.15703703703703706</v>
-      </c>
-      <c r="G89" s="175">
-        <v>8.5142857142857117E-2</v>
-      </c>
-      <c r="H89" s="175">
-        <v>8.2666666666666735E-2</v>
-      </c>
-      <c r="I89" s="175">
-        <v>7.8761904761904672E-2</v>
-      </c>
-      <c r="J89" s="175">
-        <v>9.6476190476190521E-2</v>
-      </c>
-      <c r="K89" s="175">
-        <v>7.9333333333333311E-2</v>
-      </c>
-      <c r="L89" s="239">
-        <v>0.1</v>
-      </c>
-      <c r="M89" s="239">
-        <v>0.1</v>
-      </c>
-      <c r="N89" s="239">
-        <v>0.1</v>
-      </c>
-      <c r="O89" s="239">
-        <v>0.1</v>
-      </c>
-      <c r="P89" s="239">
-        <v>0.1</v>
-      </c>
-      <c r="Q89" s="239">
+      <c r="O94" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="P94" s="140">
+        <v>0.09</v>
+      </c>
+      <c r="Q94" s="147">
+        <v>9.1305790010315954E-2</v>
+      </c>
+      <c r="R94" s="142">
+        <v>0.10087312735900489</v>
+      </c>
+      <c r="S94" s="142">
+        <v>0.10413426407349512</v>
+      </c>
+      <c r="T94" s="142">
+        <v>9.6165906474037263E-2</v>
+      </c>
+      <c r="U94" s="143">
+        <v>0.10088850483912387</v>
+      </c>
+      <c r="W94" s="195" t="s">
+        <v>47</v>
+      </c>
+      <c r="X94" s="199"/>
+      <c r="Y94" s="170">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Z94" s="171">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AA94" s="171">
+        <v>2E-3</v>
+      </c>
+      <c r="AB94" s="171">
+        <v>1E-3</v>
+      </c>
+      <c r="AC94" s="172">
+        <v>2E-3</v>
+      </c>
+      <c r="AD94" s="171">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AE94" s="171">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AF94" s="171">
+        <v>2E-3</v>
+      </c>
+      <c r="AG94" s="171">
+        <v>1E-3</v>
+      </c>
+      <c r="AH94" s="173">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A95" s="130" t="s">
+        <v>105</v>
+      </c>
+      <c r="B95" s="141">
+        <v>0.13034482758620691</v>
+      </c>
+      <c r="C95" s="147">
+        <v>7.3793103448275887E-2</v>
+      </c>
+      <c r="D95" s="142">
+        <v>9.2413793103448286E-2</v>
+      </c>
+      <c r="E95" s="142">
+        <v>0.13034482758620691</v>
+      </c>
+      <c r="F95" s="143">
+        <v>8.7241379310344869E-2</v>
+      </c>
+      <c r="G95" s="142">
+        <v>0.13415841584158425</v>
+      </c>
+      <c r="H95" s="147">
+        <v>7.2772277227722657E-2</v>
+      </c>
+      <c r="I95" s="142">
+        <v>9.3663366336633649E-2</v>
+      </c>
+      <c r="J95" s="142">
+        <v>0.13415841584158425</v>
+      </c>
+      <c r="K95" s="143">
+        <v>8.782178217821783E-2</v>
+      </c>
+      <c r="L95" s="142">
+        <v>8.1481056458396206E-2</v>
+      </c>
+      <c r="M95" s="147">
+        <v>7.4661799043776081E-2</v>
+      </c>
+      <c r="N95" s="142">
+        <v>7.7489869034317385E-2</v>
+      </c>
+      <c r="O95" s="142">
+        <v>8.1481056458396206E-2</v>
+      </c>
+      <c r="P95" s="146">
+        <v>7.3915808850539874E-2</v>
+      </c>
+      <c r="Q95" s="139">
+        <v>0.06</v>
+      </c>
+      <c r="R95" s="144">
         <v>0.05</v>
       </c>
-      <c r="R89" s="239">
+      <c r="S95" s="139">
+        <v>0.06</v>
+      </c>
+      <c r="T95" s="139">
+        <v>0.06</v>
+      </c>
+      <c r="U95" s="151">
         <v>0.05</v>
       </c>
-      <c r="S89" s="239">
-        <v>0.05</v>
-      </c>
-      <c r="T89" s="239">
+      <c r="W95" s="195" t="s">
+        <v>50</v>
+      </c>
+      <c r="X95" s="199"/>
+      <c r="Y95" s="165">
+        <v>5.5608999999999999E-2</v>
+      </c>
+      <c r="Z95" s="166">
+        <v>6.7808999999999994E-2</v>
+      </c>
+      <c r="AA95" s="166">
+        <v>4.2673000000000003E-2</v>
+      </c>
+      <c r="AB95" s="166">
+        <v>3.1952000000000001E-2</v>
+      </c>
+      <c r="AC95" s="167">
+        <v>3.9856999999999997E-2</v>
+      </c>
+      <c r="AD95" s="168">
+        <v>6.6188999999999998E-2</v>
+      </c>
+      <c r="AE95" s="168">
+        <v>6.8312999999999999E-2</v>
+      </c>
+      <c r="AF95" s="168">
+        <v>3.9254999999999998E-2</v>
+      </c>
+      <c r="AG95" s="168">
+        <v>2.9488E-2</v>
+      </c>
+      <c r="AH95" s="169">
+        <v>4.2032E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A96" s="130" t="s">
+        <v>106</v>
+      </c>
+      <c r="B96" s="141">
+        <v>0.15642857142857144</v>
+      </c>
+      <c r="C96" s="147">
+        <v>0.11499999999999999</v>
+      </c>
+      <c r="D96" s="142">
+        <v>0.13392857142857142</v>
+      </c>
+      <c r="E96" s="142">
+        <v>0.15071428571428577</v>
+      </c>
+      <c r="F96" s="146">
+        <v>0.11571428571428569</v>
+      </c>
+      <c r="G96" s="142">
+        <v>0.1766336633663366</v>
+      </c>
+      <c r="H96" s="147">
+        <v>0.12891089108910894</v>
+      </c>
+      <c r="I96" s="147">
+        <v>0.13108910891089115</v>
+      </c>
+      <c r="J96" s="142">
+        <v>0.16871287128712878</v>
+      </c>
+      <c r="K96" s="146">
+        <v>0.13000000000000003</v>
+      </c>
+      <c r="L96" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="M96" s="139">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N96" s="144">
+        <v>0.04</v>
+      </c>
+      <c r="O96" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="P96" s="140">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q96" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="R96" s="139">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S96" s="144">
+        <v>0.04</v>
+      </c>
+      <c r="T96" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="U96" s="140">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="152" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" s="141">
+        <v>0.15678571428571428</v>
+      </c>
+      <c r="C97" s="142">
+        <v>9.2857142857142874E-2</v>
+      </c>
+      <c r="D97" s="142">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E97" s="142">
+        <v>8.9285714285714302E-2</v>
+      </c>
+      <c r="F97" s="146">
+        <v>7.3214285714285746E-2</v>
+      </c>
+      <c r="G97" s="142">
+        <v>0.14509615384615387</v>
+      </c>
+      <c r="H97" s="142">
+        <v>7.9903846153846131E-2</v>
+      </c>
+      <c r="I97" s="142">
+        <v>6.6442307692307606E-2</v>
+      </c>
+      <c r="J97" s="142">
+        <v>7.5961538461538497E-2</v>
+      </c>
+      <c r="K97" s="146">
+        <v>5.3846153846153794E-2</v>
+      </c>
+      <c r="L97" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="M97" s="144">
         <v>0.06</v>
       </c>
-      <c r="U89" s="239">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A90" s="236" t="s">
-        <v>101</v>
-      </c>
-      <c r="B90" s="175">
-        <v>0.26964285714285713</v>
-      </c>
-      <c r="C90" s="175">
-        <v>0.11535714285714291</v>
-      </c>
-      <c r="D90" s="175">
-        <v>8.3928571428571436E-2</v>
-      </c>
-      <c r="E90" s="175">
-        <v>0.115</v>
-      </c>
-      <c r="F90" s="175">
-        <v>8.4642857142857131E-2</v>
-      </c>
-      <c r="G90" s="175">
-        <v>0.27780952380952373</v>
-      </c>
-      <c r="H90" s="175">
-        <v>0.11476190476190475</v>
-      </c>
-      <c r="I90" s="175">
-        <v>8.7809523809523796E-2</v>
-      </c>
-      <c r="J90" s="175">
-        <v>0.12628571428571433</v>
-      </c>
-      <c r="K90" s="175">
-        <v>8.9904761904761848E-2</v>
-      </c>
-      <c r="L90" s="239">
-        <v>0.09</v>
-      </c>
-      <c r="M90" s="239">
+      <c r="N97" s="144">
         <v>0.06</v>
       </c>
-      <c r="N90" s="239">
-        <v>0.05</v>
-      </c>
-      <c r="O90" s="239">
-        <v>0.09</v>
-      </c>
-      <c r="P90" s="239">
-        <v>0.05</v>
-      </c>
-      <c r="Q90" s="175">
-        <v>9.4492378125484652E-2</v>
-      </c>
-      <c r="R90" s="175">
-        <v>6.3474635123246664E-2</v>
-      </c>
-      <c r="S90" s="175">
-        <v>5.2311584104305496E-2</v>
-      </c>
-      <c r="T90" s="175">
-        <v>8.9499217259760899E-2</v>
-      </c>
-      <c r="U90" s="175">
-        <v>5.2339410766781939E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A91" s="236" t="s">
-        <v>102</v>
-      </c>
-      <c r="B91" s="175">
-        <v>0.2688888888888889</v>
-      </c>
-      <c r="C91" s="175">
-        <v>0.17629629629629626</v>
-      </c>
-      <c r="D91" s="175">
-        <v>0.1159259259259259</v>
-      </c>
-      <c r="E91" s="175">
-        <v>0.12777777777777774</v>
-      </c>
-      <c r="F91" s="175">
-        <v>0.10074074074074073</v>
-      </c>
-      <c r="G91" s="175">
-        <v>0.21163636363636373</v>
-      </c>
-      <c r="H91" s="175">
-        <v>0.11772727272727271</v>
-      </c>
-      <c r="I91" s="175">
-        <v>6.981818181818171E-2</v>
-      </c>
-      <c r="J91" s="175">
-        <v>7.3272727272727184E-2</v>
-      </c>
-      <c r="K91" s="175">
-        <v>6.4454545454545403E-2</v>
-      </c>
-      <c r="L91" s="239">
+      <c r="O97" s="139">
         <v>0.08</v>
       </c>
-      <c r="M91" s="239">
-        <v>0.08</v>
-      </c>
-      <c r="N91" s="239">
+      <c r="P97" s="140">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O91" s="239">
-        <v>0.08</v>
-      </c>
-      <c r="P91" s="239">
-        <v>0.05</v>
-      </c>
-      <c r="Q91" s="175">
-        <v>6.758653675073352E-2</v>
-      </c>
-      <c r="R91" s="175">
-        <v>6.8344232468876248E-2</v>
-      </c>
-      <c r="S91" s="175">
-        <v>5.7660534866297977E-2</v>
-      </c>
-      <c r="T91" s="175">
-        <v>6.0972381940237824E-2</v>
-      </c>
-      <c r="U91" s="175">
-        <v>4.5787429941166059E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A92" s="236" t="s">
-        <v>103</v>
-      </c>
-      <c r="B92" s="175">
-        <v>0.11642857142857144</v>
-      </c>
-      <c r="C92" s="175">
-        <v>9.857142857142856E-2</v>
-      </c>
-      <c r="D92" s="175">
-        <v>0.10142857142857145</v>
-      </c>
-      <c r="E92" s="175">
-        <v>0.1357142857142857</v>
-      </c>
-      <c r="F92" s="175">
-        <v>0.11214285714285717</v>
-      </c>
-      <c r="G92" s="175">
-        <v>0.12141509433962275</v>
-      </c>
-      <c r="H92" s="175">
-        <v>0.10830188679245289</v>
-      </c>
-      <c r="I92" s="175">
-        <v>0.1218867924528301</v>
-      </c>
-      <c r="J92" s="175">
-        <v>0.1379245283018867</v>
-      </c>
-      <c r="K92" s="175">
-        <v>0.11632075471698125</v>
-      </c>
-      <c r="L92" s="175">
-        <v>4.5233082429033691E-2</v>
-      </c>
-      <c r="M92" s="175">
-        <v>4.300855089090367E-2</v>
-      </c>
-      <c r="N92" s="175">
-        <v>5.6089497644672665E-2</v>
-      </c>
-      <c r="O92" s="175">
-        <v>4.7409060817728187E-2</v>
-      </c>
-      <c r="P92" s="175">
-        <v>4.4998530252306324E-2</v>
-      </c>
-      <c r="Q92" s="175">
-        <v>6.4843234830815694E-2</v>
-      </c>
-      <c r="R92" s="175">
-        <v>6.074884593241571E-2</v>
-      </c>
-      <c r="S92" s="175">
-        <v>4.6987601354423716E-2</v>
-      </c>
-      <c r="T92" s="175">
-        <v>6.8239312522804144E-2</v>
-      </c>
-      <c r="U92" s="175">
-        <v>6.72497190179734E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A93" s="236" t="s">
-        <v>105</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
-      <c r="K93" s="5"/>
-      <c r="L93" s="4"/>
-      <c r="M93" s="4"/>
-      <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
-      <c r="P93" s="5"/>
-      <c r="Q93" s="4"/>
-      <c r="R93" s="4"/>
-      <c r="S93" s="4"/>
-      <c r="T93" s="4"/>
-      <c r="U93" s="5"/>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A94" s="236" t="s">
-        <v>106</v>
-      </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
-      <c r="I94" s="4"/>
-      <c r="J94" s="4"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="4"/>
-      <c r="M94" s="4"/>
-      <c r="N94" s="4"/>
-      <c r="O94" s="4"/>
-      <c r="P94" s="5"/>
-      <c r="Q94" s="4"/>
-      <c r="R94" s="4"/>
-      <c r="S94" s="4"/>
-      <c r="T94" s="4"/>
-      <c r="U94" s="5"/>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A95" s="236" t="s">
-        <v>107</v>
-      </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
-      <c r="K95" s="5"/>
-      <c r="L95" s="4"/>
-      <c r="M95" s="4"/>
-      <c r="N95" s="4"/>
-      <c r="O95" s="4"/>
-      <c r="P95" s="5"/>
-      <c r="Q95" s="4"/>
-      <c r="R95" s="4"/>
-      <c r="S95" s="4"/>
-      <c r="T95" s="4"/>
-      <c r="U95" s="5"/>
-    </row>
-    <row r="96" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="237" t="s">
+      <c r="Q97" s="139">
+        <v>0.04</v>
+      </c>
+      <c r="R97" s="144">
+        <v>0.03</v>
+      </c>
+      <c r="S97" s="139">
+        <v>0.04</v>
+      </c>
+      <c r="T97" s="139">
+        <v>0.04</v>
+      </c>
+      <c r="U97" s="151">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="193"/>
+      <c r="B98" s="207" t="s">
+        <v>89</v>
+      </c>
+      <c r="C98" s="203"/>
+      <c r="D98" s="203"/>
+      <c r="E98" s="203"/>
+      <c r="F98" s="203"/>
+      <c r="G98" s="193"/>
+      <c r="H98" s="203" t="s">
+        <v>90</v>
+      </c>
+      <c r="I98" s="203"/>
+      <c r="J98" s="203"/>
+      <c r="K98" s="203"/>
+      <c r="L98" s="203"/>
+      <c r="M98" s="193"/>
+      <c r="N98" s="203" t="s">
+        <v>89</v>
+      </c>
+      <c r="O98" s="203"/>
+      <c r="P98" s="203"/>
+      <c r="Q98" s="203"/>
+      <c r="R98" s="203"/>
+      <c r="S98" s="193"/>
+      <c r="T98" s="203" t="s">
+        <v>90</v>
+      </c>
+      <c r="U98" s="203"/>
+      <c r="V98" s="203"/>
+      <c r="W98" s="203"/>
+      <c r="X98" s="203"/>
+      <c r="Y98" s="193"/>
+    </row>
+    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A99" s="194"/>
+      <c r="B99" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B96" s="6"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
-      <c r="I96" s="7"/>
-      <c r="J96" s="7"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="7"/>
-      <c r="M96" s="7"/>
-      <c r="N96" s="7"/>
-      <c r="O96" s="7"/>
-      <c r="P96" s="8"/>
-      <c r="Q96" s="7"/>
-      <c r="R96" s="7"/>
-      <c r="S96" s="7"/>
-      <c r="T96" s="7"/>
-      <c r="U96" s="8"/>
-    </row>
-    <row r="97" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="181" t="s">
-        <v>89</v>
-      </c>
-      <c r="C97" s="181"/>
-      <c r="D97" s="181"/>
-      <c r="E97" s="181"/>
-      <c r="F97" s="181"/>
-      <c r="G97" s="181"/>
-      <c r="H97" s="181" t="s">
-        <v>90</v>
-      </c>
-      <c r="I97" s="181"/>
-      <c r="J97" s="181"/>
-      <c r="K97" s="181"/>
-      <c r="L97" s="181"/>
-      <c r="M97" s="181"/>
-      <c r="N97" s="181" t="s">
-        <v>89</v>
-      </c>
-      <c r="O97" s="181"/>
-      <c r="P97" s="181"/>
-      <c r="Q97" s="181"/>
-      <c r="R97" s="181"/>
-      <c r="S97" s="181"/>
-      <c r="T97" s="177" t="s">
-        <v>90</v>
-      </c>
-      <c r="U97" s="177"/>
-      <c r="V97" s="177"/>
-      <c r="W97" s="177"/>
-      <c r="X97" s="177"/>
-      <c r="Y97" s="177"/>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1" t="s">
+      <c r="C99" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="C98" s="131" t="s">
-        <v>111</v>
-      </c>
-      <c r="D98" s="131" t="s">
+      <c r="D99" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="E98" s="131" t="s">
+      <c r="E99" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="F98" s="131" t="s">
+      <c r="F99" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H98" s="131" t="s">
+      <c r="H99" s="131" t="s">
+        <v>109</v>
+      </c>
+      <c r="I99" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="I98" s="131" t="s">
-        <v>111</v>
-      </c>
-      <c r="J98" s="131" t="s">
+      <c r="J99" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="K98" s="131" t="s">
+      <c r="K99" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="L98" s="131" t="s">
+      <c r="L99" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="M98" s="131" t="s">
+      <c r="M99" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N98" s="1" t="s">
+      <c r="N99" s="131" t="s">
+        <v>109</v>
+      </c>
+      <c r="O99" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="O98" s="131" t="s">
-        <v>111</v>
-      </c>
-      <c r="P98" s="131" t="s">
+      <c r="P99" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="Q98" s="131" t="s">
+      <c r="Q99" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="R98" s="131" t="s">
+      <c r="R99" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="S98" s="2" t="s">
+      <c r="S99" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T98" s="131" t="s">
+      <c r="T99" s="131" t="s">
+        <v>109</v>
+      </c>
+      <c r="U99" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="U98" s="131" t="s">
-        <v>111</v>
-      </c>
-      <c r="V98" s="131" t="s">
+      <c r="V99" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="W98" s="131" t="s">
+      <c r="W99" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="X98" s="131" t="s">
+      <c r="X99" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="Y98" s="2" t="s">
+      <c r="Y99" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A99" s="130" t="s">
-        <v>98</v>
-      </c>
-      <c r="B99" s="3"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
-      <c r="K99" s="4"/>
-      <c r="L99" s="4"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="4"/>
-      <c r="R99" s="4"/>
-      <c r="S99" s="5"/>
-      <c r="T99" s="4"/>
-      <c r="U99" s="4"/>
-      <c r="V99" s="4"/>
-      <c r="W99" s="4"/>
-      <c r="X99" s="4"/>
-      <c r="Y99" s="5"/>
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100" s="130" t="s">
-        <v>104</v>
-      </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="4"/>
-      <c r="K100" s="4"/>
-      <c r="L100" s="4"/>
-      <c r="M100" s="4"/>
-      <c r="N100" s="3"/>
-      <c r="O100" s="4"/>
-      <c r="P100" s="4"/>
-      <c r="Q100" s="4"/>
-      <c r="R100" s="4"/>
-      <c r="S100" s="5"/>
-      <c r="T100" s="4"/>
-      <c r="U100" s="4"/>
-      <c r="V100" s="4"/>
-      <c r="W100" s="4"/>
-      <c r="X100" s="4"/>
-      <c r="Y100" s="5"/>
-    </row>
-    <row r="101" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="152" t="s">
-        <v>108</v>
-      </c>
-      <c r="B101" s="6"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="7"/>
-      <c r="E101" s="7"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="7"/>
-      <c r="I101" s="7"/>
-      <c r="J101" s="7"/>
-      <c r="K101" s="7"/>
-      <c r="L101" s="7"/>
-      <c r="M101" s="7"/>
-      <c r="N101" s="6"/>
-      <c r="O101" s="7"/>
-      <c r="P101" s="7"/>
-      <c r="Q101" s="7"/>
-      <c r="R101" s="7"/>
-      <c r="S101" s="8"/>
-      <c r="T101" s="7"/>
-      <c r="U101" s="7"/>
-      <c r="V101" s="7"/>
-      <c r="W101" s="7"/>
-      <c r="X101" s="7"/>
-      <c r="Y101" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="B100" s="141">
+        <v>0.28448275862068967</v>
+      </c>
+      <c r="C100" s="142">
+        <v>0.22931034482758622</v>
+      </c>
+      <c r="D100" s="142">
+        <v>0.26034482758620686</v>
+      </c>
+      <c r="E100" s="142">
+        <v>0.13275862068965519</v>
+      </c>
+      <c r="F100" s="147">
+        <v>0.12448275862068967</v>
+      </c>
+      <c r="G100" s="143">
+        <v>0.17241379310344823</v>
+      </c>
+      <c r="H100" s="142">
+        <v>0.29161904761904756</v>
+      </c>
+      <c r="I100" s="142">
+        <v>0.23485714285714299</v>
+      </c>
+      <c r="J100" s="142">
+        <v>0.26371428571428573</v>
+      </c>
+      <c r="K100" s="142">
+        <v>0.12599999999999989</v>
+      </c>
+      <c r="L100" s="147">
+        <v>0.11952380952380956</v>
+      </c>
+      <c r="M100" s="143">
+        <v>0.15742857142857147</v>
+      </c>
+      <c r="N100" s="142">
+        <v>9.8292065037118306E-2</v>
+      </c>
+      <c r="O100" s="142">
+        <v>0.11164135928699666</v>
+      </c>
+      <c r="P100" s="142">
+        <v>0.10445377510174041</v>
+      </c>
+      <c r="Q100" s="142">
+        <v>6.600306008729219E-2</v>
+      </c>
+      <c r="R100" s="147">
+        <v>5.6479212794022869E-2</v>
+      </c>
+      <c r="S100" s="143">
+        <v>7.9131679244778722E-2</v>
+      </c>
+      <c r="T100" s="139">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U100" s="139">
+        <v>0.23</v>
+      </c>
+      <c r="V100" s="139">
+        <v>0.27</v>
+      </c>
+      <c r="W100" s="139">
+        <v>0.13</v>
+      </c>
+      <c r="X100" s="139">
+        <v>0.12</v>
+      </c>
+      <c r="Y100" s="140">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A101" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" s="184">
+        <v>0.19857142857142857</v>
+      </c>
+      <c r="C101" s="185">
+        <v>0.24142857142857146</v>
+      </c>
+      <c r="D101" s="185">
+        <v>0.26571428571428574</v>
+      </c>
+      <c r="E101" s="188">
+        <v>0.12357142857142858</v>
+      </c>
+      <c r="F101" s="188">
+        <v>0.12000000000000002</v>
+      </c>
+      <c r="G101" s="186">
+        <v>0.1257142857142857</v>
+      </c>
+      <c r="H101" s="142">
+        <v>0.27296610169491548</v>
+      </c>
+      <c r="I101" s="142">
+        <v>0.17906779661016942</v>
+      </c>
+      <c r="J101" s="142">
+        <v>0.20635593220338996</v>
+      </c>
+      <c r="K101" s="142">
+        <v>9.5338983050847342E-2</v>
+      </c>
+      <c r="L101" s="142">
+        <v>0.10093220338983042</v>
+      </c>
+      <c r="M101" s="146">
+        <v>9.4406779661016862E-2</v>
+      </c>
+      <c r="N101" s="139">
+        <v>0.13</v>
+      </c>
+      <c r="O101" s="139">
+        <v>0.11</v>
+      </c>
+      <c r="P101" s="139">
+        <v>0.11</v>
+      </c>
+      <c r="Q101" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="R101" s="144">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S101" s="140">
+        <v>0.08</v>
+      </c>
+      <c r="T101" s="139">
+        <v>0.09</v>
+      </c>
+      <c r="U101" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="V101" s="139">
+        <v>0.08</v>
+      </c>
+      <c r="W101" s="139">
+        <v>0.05</v>
+      </c>
+      <c r="X101" s="139">
+        <v>0.05</v>
+      </c>
+      <c r="Y101" s="140">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="152" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102" s="153">
+        <v>0.11392857142857145</v>
+      </c>
+      <c r="C102" s="154">
+        <v>0.24357142857142863</v>
+      </c>
+      <c r="D102" s="154">
+        <v>0.28892857142857137</v>
+      </c>
+      <c r="E102" s="189">
+        <v>0.10071428571428571</v>
+      </c>
+      <c r="F102" s="189">
+        <v>0.10250000000000001</v>
+      </c>
+      <c r="G102" s="155">
+        <v>0.13857142857142857</v>
+      </c>
+      <c r="H102" s="190">
+        <v>0.10262626262626262</v>
+      </c>
+      <c r="I102" s="180">
+        <v>0.25919191919191886</v>
+      </c>
+      <c r="J102" s="180">
+        <v>0.28757575757575732</v>
+      </c>
+      <c r="K102" s="180">
+        <v>0.12323232323232335</v>
+      </c>
+      <c r="L102" s="180">
+        <v>0.13020202020202029</v>
+      </c>
+      <c r="M102" s="187">
+        <v>0.16646464646464632</v>
+      </c>
+      <c r="N102" s="191">
+        <v>0.04</v>
+      </c>
+      <c r="O102" s="191">
+        <v>0.04</v>
+      </c>
+      <c r="P102" s="191">
+        <v>0.04</v>
+      </c>
+      <c r="Q102" s="191">
+        <v>0.04</v>
+      </c>
+      <c r="R102" s="191">
+        <v>0.04</v>
+      </c>
+      <c r="S102" s="192">
+        <v>0.04</v>
+      </c>
+      <c r="T102" s="182">
+        <v>0.04</v>
+      </c>
+      <c r="U102" s="182">
+        <v>0.04</v>
+      </c>
+      <c r="V102" s="191">
+        <v>0.03</v>
+      </c>
+      <c r="W102" s="191">
+        <v>0.03</v>
+      </c>
+      <c r="X102" s="182">
+        <v>0.04</v>
+      </c>
+      <c r="Y102" s="183">
+        <v>0.04</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="79">
     <mergeCell ref="B84:F84"/>
     <mergeCell ref="G84:K84"/>
     <mergeCell ref="L84:P84"/>
     <mergeCell ref="Q84:U84"/>
-    <mergeCell ref="B97:G97"/>
-    <mergeCell ref="H97:M97"/>
-    <mergeCell ref="N97:S97"/>
-    <mergeCell ref="T97:Y97"/>
+    <mergeCell ref="B98:G98"/>
+    <mergeCell ref="H98:M98"/>
+    <mergeCell ref="N98:S98"/>
+    <mergeCell ref="T98:Y98"/>
     <mergeCell ref="W73:X73"/>
     <mergeCell ref="W74:X74"/>
     <mergeCell ref="W75:X75"/>
@@ -7915,6 +8832,18 @@
     <mergeCell ref="AB23:AD23"/>
     <mergeCell ref="AE23:AG23"/>
     <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="X85:AH85"/>
+    <mergeCell ref="Y86:AC86"/>
+    <mergeCell ref="AD86:AH86"/>
+    <mergeCell ref="W88:X88"/>
+    <mergeCell ref="W89:X89"/>
+    <mergeCell ref="W90:X90"/>
+    <mergeCell ref="W91:X91"/>
+    <mergeCell ref="W92:X92"/>
+    <mergeCell ref="W93:X93"/>
+    <mergeCell ref="W94:X94"/>
+    <mergeCell ref="W95:X95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7957,48 +8886,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="220" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="222"/>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="222"/>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="222"/>
-      <c r="K1" s="223"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
+      <c r="I1" s="241"/>
+      <c r="J1" s="241"/>
+      <c r="K1" s="242"/>
       <c r="L1" s="65"/>
-      <c r="M1" s="201" t="s">
+      <c r="M1" s="220" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="202"/>
-      <c r="O1" s="202"/>
-      <c r="P1" s="202"/>
-      <c r="Q1" s="202"/>
-      <c r="R1" s="202"/>
-      <c r="S1" s="202"/>
-      <c r="T1" s="202"/>
-      <c r="U1" s="202"/>
-      <c r="V1" s="202"/>
-      <c r="W1" s="202"/>
-      <c r="X1" s="202"/>
-      <c r="Y1" s="202"/>
-      <c r="Z1" s="202"/>
-      <c r="AA1" s="202"/>
-      <c r="AB1" s="202"/>
-      <c r="AC1" s="202"/>
-      <c r="AD1" s="202"/>
-      <c r="AE1" s="202"/>
-      <c r="AF1" s="202"/>
-      <c r="AG1" s="202"/>
-      <c r="AH1" s="202"/>
-      <c r="AI1" s="202"/>
-      <c r="AJ1" s="202"/>
-      <c r="AK1" s="202"/>
-      <c r="AL1" s="203"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="221"/>
+      <c r="R1" s="221"/>
+      <c r="S1" s="221"/>
+      <c r="T1" s="221"/>
+      <c r="U1" s="221"/>
+      <c r="V1" s="221"/>
+      <c r="W1" s="221"/>
+      <c r="X1" s="221"/>
+      <c r="Y1" s="221"/>
+      <c r="Z1" s="221"/>
+      <c r="AA1" s="221"/>
+      <c r="AB1" s="221"/>
+      <c r="AC1" s="221"/>
+      <c r="AD1" s="221"/>
+      <c r="AE1" s="221"/>
+      <c r="AF1" s="221"/>
+      <c r="AG1" s="221"/>
+      <c r="AH1" s="221"/>
+      <c r="AI1" s="221"/>
+      <c r="AJ1" s="221"/>
+      <c r="AK1" s="221"/>
+      <c r="AL1" s="222"/>
       <c r="AM1" s="71"/>
       <c r="AN1" s="71"/>
       <c r="AO1" s="71"/>
@@ -8014,44 +8943,44 @@
       <c r="AY1" s="72"/>
     </row>
     <row r="2" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="204"/>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="225"/>
+      <c r="A2" s="223"/>
+      <c r="B2" s="243"/>
+      <c r="C2" s="243"/>
+      <c r="D2" s="243"/>
+      <c r="E2" s="243"/>
+      <c r="F2" s="243"/>
+      <c r="G2" s="243"/>
+      <c r="H2" s="243"/>
+      <c r="I2" s="243"/>
+      <c r="J2" s="243"/>
+      <c r="K2" s="244"/>
       <c r="L2" s="74"/>
-      <c r="M2" s="204"/>
-      <c r="N2" s="205"/>
-      <c r="O2" s="205"/>
-      <c r="P2" s="205"/>
-      <c r="Q2" s="205"/>
-      <c r="R2" s="205"/>
-      <c r="S2" s="205"/>
-      <c r="T2" s="205"/>
-      <c r="U2" s="205"/>
-      <c r="V2" s="205"/>
-      <c r="W2" s="205"/>
-      <c r="X2" s="205"/>
-      <c r="Y2" s="205"/>
-      <c r="Z2" s="205"/>
-      <c r="AA2" s="205"/>
-      <c r="AB2" s="205"/>
-      <c r="AC2" s="205"/>
-      <c r="AD2" s="205"/>
-      <c r="AE2" s="205"/>
-      <c r="AF2" s="205"/>
-      <c r="AG2" s="205"/>
-      <c r="AH2" s="205"/>
-      <c r="AI2" s="205"/>
-      <c r="AJ2" s="205"/>
-      <c r="AK2" s="205"/>
-      <c r="AL2" s="206"/>
+      <c r="M2" s="223"/>
+      <c r="N2" s="224"/>
+      <c r="O2" s="224"/>
+      <c r="P2" s="224"/>
+      <c r="Q2" s="224"/>
+      <c r="R2" s="224"/>
+      <c r="S2" s="224"/>
+      <c r="T2" s="224"/>
+      <c r="U2" s="224"/>
+      <c r="V2" s="224"/>
+      <c r="W2" s="224"/>
+      <c r="X2" s="224"/>
+      <c r="Y2" s="224"/>
+      <c r="Z2" s="224"/>
+      <c r="AA2" s="224"/>
+      <c r="AB2" s="224"/>
+      <c r="AC2" s="224"/>
+      <c r="AD2" s="224"/>
+      <c r="AE2" s="224"/>
+      <c r="AF2" s="224"/>
+      <c r="AG2" s="224"/>
+      <c r="AH2" s="224"/>
+      <c r="AI2" s="224"/>
+      <c r="AJ2" s="224"/>
+      <c r="AK2" s="224"/>
+      <c r="AL2" s="225"/>
       <c r="AM2" s="66"/>
       <c r="AN2" s="66"/>
       <c r="AO2" s="66"/>
@@ -8067,7 +8996,7 @@
       <c r="AY2" s="73"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A3" s="232"/>
+      <c r="A3" s="251"/>
       <c r="B3" s="93" t="s">
         <v>76</v>
       </c>
@@ -8086,57 +9015,57 @@
       <c r="G3" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="217" t="s">
+      <c r="H3" s="236" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="215" t="s">
+      <c r="I3" s="234" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="215" t="s">
+      <c r="J3" s="234" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="216" t="s">
+      <c r="K3" s="235" t="s">
         <v>70</v>
       </c>
       <c r="L3" s="77"/>
-      <c r="M3" s="226"/>
-      <c r="N3" s="227"/>
-      <c r="O3" s="214" t="s">
+      <c r="M3" s="245"/>
+      <c r="N3" s="246"/>
+      <c r="O3" s="233" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="215"/>
-      <c r="Q3" s="215"/>
-      <c r="R3" s="216"/>
-      <c r="S3" s="215" t="s">
+      <c r="P3" s="234"/>
+      <c r="Q3" s="234"/>
+      <c r="R3" s="235"/>
+      <c r="S3" s="234" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="215"/>
-      <c r="U3" s="215"/>
-      <c r="V3" s="216"/>
-      <c r="W3" s="197" t="s">
+      <c r="T3" s="234"/>
+      <c r="U3" s="234"/>
+      <c r="V3" s="235"/>
+      <c r="W3" s="216" t="s">
         <v>18</v>
       </c>
-      <c r="X3" s="197"/>
-      <c r="Y3" s="197"/>
-      <c r="Z3" s="198"/>
-      <c r="AA3" s="197" t="s">
+      <c r="X3" s="216"/>
+      <c r="Y3" s="216"/>
+      <c r="Z3" s="217"/>
+      <c r="AA3" s="216" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="197"/>
-      <c r="AC3" s="197"/>
-      <c r="AD3" s="198"/>
-      <c r="AE3" s="197" t="s">
+      <c r="AB3" s="216"/>
+      <c r="AC3" s="216"/>
+      <c r="AD3" s="217"/>
+      <c r="AE3" s="216" t="s">
         <v>20</v>
       </c>
-      <c r="AF3" s="197"/>
-      <c r="AG3" s="197"/>
-      <c r="AH3" s="198"/>
-      <c r="AI3" s="197" t="s">
+      <c r="AF3" s="216"/>
+      <c r="AG3" s="216"/>
+      <c r="AH3" s="217"/>
+      <c r="AI3" s="216" t="s">
         <v>21</v>
       </c>
-      <c r="AJ3" s="197"/>
-      <c r="AK3" s="197"/>
-      <c r="AL3" s="198"/>
+      <c r="AJ3" s="216"/>
+      <c r="AK3" s="216"/>
+      <c r="AL3" s="217"/>
       <c r="AM3" s="68"/>
       <c r="AN3" s="68"/>
       <c r="AO3" s="68"/>
@@ -8152,80 +9081,80 @@
       <c r="AY3" s="68"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A4" s="233"/>
-      <c r="B4" s="207" t="s">
+      <c r="A4" s="252"/>
+      <c r="B4" s="226" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="209" t="s">
+      <c r="C4" s="228" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="209" t="s">
+      <c r="D4" s="228" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="209" t="s">
+      <c r="E4" s="228" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="209" t="s">
+      <c r="F4" s="228" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="211" t="s">
+      <c r="G4" s="230" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="218"/>
-      <c r="I4" s="209"/>
-      <c r="J4" s="209"/>
-      <c r="K4" s="213"/>
+      <c r="H4" s="237"/>
+      <c r="I4" s="228"/>
+      <c r="J4" s="228"/>
+      <c r="K4" s="232"/>
       <c r="L4" s="77"/>
-      <c r="M4" s="228"/>
-      <c r="N4" s="229"/>
-      <c r="O4" s="207" t="s">
+      <c r="M4" s="247"/>
+      <c r="N4" s="248"/>
+      <c r="O4" s="226" t="s">
         <v>74</v>
       </c>
-      <c r="P4" s="209"/>
-      <c r="Q4" s="209" t="s">
+      <c r="P4" s="228"/>
+      <c r="Q4" s="228" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="213"/>
-      <c r="S4" s="209" t="s">
+      <c r="R4" s="232"/>
+      <c r="S4" s="228" t="s">
         <v>74</v>
       </c>
-      <c r="T4" s="209"/>
-      <c r="U4" s="209" t="s">
+      <c r="T4" s="228"/>
+      <c r="U4" s="228" t="s">
         <v>75</v>
       </c>
-      <c r="V4" s="213"/>
-      <c r="W4" s="199" t="s">
+      <c r="V4" s="232"/>
+      <c r="W4" s="218" t="s">
         <v>74</v>
       </c>
-      <c r="X4" s="199"/>
-      <c r="Y4" s="199" t="s">
+      <c r="X4" s="218"/>
+      <c r="Y4" s="218" t="s">
         <v>75</v>
       </c>
-      <c r="Z4" s="200"/>
-      <c r="AA4" s="199" t="s">
+      <c r="Z4" s="219"/>
+      <c r="AA4" s="218" t="s">
         <v>74</v>
       </c>
-      <c r="AB4" s="199"/>
-      <c r="AC4" s="199" t="s">
+      <c r="AB4" s="218"/>
+      <c r="AC4" s="218" t="s">
         <v>75</v>
       </c>
-      <c r="AD4" s="200"/>
-      <c r="AE4" s="199" t="s">
+      <c r="AD4" s="219"/>
+      <c r="AE4" s="218" t="s">
         <v>74</v>
       </c>
-      <c r="AF4" s="199"/>
-      <c r="AG4" s="199" t="s">
+      <c r="AF4" s="218"/>
+      <c r="AG4" s="218" t="s">
         <v>75</v>
       </c>
-      <c r="AH4" s="200"/>
-      <c r="AI4" s="199" t="s">
+      <c r="AH4" s="219"/>
+      <c r="AI4" s="218" t="s">
         <v>74</v>
       </c>
-      <c r="AJ4" s="199"/>
-      <c r="AK4" s="199" t="s">
+      <c r="AJ4" s="218"/>
+      <c r="AK4" s="218" t="s">
         <v>75</v>
       </c>
-      <c r="AL4" s="200"/>
+      <c r="AL4" s="219"/>
       <c r="AM4" s="68"/>
       <c r="AN4" s="68"/>
       <c r="AO4" s="68"/>
@@ -8241,20 +9170,20 @@
       <c r="AY4" s="68"/>
     </row>
     <row r="5" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="234"/>
-      <c r="B5" s="208"/>
-      <c r="C5" s="210"/>
-      <c r="D5" s="210"/>
-      <c r="E5" s="210"/>
-      <c r="F5" s="210"/>
-      <c r="G5" s="212"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="210"/>
-      <c r="J5" s="210"/>
-      <c r="K5" s="220"/>
+      <c r="A5" s="253"/>
+      <c r="B5" s="227"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
+      <c r="G5" s="231"/>
+      <c r="H5" s="238"/>
+      <c r="I5" s="229"/>
+      <c r="J5" s="229"/>
+      <c r="K5" s="239"/>
       <c r="L5" s="78"/>
-      <c r="M5" s="230"/>
-      <c r="N5" s="231"/>
+      <c r="M5" s="249"/>
+      <c r="N5" s="250"/>
       <c r="O5" s="95" t="s">
         <v>73</v>
       </c>
@@ -9675,29 +10604,29 @@
     </row>
     <row r="24" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="220" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="222"/>
-      <c r="C25" s="222"/>
-      <c r="D25" s="222"/>
-      <c r="E25" s="222"/>
-      <c r="F25" s="222"/>
-      <c r="G25" s="222"/>
-      <c r="H25" s="222"/>
-      <c r="I25" s="222"/>
-      <c r="J25" s="222"/>
-      <c r="K25" s="222"/>
-      <c r="L25" s="222"/>
-      <c r="M25" s="222"/>
-      <c r="N25" s="222"/>
-      <c r="O25" s="222"/>
-      <c r="P25" s="222"/>
-      <c r="Q25" s="222"/>
-      <c r="R25" s="222"/>
-      <c r="S25" s="222"/>
-      <c r="T25" s="222"/>
-      <c r="U25" s="223"/>
+      <c r="B25" s="241"/>
+      <c r="C25" s="241"/>
+      <c r="D25" s="241"/>
+      <c r="E25" s="241"/>
+      <c r="F25" s="241"/>
+      <c r="G25" s="241"/>
+      <c r="H25" s="241"/>
+      <c r="I25" s="241"/>
+      <c r="J25" s="241"/>
+      <c r="K25" s="241"/>
+      <c r="L25" s="241"/>
+      <c r="M25" s="241"/>
+      <c r="N25" s="241"/>
+      <c r="O25" s="241"/>
+      <c r="P25" s="241"/>
+      <c r="Q25" s="241"/>
+      <c r="R25" s="241"/>
+      <c r="S25" s="241"/>
+      <c r="T25" s="241"/>
+      <c r="U25" s="242"/>
       <c r="Z25" s="4"/>
       <c r="AA25" s="66"/>
       <c r="AB25" s="66"/>
@@ -9726,27 +10655,27 @@
       <c r="AY25" s="66"/>
     </row>
     <row r="26" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="204"/>
-      <c r="B26" s="224"/>
-      <c r="C26" s="224"/>
-      <c r="D26" s="224"/>
-      <c r="E26" s="224"/>
-      <c r="F26" s="224"/>
-      <c r="G26" s="224"/>
-      <c r="H26" s="224"/>
-      <c r="I26" s="224"/>
-      <c r="J26" s="224"/>
-      <c r="K26" s="224"/>
-      <c r="L26" s="224"/>
-      <c r="M26" s="224"/>
-      <c r="N26" s="224"/>
-      <c r="O26" s="224"/>
-      <c r="P26" s="224"/>
-      <c r="Q26" s="224"/>
-      <c r="R26" s="224"/>
-      <c r="S26" s="224"/>
-      <c r="T26" s="224"/>
-      <c r="U26" s="225"/>
+      <c r="A26" s="223"/>
+      <c r="B26" s="243"/>
+      <c r="C26" s="243"/>
+      <c r="D26" s="243"/>
+      <c r="E26" s="243"/>
+      <c r="F26" s="243"/>
+      <c r="G26" s="243"/>
+      <c r="H26" s="243"/>
+      <c r="I26" s="243"/>
+      <c r="J26" s="243"/>
+      <c r="K26" s="243"/>
+      <c r="L26" s="243"/>
+      <c r="M26" s="243"/>
+      <c r="N26" s="243"/>
+      <c r="O26" s="243"/>
+      <c r="P26" s="243"/>
+      <c r="Q26" s="243"/>
+      <c r="R26" s="243"/>
+      <c r="S26" s="243"/>
+      <c r="T26" s="243"/>
+      <c r="U26" s="244"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="66"/>
       <c r="AB26" s="66"/>
@@ -9776,46 +10705,46 @@
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" s="75"/>
-      <c r="B27" s="181" t="s">
+      <c r="B27" s="203" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="186"/>
-      <c r="D27" s="181" t="s">
+      <c r="C27" s="193"/>
+      <c r="D27" s="203" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="186"/>
-      <c r="F27" s="178" t="s">
+      <c r="E27" s="193"/>
+      <c r="F27" s="200" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="221"/>
-      <c r="H27" s="182" t="s">
+      <c r="G27" s="240"/>
+      <c r="H27" s="204" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="221"/>
-      <c r="J27" s="178" t="s">
+      <c r="I27" s="240"/>
+      <c r="J27" s="200" t="s">
         <v>82</v>
       </c>
-      <c r="K27" s="221"/>
-      <c r="L27" s="178" t="s">
+      <c r="K27" s="240"/>
+      <c r="L27" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="M27" s="221"/>
-      <c r="N27" s="178" t="s">
+      <c r="M27" s="240"/>
+      <c r="N27" s="200" t="s">
         <v>84</v>
       </c>
-      <c r="O27" s="221"/>
-      <c r="P27" s="178" t="s">
+      <c r="O27" s="240"/>
+      <c r="P27" s="200" t="s">
         <v>85</v>
       </c>
-      <c r="Q27" s="221"/>
-      <c r="R27" s="178" t="s">
+      <c r="Q27" s="240"/>
+      <c r="R27" s="200" t="s">
         <v>86</v>
       </c>
-      <c r="S27" s="221"/>
-      <c r="T27" s="178" t="s">
+      <c r="S27" s="240"/>
+      <c r="T27" s="200" t="s">
         <v>87</v>
       </c>
-      <c r="U27" s="221"/>
+      <c r="U27" s="240"/>
     </row>
     <row r="28" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="76"/>
@@ -10821,95 +11750,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="I1" s="200"/>
+      <c r="J1" s="200"/>
+      <c r="K1" s="200"/>
+      <c r="L1" s="200"/>
+      <c r="M1" s="200"/>
+      <c r="N1" s="200"/>
+      <c r="O1" s="200"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="181" t="s">
+      <c r="S1" s="203" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="181"/>
-      <c r="U1" s="181"/>
-      <c r="V1" s="181"/>
-      <c r="W1" s="181"/>
-      <c r="X1" s="181"/>
-      <c r="Y1" s="181"/>
-      <c r="Z1" s="181"/>
-      <c r="AA1" s="181"/>
-      <c r="AB1" s="181"/>
-      <c r="AC1" s="181"/>
-      <c r="AD1" s="181"/>
-      <c r="AE1" s="181"/>
-      <c r="AF1" s="181"/>
+      <c r="T1" s="203"/>
+      <c r="U1" s="203"/>
+      <c r="V1" s="203"/>
+      <c r="W1" s="203"/>
+      <c r="X1" s="203"/>
+      <c r="Y1" s="203"/>
+      <c r="Z1" s="203"/>
+      <c r="AA1" s="203"/>
+      <c r="AB1" s="203"/>
+      <c r="AC1" s="203"/>
+      <c r="AD1" s="203"/>
+      <c r="AE1" s="203"/>
+      <c r="AF1" s="203"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179" t="s">
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179" t="s">
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="179"/>
-      <c r="J2" s="179"/>
-      <c r="K2" s="179" t="s">
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="179"/>
-      <c r="M2" s="179"/>
-      <c r="N2" s="179" t="s">
+      <c r="L2" s="201"/>
+      <c r="M2" s="201"/>
+      <c r="N2" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="179"/>
-      <c r="P2" s="180"/>
+      <c r="O2" s="201"/>
+      <c r="P2" s="202"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="179" t="s">
+      <c r="S2" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="179"/>
-      <c r="U2" s="179"/>
-      <c r="V2" s="179" t="s">
+      <c r="T2" s="201"/>
+      <c r="U2" s="201"/>
+      <c r="V2" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="179"/>
-      <c r="X2" s="179"/>
-      <c r="Y2" s="179" t="s">
+      <c r="W2" s="201"/>
+      <c r="X2" s="201"/>
+      <c r="Y2" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="179"/>
-      <c r="AA2" s="179"/>
-      <c r="AB2" s="179" t="s">
+      <c r="Z2" s="201"/>
+      <c r="AA2" s="201"/>
+      <c r="AB2" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="179"/>
-      <c r="AD2" s="179"/>
-      <c r="AE2" s="179" t="s">
+      <c r="AC2" s="201"/>
+      <c r="AD2" s="201"/>
+      <c r="AE2" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="180"/>
+      <c r="AF2" s="201"/>
+      <c r="AG2" s="202"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -11678,95 +12607,95 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="178" t="s">
+      <c r="B22" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="178"/>
-      <c r="D22" s="178"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="178"/>
-      <c r="H22" s="178"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="178"/>
-      <c r="K22" s="178"/>
-      <c r="L22" s="178"/>
-      <c r="M22" s="178"/>
-      <c r="N22" s="178"/>
-      <c r="O22" s="178"/>
+      <c r="C22" s="200"/>
+      <c r="D22" s="200"/>
+      <c r="E22" s="200"/>
+      <c r="F22" s="200"/>
+      <c r="G22" s="200"/>
+      <c r="H22" s="200"/>
+      <c r="I22" s="200"/>
+      <c r="J22" s="200"/>
+      <c r="K22" s="200"/>
+      <c r="L22" s="200"/>
+      <c r="M22" s="200"/>
+      <c r="N22" s="200"/>
+      <c r="O22" s="200"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="181" t="s">
+      <c r="S22" s="203" t="s">
         <v>29</v>
       </c>
-      <c r="T22" s="181"/>
-      <c r="U22" s="181"/>
-      <c r="V22" s="181"/>
-      <c r="W22" s="181"/>
-      <c r="X22" s="181"/>
-      <c r="Y22" s="181"/>
-      <c r="Z22" s="181"/>
-      <c r="AA22" s="181"/>
-      <c r="AB22" s="181"/>
-      <c r="AC22" s="181"/>
-      <c r="AD22" s="181"/>
-      <c r="AE22" s="181"/>
-      <c r="AF22" s="181"/>
+      <c r="T22" s="203"/>
+      <c r="U22" s="203"/>
+      <c r="V22" s="203"/>
+      <c r="W22" s="203"/>
+      <c r="X22" s="203"/>
+      <c r="Y22" s="203"/>
+      <c r="Z22" s="203"/>
+      <c r="AA22" s="203"/>
+      <c r="AB22" s="203"/>
+      <c r="AC22" s="203"/>
+      <c r="AD22" s="203"/>
+      <c r="AE22" s="203"/>
+      <c r="AF22" s="203"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="179" t="s">
+      <c r="B23" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="179"/>
-      <c r="D23" s="179"/>
-      <c r="E23" s="179" t="s">
+      <c r="C23" s="201"/>
+      <c r="D23" s="201"/>
+      <c r="E23" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="179"/>
-      <c r="G23" s="179"/>
-      <c r="H23" s="179" t="s">
+      <c r="F23" s="201"/>
+      <c r="G23" s="201"/>
+      <c r="H23" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="179"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="179" t="s">
+      <c r="I23" s="201"/>
+      <c r="J23" s="201"/>
+      <c r="K23" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="179"/>
-      <c r="M23" s="179"/>
-      <c r="N23" s="179" t="s">
+      <c r="L23" s="201"/>
+      <c r="M23" s="201"/>
+      <c r="N23" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="179"/>
+      <c r="O23" s="201"/>
       <c r="P23" s="5"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="179" t="s">
+      <c r="S23" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="179"/>
-      <c r="U23" s="179"/>
-      <c r="V23" s="179" t="s">
+      <c r="T23" s="201"/>
+      <c r="U23" s="201"/>
+      <c r="V23" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="179"/>
-      <c r="X23" s="179"/>
-      <c r="Y23" s="179" t="s">
+      <c r="W23" s="201"/>
+      <c r="X23" s="201"/>
+      <c r="Y23" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="179"/>
-      <c r="AA23" s="179"/>
-      <c r="AB23" s="179" t="s">
+      <c r="Z23" s="201"/>
+      <c r="AA23" s="201"/>
+      <c r="AB23" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="179"/>
-      <c r="AD23" s="179"/>
-      <c r="AE23" s="179" t="s">
+      <c r="AC23" s="201"/>
+      <c r="AD23" s="201"/>
+      <c r="AE23" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="179"/>
-      <c r="AG23" s="180"/>
+      <c r="AF23" s="201"/>
+      <c r="AG23" s="202"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -12533,95 +13462,95 @@
     <row r="42" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="178" t="s">
+      <c r="B43" s="200" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="178"/>
-      <c r="F43" s="178"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="178"/>
-      <c r="K43" s="178"/>
-      <c r="L43" s="178"/>
-      <c r="M43" s="178"/>
-      <c r="N43" s="178"/>
-      <c r="O43" s="178"/>
+      <c r="C43" s="200"/>
+      <c r="D43" s="200"/>
+      <c r="E43" s="200"/>
+      <c r="F43" s="200"/>
+      <c r="G43" s="200"/>
+      <c r="H43" s="200"/>
+      <c r="I43" s="200"/>
+      <c r="J43" s="200"/>
+      <c r="K43" s="200"/>
+      <c r="L43" s="200"/>
+      <c r="M43" s="200"/>
+      <c r="N43" s="200"/>
+      <c r="O43" s="200"/>
       <c r="P43" s="2"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="178" t="s">
+      <c r="S43" s="200" t="s">
         <v>30</v>
       </c>
-      <c r="T43" s="178"/>
-      <c r="U43" s="178"/>
-      <c r="V43" s="178"/>
-      <c r="W43" s="178"/>
-      <c r="X43" s="178"/>
-      <c r="Y43" s="178"/>
-      <c r="Z43" s="178"/>
-      <c r="AA43" s="178"/>
-      <c r="AB43" s="178"/>
-      <c r="AC43" s="178"/>
-      <c r="AD43" s="178"/>
-      <c r="AE43" s="178"/>
-      <c r="AF43" s="178"/>
+      <c r="T43" s="200"/>
+      <c r="U43" s="200"/>
+      <c r="V43" s="200"/>
+      <c r="W43" s="200"/>
+      <c r="X43" s="200"/>
+      <c r="Y43" s="200"/>
+      <c r="Z43" s="200"/>
+      <c r="AA43" s="200"/>
+      <c r="AB43" s="200"/>
+      <c r="AC43" s="200"/>
+      <c r="AD43" s="200"/>
+      <c r="AE43" s="200"/>
+      <c r="AF43" s="200"/>
       <c r="AG43" s="2"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="179" t="s">
+      <c r="B44" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="179"/>
-      <c r="D44" s="179"/>
-      <c r="E44" s="179" t="s">
+      <c r="C44" s="201"/>
+      <c r="D44" s="201"/>
+      <c r="E44" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="179"/>
-      <c r="G44" s="179"/>
-      <c r="H44" s="179" t="s">
+      <c r="F44" s="201"/>
+      <c r="G44" s="201"/>
+      <c r="H44" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="179"/>
-      <c r="J44" s="179"/>
-      <c r="K44" s="179" t="s">
+      <c r="I44" s="201"/>
+      <c r="J44" s="201"/>
+      <c r="K44" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="L44" s="179"/>
-      <c r="M44" s="179"/>
+      <c r="L44" s="201"/>
+      <c r="M44" s="201"/>
       <c r="N44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="O44" s="14"/>
       <c r="P44" s="5"/>
       <c r="R44" s="9"/>
-      <c r="S44" s="179" t="s">
+      <c r="S44" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="T44" s="179"/>
-      <c r="U44" s="179"/>
-      <c r="V44" s="179" t="s">
+      <c r="T44" s="201"/>
+      <c r="U44" s="201"/>
+      <c r="V44" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="W44" s="179"/>
-      <c r="X44" s="179"/>
-      <c r="Y44" s="179" t="s">
+      <c r="W44" s="201"/>
+      <c r="X44" s="201"/>
+      <c r="Y44" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="Z44" s="179"/>
-      <c r="AA44" s="179"/>
-      <c r="AB44" s="179" t="s">
+      <c r="Z44" s="201"/>
+      <c r="AA44" s="201"/>
+      <c r="AB44" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="AC44" s="179"/>
-      <c r="AD44" s="179"/>
-      <c r="AE44" s="179" t="s">
+      <c r="AC44" s="201"/>
+      <c r="AD44" s="201"/>
+      <c r="AE44" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="AF44" s="179"/>
-      <c r="AG44" s="180"/>
+      <c r="AF44" s="201"/>
+      <c r="AG44" s="202"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
@@ -13445,95 +14374,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="200" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="I1" s="200"/>
+      <c r="J1" s="200"/>
+      <c r="K1" s="200"/>
+      <c r="L1" s="200"/>
+      <c r="M1" s="200"/>
+      <c r="N1" s="200"/>
+      <c r="O1" s="200"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="178" t="s">
+      <c r="S1" s="200" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="178"/>
+      <c r="T1" s="200"/>
+      <c r="U1" s="200"/>
+      <c r="V1" s="200"/>
+      <c r="W1" s="200"/>
+      <c r="X1" s="200"/>
+      <c r="Y1" s="200"/>
+      <c r="Z1" s="200"/>
+      <c r="AA1" s="200"/>
+      <c r="AB1" s="200"/>
+      <c r="AC1" s="200"/>
+      <c r="AD1" s="200"/>
+      <c r="AE1" s="200"/>
+      <c r="AF1" s="200"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179" t="s">
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179" t="s">
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="179"/>
-      <c r="J2" s="179"/>
-      <c r="K2" s="179" t="s">
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="179"/>
-      <c r="M2" s="179"/>
-      <c r="N2" s="179" t="s">
+      <c r="L2" s="201"/>
+      <c r="M2" s="201"/>
+      <c r="N2" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="179"/>
-      <c r="P2" s="180"/>
+      <c r="O2" s="201"/>
+      <c r="P2" s="202"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="184" t="s">
+      <c r="S2" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="184"/>
-      <c r="U2" s="184"/>
-      <c r="V2" s="184" t="s">
+      <c r="T2" s="206"/>
+      <c r="U2" s="206"/>
+      <c r="V2" s="206" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="184"/>
-      <c r="X2" s="184"/>
-      <c r="Y2" s="184" t="s">
+      <c r="W2" s="206"/>
+      <c r="X2" s="206"/>
+      <c r="Y2" s="206" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="184"/>
-      <c r="AA2" s="184"/>
-      <c r="AB2" s="184" t="s">
+      <c r="Z2" s="206"/>
+      <c r="AA2" s="206"/>
+      <c r="AB2" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="184"/>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184" t="s">
+      <c r="AC2" s="206"/>
+      <c r="AD2" s="206"/>
+      <c r="AE2" s="206" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="184"/>
-      <c r="AG2" s="196"/>
+      <c r="AF2" s="206"/>
+      <c r="AG2" s="194"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -14302,51 +15231,51 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="178" t="s">
+      <c r="B22" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="178"/>
-      <c r="D22" s="178"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="178"/>
-      <c r="H22" s="178"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="178"/>
-      <c r="K22" s="178"/>
-      <c r="L22" s="178"/>
-      <c r="M22" s="178"/>
-      <c r="N22" s="178"/>
-      <c r="O22" s="178"/>
+      <c r="C22" s="200"/>
+      <c r="D22" s="200"/>
+      <c r="E22" s="200"/>
+      <c r="F22" s="200"/>
+      <c r="G22" s="200"/>
+      <c r="H22" s="200"/>
+      <c r="I22" s="200"/>
+      <c r="J22" s="200"/>
+      <c r="K22" s="200"/>
+      <c r="L22" s="200"/>
+      <c r="M22" s="200"/>
+      <c r="N22" s="200"/>
+      <c r="O22" s="200"/>
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="179" t="s">
+      <c r="B23" s="201" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="179"/>
-      <c r="D23" s="179"/>
-      <c r="E23" s="179" t="s">
+      <c r="C23" s="201"/>
+      <c r="D23" s="201"/>
+      <c r="E23" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="179"/>
-      <c r="G23" s="179"/>
-      <c r="H23" s="179" t="s">
+      <c r="F23" s="201"/>
+      <c r="G23" s="201"/>
+      <c r="H23" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="179"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="179" t="s">
+      <c r="I23" s="201"/>
+      <c r="J23" s="201"/>
+      <c r="K23" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="179"/>
-      <c r="M23" s="179"/>
-      <c r="N23" s="179" t="s">
+      <c r="L23" s="201"/>
+      <c r="M23" s="201"/>
+      <c r="N23" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="179"/>
-      <c r="P23" s="180"/>
+      <c r="O23" s="201"/>
+      <c r="P23" s="202"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>

</xml_diff>

<commit_message>
Bug fix in Matlab Scripts.
</commit_message>
<xml_diff>
--- a/Analysis/First Study/centroids_allquestions.xlsx
+++ b/Analysis/First Study/centroids_allquestions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="28700" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="26480" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Laboratory &amp; Online" sheetId="1" r:id="rId1"/>
@@ -960,7 +960,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1278,13 +1278,28 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1296,31 +1311,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1338,94 +1344,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1461,6 +1395,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="121">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -1860,10 +1864,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC102"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A75" zoomScale="118" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A63" zoomScale="118" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="AH93" sqref="AH93"/>
+      <selection pane="topRight" activeCell="M82" sqref="M82:P82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1874,36 +1878,36 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="203" t="s">
+      <c r="B1" s="197" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
-      <c r="J1" s="203"/>
-      <c r="K1" s="203"/>
-      <c r="L1" s="203"/>
-      <c r="M1" s="203"/>
-      <c r="N1" s="203"/>
-      <c r="O1" s="203"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="197"/>
+      <c r="K1" s="197"/>
+      <c r="L1" s="197"/>
+      <c r="M1" s="197"/>
+      <c r="N1" s="197"/>
+      <c r="O1" s="197"/>
       <c r="P1" s="2"/>
-      <c r="S1" s="195" t="s">
+      <c r="S1" s="199" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="195"/>
-      <c r="U1" s="195"/>
-      <c r="V1" s="195"/>
-      <c r="W1" s="195"/>
-      <c r="X1" s="195"/>
-      <c r="Y1" s="195"/>
-      <c r="Z1" s="195"/>
-      <c r="AA1" s="195"/>
-      <c r="AB1" s="195"/>
-      <c r="AC1" s="195"/>
+      <c r="T1" s="199"/>
+      <c r="U1" s="199"/>
+      <c r="V1" s="199"/>
+      <c r="W1" s="199"/>
+      <c r="X1" s="199"/>
+      <c r="Y1" s="199"/>
+      <c r="Z1" s="199"/>
+      <c r="AA1" s="199"/>
+      <c r="AB1" s="199"/>
+      <c r="AC1" s="199"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1931,21 +1935,21 @@
         <v>21</v>
       </c>
       <c r="O2" s="206"/>
-      <c r="P2" s="194"/>
-      <c r="T2" s="195" t="s">
+      <c r="P2" s="207"/>
+      <c r="T2" s="199" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="195"/>
-      <c r="V2" s="195"/>
-      <c r="W2" s="195"/>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="195" t="s">
+      <c r="U2" s="199"/>
+      <c r="V2" s="199"/>
+      <c r="W2" s="199"/>
+      <c r="X2" s="199"/>
+      <c r="Y2" s="199" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="195"/>
-      <c r="AA2" s="195"/>
-      <c r="AB2" s="195"/>
-      <c r="AC2" s="195"/>
+      <c r="Z2" s="199"/>
+      <c r="AA2" s="199"/>
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="199"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -2691,95 +2695,95 @@
     <row r="21" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="203" t="s">
+      <c r="B22" s="197" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="203"/>
-      <c r="D22" s="203"/>
-      <c r="E22" s="203"/>
-      <c r="F22" s="203"/>
-      <c r="G22" s="203"/>
-      <c r="H22" s="203"/>
-      <c r="I22" s="203"/>
-      <c r="J22" s="203"/>
-      <c r="K22" s="203"/>
-      <c r="L22" s="203"/>
-      <c r="M22" s="203"/>
-      <c r="N22" s="203"/>
-      <c r="O22" s="203"/>
+      <c r="C22" s="197"/>
+      <c r="D22" s="197"/>
+      <c r="E22" s="197"/>
+      <c r="F22" s="197"/>
+      <c r="G22" s="197"/>
+      <c r="H22" s="197"/>
+      <c r="I22" s="197"/>
+      <c r="J22" s="197"/>
+      <c r="K22" s="197"/>
+      <c r="L22" s="197"/>
+      <c r="M22" s="197"/>
+      <c r="N22" s="197"/>
+      <c r="O22" s="197"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="200" t="s">
+      <c r="S22" s="205" t="s">
         <v>60</v>
       </c>
-      <c r="T22" s="200"/>
-      <c r="U22" s="200"/>
-      <c r="V22" s="200"/>
-      <c r="W22" s="200"/>
-      <c r="X22" s="200"/>
-      <c r="Y22" s="200"/>
-      <c r="Z22" s="200"/>
-      <c r="AA22" s="200"/>
-      <c r="AB22" s="200"/>
-      <c r="AC22" s="200"/>
-      <c r="AD22" s="200"/>
-      <c r="AE22" s="200"/>
-      <c r="AF22" s="200"/>
+      <c r="T22" s="205"/>
+      <c r="U22" s="205"/>
+      <c r="V22" s="205"/>
+      <c r="W22" s="205"/>
+      <c r="X22" s="205"/>
+      <c r="Y22" s="205"/>
+      <c r="Z22" s="205"/>
+      <c r="AA22" s="205"/>
+      <c r="AB22" s="205"/>
+      <c r="AC22" s="205"/>
+      <c r="AD22" s="205"/>
+      <c r="AE22" s="205"/>
+      <c r="AF22" s="205"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="201" t="s">
+      <c r="B23" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="201"/>
-      <c r="D23" s="201"/>
-      <c r="E23" s="201" t="s">
+      <c r="C23" s="208"/>
+      <c r="D23" s="208"/>
+      <c r="E23" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="201"/>
-      <c r="G23" s="201"/>
-      <c r="H23" s="201" t="s">
+      <c r="F23" s="208"/>
+      <c r="G23" s="208"/>
+      <c r="H23" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="201"/>
-      <c r="J23" s="201"/>
-      <c r="K23" s="201" t="s">
+      <c r="I23" s="208"/>
+      <c r="J23" s="208"/>
+      <c r="K23" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="201"/>
-      <c r="M23" s="201"/>
-      <c r="N23" s="201" t="s">
+      <c r="L23" s="208"/>
+      <c r="M23" s="208"/>
+      <c r="N23" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="201"/>
-      <c r="P23" s="202"/>
+      <c r="O23" s="208"/>
+      <c r="P23" s="209"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="201" t="s">
+      <c r="S23" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="201"/>
-      <c r="U23" s="201"/>
-      <c r="V23" s="201" t="s">
+      <c r="T23" s="208"/>
+      <c r="U23" s="208"/>
+      <c r="V23" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="201"/>
-      <c r="X23" s="201"/>
-      <c r="Y23" s="201" t="s">
+      <c r="W23" s="208"/>
+      <c r="X23" s="208"/>
+      <c r="Y23" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="201"/>
-      <c r="AA23" s="201"/>
-      <c r="AB23" s="201" t="s">
+      <c r="Z23" s="208"/>
+      <c r="AA23" s="208"/>
+      <c r="AB23" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="201"/>
-      <c r="AD23" s="201"/>
-      <c r="AE23" s="201" t="s">
+      <c r="AC23" s="208"/>
+      <c r="AD23" s="208"/>
+      <c r="AE23" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="201"/>
-      <c r="AG23" s="202"/>
+      <c r="AF23" s="208"/>
+      <c r="AG23" s="209"/>
     </row>
     <row r="24" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -3863,159 +3867,159 @@
     <row r="42" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="200" t="s">
+      <c r="B43" s="205" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="200"/>
-      <c r="D43" s="200"/>
-      <c r="E43" s="200"/>
-      <c r="F43" s="200"/>
-      <c r="G43" s="200"/>
-      <c r="H43" s="200"/>
-      <c r="I43" s="200"/>
-      <c r="J43" s="200"/>
-      <c r="K43" s="200"/>
-      <c r="L43" s="200"/>
-      <c r="M43" s="200"/>
-      <c r="N43" s="200"/>
-      <c r="O43" s="200"/>
-      <c r="P43" s="200"/>
+      <c r="C43" s="205"/>
+      <c r="D43" s="205"/>
+      <c r="E43" s="205"/>
+      <c r="F43" s="205"/>
+      <c r="G43" s="205"/>
+      <c r="H43" s="205"/>
+      <c r="I43" s="205"/>
+      <c r="J43" s="205"/>
+      <c r="K43" s="205"/>
+      <c r="L43" s="205"/>
+      <c r="M43" s="205"/>
+      <c r="N43" s="205"/>
+      <c r="O43" s="205"/>
+      <c r="P43" s="205"/>
       <c r="Q43" s="46"/>
       <c r="R43" s="46"/>
       <c r="S43" s="47"/>
       <c r="T43" s="204" t="s">
         <v>62</v>
       </c>
-      <c r="U43" s="200"/>
-      <c r="V43" s="200"/>
-      <c r="W43" s="200"/>
-      <c r="X43" s="200"/>
-      <c r="Y43" s="200"/>
-      <c r="Z43" s="200"/>
-      <c r="AA43" s="200"/>
-      <c r="AB43" s="200"/>
-      <c r="AC43" s="200"/>
-      <c r="AD43" s="200"/>
-      <c r="AE43" s="200"/>
-      <c r="AF43" s="200"/>
-      <c r="AG43" s="200"/>
-      <c r="AH43" s="200"/>
+      <c r="U43" s="205"/>
+      <c r="V43" s="205"/>
+      <c r="W43" s="205"/>
+      <c r="X43" s="205"/>
+      <c r="Y43" s="205"/>
+      <c r="Z43" s="205"/>
+      <c r="AA43" s="205"/>
+      <c r="AB43" s="205"/>
+      <c r="AC43" s="205"/>
+      <c r="AD43" s="205"/>
+      <c r="AE43" s="205"/>
+      <c r="AF43" s="205"/>
+      <c r="AG43" s="205"/>
+      <c r="AH43" s="205"/>
       <c r="AI43" s="46"/>
       <c r="AJ43" s="46"/>
       <c r="AK43" s="47"/>
       <c r="AL43" s="204" t="s">
         <v>63</v>
       </c>
-      <c r="AM43" s="200"/>
-      <c r="AN43" s="200"/>
-      <c r="AO43" s="200"/>
-      <c r="AP43" s="200"/>
-      <c r="AQ43" s="200"/>
-      <c r="AR43" s="200"/>
-      <c r="AS43" s="200"/>
-      <c r="AT43" s="200"/>
-      <c r="AU43" s="200"/>
-      <c r="AV43" s="200"/>
-      <c r="AW43" s="200"/>
-      <c r="AX43" s="200"/>
-      <c r="AY43" s="200"/>
-      <c r="AZ43" s="200"/>
+      <c r="AM43" s="205"/>
+      <c r="AN43" s="205"/>
+      <c r="AO43" s="205"/>
+      <c r="AP43" s="205"/>
+      <c r="AQ43" s="205"/>
+      <c r="AR43" s="205"/>
+      <c r="AS43" s="205"/>
+      <c r="AT43" s="205"/>
+      <c r="AU43" s="205"/>
+      <c r="AV43" s="205"/>
+      <c r="AW43" s="205"/>
+      <c r="AX43" s="205"/>
+      <c r="AY43" s="205"/>
+      <c r="AZ43" s="205"/>
       <c r="BA43" s="48"/>
       <c r="BB43" s="48"/>
       <c r="BC43" s="49"/>
     </row>
     <row r="44" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
-      <c r="B44" s="212" t="s">
+      <c r="B44" s="214" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="212"/>
-      <c r="D44" s="212"/>
-      <c r="E44" s="209" t="s">
+      <c r="C44" s="214"/>
+      <c r="D44" s="214"/>
+      <c r="E44" s="211" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="209"/>
-      <c r="G44" s="209"/>
-      <c r="H44" s="209" t="s">
+      <c r="F44" s="211"/>
+      <c r="G44" s="211"/>
+      <c r="H44" s="211" t="s">
         <v>18</v>
       </c>
-      <c r="I44" s="209"/>
-      <c r="J44" s="209"/>
-      <c r="K44" s="210" t="s">
+      <c r="I44" s="211"/>
+      <c r="J44" s="211"/>
+      <c r="K44" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="L44" s="201"/>
-      <c r="M44" s="211"/>
-      <c r="N44" s="209" t="s">
+      <c r="L44" s="208"/>
+      <c r="M44" s="213"/>
+      <c r="N44" s="211" t="s">
         <v>20</v>
       </c>
-      <c r="O44" s="209"/>
-      <c r="P44" s="209"/>
-      <c r="Q44" s="201" t="s">
+      <c r="O44" s="211"/>
+      <c r="P44" s="211"/>
+      <c r="Q44" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="R44" s="201"/>
-      <c r="S44" s="202"/>
-      <c r="T44" s="205" t="s">
+      <c r="R44" s="208"/>
+      <c r="S44" s="209"/>
+      <c r="T44" s="215" t="s">
         <v>54</v>
       </c>
       <c r="U44" s="206"/>
       <c r="V44" s="206"/>
-      <c r="W44" s="201" t="s">
+      <c r="W44" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="X44" s="201"/>
-      <c r="Y44" s="201"/>
-      <c r="Z44" s="201" t="s">
+      <c r="X44" s="208"/>
+      <c r="Y44" s="208"/>
+      <c r="Z44" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="AA44" s="201"/>
-      <c r="AB44" s="201"/>
-      <c r="AC44" s="201" t="s">
+      <c r="AA44" s="208"/>
+      <c r="AB44" s="208"/>
+      <c r="AC44" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="AD44" s="201"/>
-      <c r="AE44" s="201"/>
-      <c r="AF44" s="201" t="s">
+      <c r="AD44" s="208"/>
+      <c r="AE44" s="208"/>
+      <c r="AF44" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="AG44" s="201"/>
-      <c r="AH44" s="201"/>
-      <c r="AI44" s="201" t="s">
+      <c r="AG44" s="208"/>
+      <c r="AH44" s="208"/>
+      <c r="AI44" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="AJ44" s="201"/>
-      <c r="AK44" s="202"/>
-      <c r="AL44" s="208" t="s">
+      <c r="AJ44" s="208"/>
+      <c r="AK44" s="209"/>
+      <c r="AL44" s="210" t="s">
         <v>54</v>
       </c>
-      <c r="AM44" s="201"/>
-      <c r="AN44" s="201"/>
-      <c r="AO44" s="201" t="s">
+      <c r="AM44" s="208"/>
+      <c r="AN44" s="208"/>
+      <c r="AO44" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="AP44" s="201"/>
-      <c r="AQ44" s="201"/>
-      <c r="AR44" s="201" t="s">
+      <c r="AP44" s="208"/>
+      <c r="AQ44" s="208"/>
+      <c r="AR44" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="AS44" s="201"/>
-      <c r="AT44" s="201"/>
-      <c r="AU44" s="201" t="s">
+      <c r="AS44" s="208"/>
+      <c r="AT44" s="208"/>
+      <c r="AU44" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="AV44" s="201"/>
-      <c r="AW44" s="201"/>
-      <c r="AX44" s="201" t="s">
+      <c r="AV44" s="208"/>
+      <c r="AW44" s="208"/>
+      <c r="AX44" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="AY44" s="201"/>
-      <c r="AZ44" s="201"/>
-      <c r="BA44" s="201" t="s">
+      <c r="AY44" s="208"/>
+      <c r="AZ44" s="208"/>
+      <c r="BA44" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="BB44" s="201"/>
-      <c r="BC44" s="202"/>
+      <c r="BB44" s="208"/>
+      <c r="BC44" s="209"/>
     </row>
     <row r="45" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
@@ -5804,61 +5808,61 @@
     </row>
     <row r="64" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="203" t="s">
+      <c r="B64" s="197" t="s">
         <v>91</v>
       </c>
-      <c r="C64" s="203"/>
-      <c r="D64" s="203"/>
-      <c r="E64" s="203"/>
-      <c r="F64" s="203"/>
-      <c r="G64" s="203"/>
-      <c r="H64" s="203"/>
-      <c r="I64" s="203"/>
-      <c r="J64" s="203"/>
-      <c r="K64" s="193"/>
-      <c r="L64" s="203" t="s">
+      <c r="C64" s="197"/>
+      <c r="D64" s="197"/>
+      <c r="E64" s="197"/>
+      <c r="F64" s="197"/>
+      <c r="G64" s="197"/>
+      <c r="H64" s="197"/>
+      <c r="I64" s="197"/>
+      <c r="J64" s="197"/>
+      <c r="K64" s="198"/>
+      <c r="L64" s="197" t="s">
         <v>92</v>
       </c>
-      <c r="M64" s="203"/>
-      <c r="N64" s="203"/>
-      <c r="O64" s="203"/>
-      <c r="P64" s="203"/>
-      <c r="Q64" s="203"/>
-      <c r="R64" s="203"/>
-      <c r="S64" s="203"/>
-      <c r="T64" s="203"/>
-      <c r="U64" s="193"/>
+      <c r="M64" s="197"/>
+      <c r="N64" s="197"/>
+      <c r="O64" s="197"/>
+      <c r="P64" s="197"/>
+      <c r="Q64" s="197"/>
+      <c r="R64" s="197"/>
+      <c r="S64" s="197"/>
+      <c r="T64" s="197"/>
+      <c r="U64" s="198"/>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-      <c r="B65" s="207" t="s">
+      <c r="B65" s="196" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="203"/>
-      <c r="D65" s="203"/>
-      <c r="E65" s="203"/>
-      <c r="F65" s="193"/>
-      <c r="G65" s="203" t="s">
+      <c r="C65" s="197"/>
+      <c r="D65" s="197"/>
+      <c r="E65" s="197"/>
+      <c r="F65" s="198"/>
+      <c r="G65" s="197" t="s">
         <v>90</v>
       </c>
-      <c r="H65" s="203"/>
-      <c r="I65" s="203"/>
-      <c r="J65" s="203"/>
-      <c r="K65" s="193"/>
-      <c r="L65" s="203" t="s">
+      <c r="H65" s="197"/>
+      <c r="I65" s="197"/>
+      <c r="J65" s="197"/>
+      <c r="K65" s="198"/>
+      <c r="L65" s="197" t="s">
         <v>89</v>
       </c>
-      <c r="M65" s="203"/>
-      <c r="N65" s="203"/>
-      <c r="O65" s="203"/>
-      <c r="P65" s="193"/>
-      <c r="Q65" s="203" t="s">
+      <c r="M65" s="197"/>
+      <c r="N65" s="197"/>
+      <c r="O65" s="197"/>
+      <c r="P65" s="198"/>
+      <c r="Q65" s="197" t="s">
         <v>90</v>
       </c>
-      <c r="R65" s="203"/>
-      <c r="S65" s="203"/>
-      <c r="T65" s="203"/>
-      <c r="U65" s="193"/>
+      <c r="R65" s="197"/>
+      <c r="S65" s="197"/>
+      <c r="T65" s="197"/>
+      <c r="U65" s="198"/>
     </row>
     <row r="66" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
@@ -5987,19 +5991,19 @@
       <c r="U67" s="140">
         <v>0.08</v>
       </c>
-      <c r="X67" s="195" t="s">
+      <c r="X67" s="199" t="s">
         <v>111</v>
       </c>
-      <c r="Y67" s="195"/>
-      <c r="Z67" s="195"/>
-      <c r="AA67" s="195"/>
-      <c r="AB67" s="195"/>
-      <c r="AC67" s="195"/>
-      <c r="AD67" s="195"/>
-      <c r="AE67" s="195"/>
-      <c r="AF67" s="195"/>
-      <c r="AG67" s="195"/>
-      <c r="AH67" s="195"/>
+      <c r="Y67" s="199"/>
+      <c r="Z67" s="199"/>
+      <c r="AA67" s="199"/>
+      <c r="AB67" s="199"/>
+      <c r="AC67" s="199"/>
+      <c r="AD67" s="199"/>
+      <c r="AE67" s="199"/>
+      <c r="AF67" s="199"/>
+      <c r="AG67" s="199"/>
+      <c r="AH67" s="199"/>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68" s="130" t="s">
@@ -6065,20 +6069,20 @@
       <c r="U68" s="5">
         <v>0.05</v>
       </c>
-      <c r="Y68" s="196" t="s">
+      <c r="Y68" s="201" t="s">
         <v>49</v>
       </c>
-      <c r="Z68" s="197"/>
-      <c r="AA68" s="197"/>
-      <c r="AB68" s="197"/>
-      <c r="AC68" s="198"/>
-      <c r="AD68" s="197" t="s">
+      <c r="Z68" s="202"/>
+      <c r="AA68" s="202"/>
+      <c r="AB68" s="202"/>
+      <c r="AC68" s="203"/>
+      <c r="AD68" s="202" t="s">
         <v>48</v>
       </c>
-      <c r="AE68" s="197"/>
-      <c r="AF68" s="197"/>
-      <c r="AG68" s="197"/>
-      <c r="AH68" s="198"/>
+      <c r="AE68" s="202"/>
+      <c r="AF68" s="202"/>
+      <c r="AG68" s="202"/>
+      <c r="AH68" s="203"/>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" s="130" t="s">
@@ -6207,10 +6211,10 @@
       <c r="S70" s="135"/>
       <c r="T70" s="135"/>
       <c r="U70" s="136"/>
-      <c r="W70" s="195" t="s">
+      <c r="W70" s="199" t="s">
         <v>34</v>
       </c>
-      <c r="X70" s="199"/>
+      <c r="X70" s="200"/>
       <c r="Y70" s="54"/>
       <c r="Z70" s="15"/>
       <c r="AA70" s="15"/>
@@ -6286,10 +6290,10 @@
       <c r="U71" s="140">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W71" s="195" t="s">
+      <c r="W71" s="199" t="s">
         <v>35</v>
       </c>
-      <c r="X71" s="199"/>
+      <c r="X71" s="200"/>
       <c r="Y71" s="159">
         <v>0.14179</v>
       </c>
@@ -6385,10 +6389,10 @@
       <c r="U72" s="151">
         <v>0.03</v>
       </c>
-      <c r="W72" s="195" t="s">
+      <c r="W72" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="X72" s="199"/>
+      <c r="X72" s="200"/>
       <c r="Y72" s="159">
         <v>0.125</v>
       </c>
@@ -6484,10 +6488,10 @@
       <c r="U73" s="140">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W73" s="195" t="s">
+      <c r="W73" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="X73" s="199"/>
+      <c r="X73" s="200"/>
       <c r="Y73" s="159">
         <v>0.3</v>
       </c>
@@ -6583,10 +6587,10 @@
       <c r="U74" s="143">
         <v>6.7831876028940266E-2</v>
       </c>
-      <c r="W74" s="195" t="s">
+      <c r="W74" s="199" t="s">
         <v>38</v>
       </c>
-      <c r="X74" s="199"/>
+      <c r="X74" s="200"/>
       <c r="Y74" s="159">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -6682,10 +6686,10 @@
       <c r="U75" s="140">
         <v>0.06</v>
       </c>
-      <c r="W75" s="195" t="s">
+      <c r="W75" s="199" t="s">
         <v>45</v>
       </c>
-      <c r="X75" s="199"/>
+      <c r="X75" s="200"/>
       <c r="Y75" s="159">
         <v>0.255</v>
       </c>
@@ -6781,10 +6785,10 @@
       <c r="U76" s="140">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W76" s="195" t="s">
+      <c r="W76" s="199" t="s">
         <v>47</v>
       </c>
-      <c r="X76" s="199"/>
+      <c r="X76" s="200"/>
       <c r="Y76" s="170">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -6823,35 +6827,67 @@
       <c r="B77" s="149">
         <v>0.06</v>
       </c>
-      <c r="C77" s="135"/>
-      <c r="D77" s="135"/>
-      <c r="E77" s="135"/>
-      <c r="F77" s="136"/>
+      <c r="C77" s="135">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D77" s="135">
+        <v>0.13</v>
+      </c>
+      <c r="E77" s="135">
+        <v>0.18</v>
+      </c>
+      <c r="F77" s="136">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="G77" s="150">
         <v>0.04</v>
       </c>
-      <c r="H77" s="135"/>
-      <c r="I77" s="135"/>
-      <c r="J77" s="135"/>
-      <c r="K77" s="136"/>
+      <c r="H77" s="254">
+        <v>0.12249999999999994</v>
+      </c>
+      <c r="I77" s="254">
+        <v>0.13617647058823532</v>
+      </c>
+      <c r="J77" s="254">
+        <v>0.18735294117647053</v>
+      </c>
+      <c r="K77" s="254">
+        <v>0.14735294117647074</v>
+      </c>
       <c r="L77" s="150">
         <v>0.09</v>
       </c>
-      <c r="M77" s="135"/>
-      <c r="N77" s="135"/>
-      <c r="O77" s="135"/>
-      <c r="P77" s="136"/>
+      <c r="M77" s="135">
+        <v>0.11752</v>
+      </c>
+      <c r="N77" s="135">
+        <v>0.28520000000000001</v>
+      </c>
+      <c r="O77" s="135">
+        <v>3.986E-2</v>
+      </c>
+      <c r="P77" s="136">
+        <v>2.7269999999999999E-2</v>
+      </c>
       <c r="Q77" s="150">
         <v>0.06</v>
       </c>
-      <c r="R77" s="135"/>
-      <c r="S77" s="135"/>
-      <c r="T77" s="135"/>
-      <c r="U77" s="136"/>
-      <c r="W77" s="195" t="s">
+      <c r="R77" s="255">
+        <v>0.1</v>
+      </c>
+      <c r="S77" s="255">
+        <v>0.02</v>
+      </c>
+      <c r="T77" s="255">
+        <v>0.02</v>
+      </c>
+      <c r="U77" s="255">
+        <v>0.01</v>
+      </c>
+      <c r="W77" s="199" t="s">
         <v>50</v>
       </c>
-      <c r="X77" s="199"/>
+      <c r="X77" s="200"/>
       <c r="Y77" s="165">
         <v>7.5743000000000005E-2</v>
       </c>
@@ -7150,31 +7186,63 @@
       <c r="B82" s="9">
         <v>0.21</v>
       </c>
-      <c r="C82" s="135"/>
-      <c r="D82" s="135"/>
-      <c r="E82" s="135"/>
-      <c r="F82" s="136"/>
+      <c r="C82" s="256">
+        <v>0.22</v>
+      </c>
+      <c r="D82" s="256">
+        <v>0.1</v>
+      </c>
+      <c r="E82" s="256">
+        <v>0.16</v>
+      </c>
+      <c r="F82" s="256">
+        <v>0.12</v>
+      </c>
       <c r="G82" s="10">
         <v>0.19</v>
       </c>
-      <c r="H82" s="135"/>
-      <c r="I82" s="135"/>
-      <c r="J82" s="135"/>
-      <c r="K82" s="136"/>
+      <c r="H82" s="256">
+        <v>0.17</v>
+      </c>
+      <c r="I82" s="256">
+        <v>0.1</v>
+      </c>
+      <c r="J82" s="256">
+        <v>0.15</v>
+      </c>
+      <c r="K82" s="256">
+        <v>0.11</v>
+      </c>
       <c r="L82" s="10">
         <v>0.1</v>
       </c>
-      <c r="M82" s="135"/>
-      <c r="N82" s="135"/>
-      <c r="O82" s="135"/>
-      <c r="P82" s="136"/>
+      <c r="M82" s="257">
+        <v>0.12</v>
+      </c>
+      <c r="N82" s="257">
+        <v>0.05</v>
+      </c>
+      <c r="O82" s="257">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P82" s="257">
+        <v>0.08</v>
+      </c>
       <c r="Q82" s="10">
         <v>0.12</v>
       </c>
-      <c r="R82" s="135"/>
-      <c r="S82" s="135"/>
-      <c r="T82" s="135"/>
-      <c r="U82" s="136"/>
+      <c r="R82" s="257">
+        <v>0.09</v>
+      </c>
+      <c r="S82" s="257">
+        <v>0.06</v>
+      </c>
+      <c r="T82" s="257">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U82" s="257">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="83" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="152" t="s">
@@ -7242,34 +7310,34 @@
       </c>
     </row>
     <row r="84" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="213" t="s">
+      <c r="B84" s="193" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="214"/>
-      <c r="D84" s="214"/>
-      <c r="E84" s="214"/>
-      <c r="F84" s="215"/>
-      <c r="G84" s="214" t="s">
+      <c r="C84" s="194"/>
+      <c r="D84" s="194"/>
+      <c r="E84" s="194"/>
+      <c r="F84" s="195"/>
+      <c r="G84" s="194" t="s">
         <v>90</v>
       </c>
-      <c r="H84" s="214"/>
-      <c r="I84" s="214"/>
-      <c r="J84" s="214"/>
-      <c r="K84" s="215"/>
-      <c r="L84" s="214" t="s">
+      <c r="H84" s="194"/>
+      <c r="I84" s="194"/>
+      <c r="J84" s="194"/>
+      <c r="K84" s="195"/>
+      <c r="L84" s="194" t="s">
         <v>89</v>
       </c>
-      <c r="M84" s="214"/>
-      <c r="N84" s="214"/>
-      <c r="O84" s="214"/>
-      <c r="P84" s="215"/>
-      <c r="Q84" s="214" t="s">
+      <c r="M84" s="194"/>
+      <c r="N84" s="194"/>
+      <c r="O84" s="194"/>
+      <c r="P84" s="195"/>
+      <c r="Q84" s="194" t="s">
         <v>90</v>
       </c>
-      <c r="R84" s="214"/>
-      <c r="S84" s="214"/>
-      <c r="T84" s="214"/>
-      <c r="U84" s="215"/>
+      <c r="R84" s="194"/>
+      <c r="S84" s="194"/>
+      <c r="T84" s="194"/>
+      <c r="U84" s="195"/>
     </row>
     <row r="85" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B85" s="177" t="s">
@@ -7332,19 +7400,19 @@
       <c r="U85" s="179" t="s">
         <v>39</v>
       </c>
-      <c r="X85" s="195" t="s">
+      <c r="X85" s="199" t="s">
         <v>112</v>
       </c>
-      <c r="Y85" s="195"/>
-      <c r="Z85" s="195"/>
-      <c r="AA85" s="195"/>
-      <c r="AB85" s="195"/>
-      <c r="AC85" s="195"/>
-      <c r="AD85" s="195"/>
-      <c r="AE85" s="195"/>
-      <c r="AF85" s="195"/>
-      <c r="AG85" s="195"/>
-      <c r="AH85" s="195"/>
+      <c r="Y85" s="199"/>
+      <c r="Z85" s="199"/>
+      <c r="AA85" s="199"/>
+      <c r="AB85" s="199"/>
+      <c r="AC85" s="199"/>
+      <c r="AD85" s="199"/>
+      <c r="AE85" s="199"/>
+      <c r="AF85" s="199"/>
+      <c r="AG85" s="199"/>
+      <c r="AH85" s="199"/>
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86" s="181" t="s">
@@ -7410,20 +7478,20 @@
       <c r="U86" s="143">
         <v>9.7044040453526839E-2</v>
       </c>
-      <c r="Y86" s="196" t="s">
+      <c r="Y86" s="201" t="s">
         <v>49</v>
       </c>
-      <c r="Z86" s="197"/>
-      <c r="AA86" s="197"/>
-      <c r="AB86" s="197"/>
-      <c r="AC86" s="198"/>
-      <c r="AD86" s="197" t="s">
+      <c r="Z86" s="202"/>
+      <c r="AA86" s="202"/>
+      <c r="AB86" s="202"/>
+      <c r="AC86" s="203"/>
+      <c r="AD86" s="202" t="s">
         <v>48</v>
       </c>
-      <c r="AE86" s="197"/>
-      <c r="AF86" s="197"/>
-      <c r="AG86" s="197"/>
-      <c r="AH86" s="198"/>
+      <c r="AE86" s="202"/>
+      <c r="AF86" s="202"/>
+      <c r="AG86" s="202"/>
+      <c r="AH86" s="203"/>
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87" s="130" t="s">
@@ -7584,10 +7652,10 @@
       <c r="U88" s="151">
         <v>0.06</v>
       </c>
-      <c r="W88" s="195" t="s">
+      <c r="W88" s="199" t="s">
         <v>34</v>
       </c>
-      <c r="X88" s="199"/>
+      <c r="X88" s="200"/>
       <c r="Y88" s="54"/>
       <c r="Z88" s="15"/>
       <c r="AA88" s="15"/>
@@ -7663,10 +7731,10 @@
       <c r="U89" s="140">
         <v>0.09</v>
       </c>
-      <c r="W89" s="195" t="s">
+      <c r="W89" s="199" t="s">
         <v>35</v>
       </c>
-      <c r="X89" s="199"/>
+      <c r="X89" s="200"/>
       <c r="Y89" s="159">
         <v>0.17732999999999999</v>
       </c>
@@ -7762,10 +7830,10 @@
       <c r="U90" s="151">
         <v>0.05</v>
       </c>
-      <c r="W90" s="195" t="s">
+      <c r="W90" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="X90" s="199"/>
+      <c r="X90" s="200"/>
       <c r="Y90" s="159">
         <v>0.16</v>
       </c>
@@ -7861,10 +7929,10 @@
       <c r="U91" s="146">
         <v>5.2339410766781939E-2</v>
       </c>
-      <c r="W91" s="195" t="s">
+      <c r="W91" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="X91" s="199"/>
+      <c r="X91" s="200"/>
       <c r="Y91" s="159">
         <v>0.28000000000000003</v>
       </c>
@@ -7960,10 +8028,10 @@
       <c r="U92" s="146">
         <v>4.5787429941166059E-2</v>
       </c>
-      <c r="W92" s="195" t="s">
+      <c r="W92" s="199" t="s">
         <v>38</v>
       </c>
-      <c r="X92" s="199"/>
+      <c r="X92" s="200"/>
       <c r="Y92" s="159">
         <v>0.11</v>
       </c>
@@ -8059,10 +8127,10 @@
       <c r="U93" s="143">
         <v>6.72497190179734E-2</v>
       </c>
-      <c r="W93" s="195" t="s">
+      <c r="W93" s="199" t="s">
         <v>45</v>
       </c>
-      <c r="X93" s="199"/>
+      <c r="X93" s="200"/>
       <c r="Y93" s="159">
         <v>0.17</v>
       </c>
@@ -8158,10 +8226,10 @@
       <c r="U94" s="143">
         <v>0.10088850483912387</v>
       </c>
-      <c r="W94" s="195" t="s">
+      <c r="W94" s="199" t="s">
         <v>47</v>
       </c>
-      <c r="X94" s="199"/>
+      <c r="X94" s="200"/>
       <c r="Y94" s="170">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -8257,10 +8325,10 @@
       <c r="U95" s="151">
         <v>0.05</v>
       </c>
-      <c r="W95" s="195" t="s">
+      <c r="W95" s="199" t="s">
         <v>50</v>
       </c>
-      <c r="X95" s="199"/>
+      <c r="X95" s="200"/>
       <c r="Y95" s="165">
         <v>5.5608999999999999E-2</v>
       </c>
@@ -8423,42 +8491,42 @@
       </c>
     </row>
     <row r="98" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="193"/>
-      <c r="B98" s="207" t="s">
+      <c r="A98" s="198"/>
+      <c r="B98" s="196" t="s">
         <v>89</v>
       </c>
-      <c r="C98" s="203"/>
-      <c r="D98" s="203"/>
-      <c r="E98" s="203"/>
-      <c r="F98" s="203"/>
-      <c r="G98" s="193"/>
-      <c r="H98" s="203" t="s">
+      <c r="C98" s="197"/>
+      <c r="D98" s="197"/>
+      <c r="E98" s="197"/>
+      <c r="F98" s="197"/>
+      <c r="G98" s="198"/>
+      <c r="H98" s="197" t="s">
         <v>90</v>
       </c>
-      <c r="I98" s="203"/>
-      <c r="J98" s="203"/>
-      <c r="K98" s="203"/>
-      <c r="L98" s="203"/>
-      <c r="M98" s="193"/>
-      <c r="N98" s="203" t="s">
+      <c r="I98" s="197"/>
+      <c r="J98" s="197"/>
+      <c r="K98" s="197"/>
+      <c r="L98" s="197"/>
+      <c r="M98" s="198"/>
+      <c r="N98" s="197" t="s">
         <v>89</v>
       </c>
-      <c r="O98" s="203"/>
-      <c r="P98" s="203"/>
-      <c r="Q98" s="203"/>
-      <c r="R98" s="203"/>
-      <c r="S98" s="193"/>
-      <c r="T98" s="203" t="s">
+      <c r="O98" s="197"/>
+      <c r="P98" s="197"/>
+      <c r="Q98" s="197"/>
+      <c r="R98" s="197"/>
+      <c r="S98" s="198"/>
+      <c r="T98" s="197" t="s">
         <v>90</v>
       </c>
-      <c r="U98" s="203"/>
-      <c r="V98" s="203"/>
-      <c r="W98" s="203"/>
-      <c r="X98" s="203"/>
-      <c r="Y98" s="193"/>
+      <c r="U98" s="197"/>
+      <c r="V98" s="197"/>
+      <c r="W98" s="197"/>
+      <c r="X98" s="197"/>
+      <c r="Y98" s="198"/>
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A99" s="194"/>
+      <c r="A99" s="207"/>
       <c r="B99" s="1" t="s">
         <v>109</v>
       </c>
@@ -8765,19 +8833,56 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="G84:K84"/>
-    <mergeCell ref="L84:P84"/>
-    <mergeCell ref="Q84:U84"/>
-    <mergeCell ref="B98:G98"/>
-    <mergeCell ref="H98:M98"/>
-    <mergeCell ref="N98:S98"/>
-    <mergeCell ref="T98:Y98"/>
-    <mergeCell ref="W73:X73"/>
-    <mergeCell ref="W74:X74"/>
-    <mergeCell ref="W75:X75"/>
-    <mergeCell ref="W76:X76"/>
-    <mergeCell ref="W77:X77"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="X85:AH85"/>
+    <mergeCell ref="Y86:AC86"/>
+    <mergeCell ref="AD86:AH86"/>
+    <mergeCell ref="W88:X88"/>
+    <mergeCell ref="W89:X89"/>
+    <mergeCell ref="W90:X90"/>
+    <mergeCell ref="W91:X91"/>
+    <mergeCell ref="W92:X92"/>
+    <mergeCell ref="W93:X93"/>
+    <mergeCell ref="W94:X94"/>
+    <mergeCell ref="W95:X95"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="S22:AF22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AD23"/>
+    <mergeCell ref="AE23:AG23"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="AL43:AZ43"/>
+    <mergeCell ref="AU44:AW44"/>
+    <mergeCell ref="AX44:AZ44"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="T44:V44"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="Z44:AB44"/>
+    <mergeCell ref="AC44:AE44"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="G65:K65"/>
+    <mergeCell ref="B64:K64"/>
+    <mergeCell ref="BA44:BC44"/>
+    <mergeCell ref="AF44:AH44"/>
+    <mergeCell ref="AI44:AK44"/>
+    <mergeCell ref="AL44:AN44"/>
+    <mergeCell ref="AO44:AQ44"/>
+    <mergeCell ref="AR44:AT44"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="L65:P65"/>
+    <mergeCell ref="Q65:U65"/>
     <mergeCell ref="S1:AC1"/>
     <mergeCell ref="X67:AH67"/>
     <mergeCell ref="Y68:AC68"/>
@@ -8794,56 +8899,19 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="B43:P43"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="G65:K65"/>
-    <mergeCell ref="B64:K64"/>
-    <mergeCell ref="BA44:BC44"/>
-    <mergeCell ref="AF44:AH44"/>
-    <mergeCell ref="AI44:AK44"/>
-    <mergeCell ref="AL44:AN44"/>
-    <mergeCell ref="AO44:AQ44"/>
-    <mergeCell ref="AR44:AT44"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="L65:P65"/>
-    <mergeCell ref="Q65:U65"/>
-    <mergeCell ref="AL43:AZ43"/>
-    <mergeCell ref="AU44:AW44"/>
-    <mergeCell ref="AX44:AZ44"/>
-    <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="T44:V44"/>
-    <mergeCell ref="W44:Y44"/>
-    <mergeCell ref="Z44:AB44"/>
-    <mergeCell ref="AC44:AE44"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="S22:AF22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AD23"/>
-    <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="Y2:AC2"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="X85:AH85"/>
-    <mergeCell ref="Y86:AC86"/>
-    <mergeCell ref="AD86:AH86"/>
-    <mergeCell ref="W88:X88"/>
-    <mergeCell ref="W89:X89"/>
-    <mergeCell ref="W90:X90"/>
-    <mergeCell ref="W91:X91"/>
-    <mergeCell ref="W92:X92"/>
-    <mergeCell ref="W93:X93"/>
-    <mergeCell ref="W94:X94"/>
-    <mergeCell ref="W95:X95"/>
+    <mergeCell ref="W73:X73"/>
+    <mergeCell ref="W74:X74"/>
+    <mergeCell ref="W75:X75"/>
+    <mergeCell ref="W76:X76"/>
+    <mergeCell ref="W77:X77"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="G84:K84"/>
+    <mergeCell ref="L84:P84"/>
+    <mergeCell ref="Q84:U84"/>
+    <mergeCell ref="B98:G98"/>
+    <mergeCell ref="H98:M98"/>
+    <mergeCell ref="N98:S98"/>
+    <mergeCell ref="T98:Y98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8857,7 +8925,7 @@
   </sheetPr>
   <dimension ref="A1:AY46"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B22" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="R27" activeCellId="4" sqref="A31:XFD31 D27:E27 J27:K27 P27:Q27 R27:S27"/>
     </sheetView>
   </sheetViews>
@@ -8886,48 +8954,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="220" t="s">
+      <c r="A1" s="217" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
-      <c r="E1" s="241"/>
-      <c r="F1" s="241"/>
-      <c r="G1" s="241"/>
-      <c r="H1" s="241"/>
-      <c r="I1" s="241"/>
-      <c r="J1" s="241"/>
-      <c r="K1" s="242"/>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+      <c r="K1" s="219"/>
       <c r="L1" s="65"/>
-      <c r="M1" s="220" t="s">
+      <c r="M1" s="217" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="221"/>
-      <c r="O1" s="221"/>
-      <c r="P1" s="221"/>
-      <c r="Q1" s="221"/>
-      <c r="R1" s="221"/>
-      <c r="S1" s="221"/>
-      <c r="T1" s="221"/>
-      <c r="U1" s="221"/>
-      <c r="V1" s="221"/>
-      <c r="W1" s="221"/>
-      <c r="X1" s="221"/>
-      <c r="Y1" s="221"/>
-      <c r="Z1" s="221"/>
-      <c r="AA1" s="221"/>
-      <c r="AB1" s="221"/>
-      <c r="AC1" s="221"/>
-      <c r="AD1" s="221"/>
-      <c r="AE1" s="221"/>
-      <c r="AF1" s="221"/>
-      <c r="AG1" s="221"/>
-      <c r="AH1" s="221"/>
-      <c r="AI1" s="221"/>
-      <c r="AJ1" s="221"/>
-      <c r="AK1" s="221"/>
-      <c r="AL1" s="222"/>
+      <c r="N1" s="241"/>
+      <c r="O1" s="241"/>
+      <c r="P1" s="241"/>
+      <c r="Q1" s="241"/>
+      <c r="R1" s="241"/>
+      <c r="S1" s="241"/>
+      <c r="T1" s="241"/>
+      <c r="U1" s="241"/>
+      <c r="V1" s="241"/>
+      <c r="W1" s="241"/>
+      <c r="X1" s="241"/>
+      <c r="Y1" s="241"/>
+      <c r="Z1" s="241"/>
+      <c r="AA1" s="241"/>
+      <c r="AB1" s="241"/>
+      <c r="AC1" s="241"/>
+      <c r="AD1" s="241"/>
+      <c r="AE1" s="241"/>
+      <c r="AF1" s="241"/>
+      <c r="AG1" s="241"/>
+      <c r="AH1" s="241"/>
+      <c r="AI1" s="241"/>
+      <c r="AJ1" s="241"/>
+      <c r="AK1" s="241"/>
+      <c r="AL1" s="242"/>
       <c r="AM1" s="71"/>
       <c r="AN1" s="71"/>
       <c r="AO1" s="71"/>
@@ -8943,44 +9011,44 @@
       <c r="AY1" s="72"/>
     </row>
     <row r="2" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="223"/>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
-      <c r="F2" s="243"/>
-      <c r="G2" s="243"/>
-      <c r="H2" s="243"/>
-      <c r="I2" s="243"/>
-      <c r="J2" s="243"/>
-      <c r="K2" s="244"/>
+      <c r="A2" s="220"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="222"/>
       <c r="L2" s="74"/>
-      <c r="M2" s="223"/>
-      <c r="N2" s="224"/>
-      <c r="O2" s="224"/>
-      <c r="P2" s="224"/>
-      <c r="Q2" s="224"/>
-      <c r="R2" s="224"/>
-      <c r="S2" s="224"/>
-      <c r="T2" s="224"/>
-      <c r="U2" s="224"/>
-      <c r="V2" s="224"/>
-      <c r="W2" s="224"/>
-      <c r="X2" s="224"/>
-      <c r="Y2" s="224"/>
-      <c r="Z2" s="224"/>
-      <c r="AA2" s="224"/>
-      <c r="AB2" s="224"/>
-      <c r="AC2" s="224"/>
-      <c r="AD2" s="224"/>
-      <c r="AE2" s="224"/>
-      <c r="AF2" s="224"/>
-      <c r="AG2" s="224"/>
-      <c r="AH2" s="224"/>
-      <c r="AI2" s="224"/>
-      <c r="AJ2" s="224"/>
-      <c r="AK2" s="224"/>
-      <c r="AL2" s="225"/>
+      <c r="M2" s="220"/>
+      <c r="N2" s="243"/>
+      <c r="O2" s="243"/>
+      <c r="P2" s="243"/>
+      <c r="Q2" s="243"/>
+      <c r="R2" s="243"/>
+      <c r="S2" s="243"/>
+      <c r="T2" s="243"/>
+      <c r="U2" s="243"/>
+      <c r="V2" s="243"/>
+      <c r="W2" s="243"/>
+      <c r="X2" s="243"/>
+      <c r="Y2" s="243"/>
+      <c r="Z2" s="243"/>
+      <c r="AA2" s="243"/>
+      <c r="AB2" s="243"/>
+      <c r="AC2" s="243"/>
+      <c r="AD2" s="243"/>
+      <c r="AE2" s="243"/>
+      <c r="AF2" s="243"/>
+      <c r="AG2" s="243"/>
+      <c r="AH2" s="243"/>
+      <c r="AI2" s="243"/>
+      <c r="AJ2" s="243"/>
+      <c r="AK2" s="243"/>
+      <c r="AL2" s="244"/>
       <c r="AM2" s="66"/>
       <c r="AN2" s="66"/>
       <c r="AO2" s="66"/>
@@ -8996,7 +9064,7 @@
       <c r="AY2" s="73"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A3" s="251"/>
+      <c r="A3" s="229"/>
       <c r="B3" s="93" t="s">
         <v>76</v>
       </c>
@@ -9015,57 +9083,57 @@
       <c r="G3" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="236" t="s">
+      <c r="H3" s="234" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="234" t="s">
+      <c r="I3" s="237" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="234" t="s">
+      <c r="J3" s="237" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="235" t="s">
+      <c r="K3" s="238" t="s">
         <v>70</v>
       </c>
       <c r="L3" s="77"/>
-      <c r="M3" s="245"/>
-      <c r="N3" s="246"/>
-      <c r="O3" s="233" t="s">
+      <c r="M3" s="223"/>
+      <c r="N3" s="224"/>
+      <c r="O3" s="249" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="234"/>
-      <c r="Q3" s="234"/>
-      <c r="R3" s="235"/>
-      <c r="S3" s="234" t="s">
+      <c r="P3" s="237"/>
+      <c r="Q3" s="237"/>
+      <c r="R3" s="238"/>
+      <c r="S3" s="237" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="234"/>
-      <c r="U3" s="234"/>
-      <c r="V3" s="235"/>
-      <c r="W3" s="216" t="s">
+      <c r="T3" s="237"/>
+      <c r="U3" s="237"/>
+      <c r="V3" s="238"/>
+      <c r="W3" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="X3" s="216"/>
-      <c r="Y3" s="216"/>
-      <c r="Z3" s="217"/>
-      <c r="AA3" s="216" t="s">
+      <c r="X3" s="250"/>
+      <c r="Y3" s="250"/>
+      <c r="Z3" s="251"/>
+      <c r="AA3" s="250" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="216"/>
-      <c r="AC3" s="216"/>
-      <c r="AD3" s="217"/>
-      <c r="AE3" s="216" t="s">
+      <c r="AB3" s="250"/>
+      <c r="AC3" s="250"/>
+      <c r="AD3" s="251"/>
+      <c r="AE3" s="250" t="s">
         <v>20</v>
       </c>
-      <c r="AF3" s="216"/>
-      <c r="AG3" s="216"/>
-      <c r="AH3" s="217"/>
-      <c r="AI3" s="216" t="s">
+      <c r="AF3" s="250"/>
+      <c r="AG3" s="250"/>
+      <c r="AH3" s="251"/>
+      <c r="AI3" s="250" t="s">
         <v>21</v>
       </c>
-      <c r="AJ3" s="216"/>
-      <c r="AK3" s="216"/>
-      <c r="AL3" s="217"/>
+      <c r="AJ3" s="250"/>
+      <c r="AK3" s="250"/>
+      <c r="AL3" s="251"/>
       <c r="AM3" s="68"/>
       <c r="AN3" s="68"/>
       <c r="AO3" s="68"/>
@@ -9081,80 +9149,80 @@
       <c r="AY3" s="68"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A4" s="252"/>
-      <c r="B4" s="226" t="s">
+      <c r="A4" s="230"/>
+      <c r="B4" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="228" t="s">
+      <c r="C4" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="228" t="s">
+      <c r="D4" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="228" t="s">
+      <c r="E4" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="228" t="s">
+      <c r="F4" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="230" t="s">
+      <c r="G4" s="247" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="237"/>
-      <c r="I4" s="228"/>
-      <c r="J4" s="228"/>
-      <c r="K4" s="232"/>
+      <c r="H4" s="235"/>
+      <c r="I4" s="232"/>
+      <c r="J4" s="232"/>
+      <c r="K4" s="239"/>
       <c r="L4" s="77"/>
-      <c r="M4" s="247"/>
-      <c r="N4" s="248"/>
-      <c r="O4" s="226" t="s">
+      <c r="M4" s="225"/>
+      <c r="N4" s="226"/>
+      <c r="O4" s="245" t="s">
         <v>74</v>
       </c>
-      <c r="P4" s="228"/>
-      <c r="Q4" s="228" t="s">
+      <c r="P4" s="232"/>
+      <c r="Q4" s="232" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="232"/>
-      <c r="S4" s="228" t="s">
+      <c r="R4" s="239"/>
+      <c r="S4" s="232" t="s">
         <v>74</v>
       </c>
-      <c r="T4" s="228"/>
-      <c r="U4" s="228" t="s">
+      <c r="T4" s="232"/>
+      <c r="U4" s="232" t="s">
         <v>75</v>
       </c>
-      <c r="V4" s="232"/>
-      <c r="W4" s="218" t="s">
+      <c r="V4" s="239"/>
+      <c r="W4" s="252" t="s">
         <v>74</v>
       </c>
-      <c r="X4" s="218"/>
-      <c r="Y4" s="218" t="s">
+      <c r="X4" s="252"/>
+      <c r="Y4" s="252" t="s">
         <v>75</v>
       </c>
-      <c r="Z4" s="219"/>
-      <c r="AA4" s="218" t="s">
+      <c r="Z4" s="253"/>
+      <c r="AA4" s="252" t="s">
         <v>74</v>
       </c>
-      <c r="AB4" s="218"/>
-      <c r="AC4" s="218" t="s">
+      <c r="AB4" s="252"/>
+      <c r="AC4" s="252" t="s">
         <v>75</v>
       </c>
-      <c r="AD4" s="219"/>
-      <c r="AE4" s="218" t="s">
+      <c r="AD4" s="253"/>
+      <c r="AE4" s="252" t="s">
         <v>74</v>
       </c>
-      <c r="AF4" s="218"/>
-      <c r="AG4" s="218" t="s">
+      <c r="AF4" s="252"/>
+      <c r="AG4" s="252" t="s">
         <v>75</v>
       </c>
-      <c r="AH4" s="219"/>
-      <c r="AI4" s="218" t="s">
+      <c r="AH4" s="253"/>
+      <c r="AI4" s="252" t="s">
         <v>74</v>
       </c>
-      <c r="AJ4" s="218"/>
-      <c r="AK4" s="218" t="s">
+      <c r="AJ4" s="252"/>
+      <c r="AK4" s="252" t="s">
         <v>75</v>
       </c>
-      <c r="AL4" s="219"/>
+      <c r="AL4" s="253"/>
       <c r="AM4" s="68"/>
       <c r="AN4" s="68"/>
       <c r="AO4" s="68"/>
@@ -9170,20 +9238,20 @@
       <c r="AY4" s="68"/>
     </row>
     <row r="5" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="253"/>
-      <c r="B5" s="227"/>
-      <c r="C5" s="229"/>
-      <c r="D5" s="229"/>
-      <c r="E5" s="229"/>
-      <c r="F5" s="229"/>
-      <c r="G5" s="231"/>
-      <c r="H5" s="238"/>
-      <c r="I5" s="229"/>
-      <c r="J5" s="229"/>
-      <c r="K5" s="239"/>
+      <c r="A5" s="231"/>
+      <c r="B5" s="246"/>
+      <c r="C5" s="233"/>
+      <c r="D5" s="233"/>
+      <c r="E5" s="233"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="236"/>
+      <c r="I5" s="233"/>
+      <c r="J5" s="233"/>
+      <c r="K5" s="240"/>
       <c r="L5" s="78"/>
-      <c r="M5" s="249"/>
-      <c r="N5" s="250"/>
+      <c r="M5" s="227"/>
+      <c r="N5" s="228"/>
       <c r="O5" s="95" t="s">
         <v>73</v>
       </c>
@@ -10604,29 +10672,29 @@
     </row>
     <row r="24" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:51" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="220" t="s">
+      <c r="A25" s="217" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="241"/>
-      <c r="C25" s="241"/>
-      <c r="D25" s="241"/>
-      <c r="E25" s="241"/>
-      <c r="F25" s="241"/>
-      <c r="G25" s="241"/>
-      <c r="H25" s="241"/>
-      <c r="I25" s="241"/>
-      <c r="J25" s="241"/>
-      <c r="K25" s="241"/>
-      <c r="L25" s="241"/>
-      <c r="M25" s="241"/>
-      <c r="N25" s="241"/>
-      <c r="O25" s="241"/>
-      <c r="P25" s="241"/>
-      <c r="Q25" s="241"/>
-      <c r="R25" s="241"/>
-      <c r="S25" s="241"/>
-      <c r="T25" s="241"/>
-      <c r="U25" s="242"/>
+      <c r="B25" s="218"/>
+      <c r="C25" s="218"/>
+      <c r="D25" s="218"/>
+      <c r="E25" s="218"/>
+      <c r="F25" s="218"/>
+      <c r="G25" s="218"/>
+      <c r="H25" s="218"/>
+      <c r="I25" s="218"/>
+      <c r="J25" s="218"/>
+      <c r="K25" s="218"/>
+      <c r="L25" s="218"/>
+      <c r="M25" s="218"/>
+      <c r="N25" s="218"/>
+      <c r="O25" s="218"/>
+      <c r="P25" s="218"/>
+      <c r="Q25" s="218"/>
+      <c r="R25" s="218"/>
+      <c r="S25" s="218"/>
+      <c r="T25" s="218"/>
+      <c r="U25" s="219"/>
       <c r="Z25" s="4"/>
       <c r="AA25" s="66"/>
       <c r="AB25" s="66"/>
@@ -10655,27 +10723,27 @@
       <c r="AY25" s="66"/>
     </row>
     <row r="26" spans="1:51" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="223"/>
-      <c r="B26" s="243"/>
-      <c r="C26" s="243"/>
-      <c r="D26" s="243"/>
-      <c r="E26" s="243"/>
-      <c r="F26" s="243"/>
-      <c r="G26" s="243"/>
-      <c r="H26" s="243"/>
-      <c r="I26" s="243"/>
-      <c r="J26" s="243"/>
-      <c r="K26" s="243"/>
-      <c r="L26" s="243"/>
-      <c r="M26" s="243"/>
-      <c r="N26" s="243"/>
-      <c r="O26" s="243"/>
-      <c r="P26" s="243"/>
-      <c r="Q26" s="243"/>
-      <c r="R26" s="243"/>
-      <c r="S26" s="243"/>
-      <c r="T26" s="243"/>
-      <c r="U26" s="244"/>
+      <c r="A26" s="220"/>
+      <c r="B26" s="221"/>
+      <c r="C26" s="221"/>
+      <c r="D26" s="221"/>
+      <c r="E26" s="221"/>
+      <c r="F26" s="221"/>
+      <c r="G26" s="221"/>
+      <c r="H26" s="221"/>
+      <c r="I26" s="221"/>
+      <c r="J26" s="221"/>
+      <c r="K26" s="221"/>
+      <c r="L26" s="221"/>
+      <c r="M26" s="221"/>
+      <c r="N26" s="221"/>
+      <c r="O26" s="221"/>
+      <c r="P26" s="221"/>
+      <c r="Q26" s="221"/>
+      <c r="R26" s="221"/>
+      <c r="S26" s="221"/>
+      <c r="T26" s="221"/>
+      <c r="U26" s="222"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="66"/>
       <c r="AB26" s="66"/>
@@ -10705,46 +10773,46 @@
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" s="75"/>
-      <c r="B27" s="203" t="s">
+      <c r="B27" s="197" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="193"/>
-      <c r="D27" s="203" t="s">
+      <c r="C27" s="198"/>
+      <c r="D27" s="197" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="193"/>
-      <c r="F27" s="200" t="s">
+      <c r="E27" s="198"/>
+      <c r="F27" s="205" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="240"/>
+      <c r="G27" s="216"/>
       <c r="H27" s="204" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="240"/>
-      <c r="J27" s="200" t="s">
+      <c r="I27" s="216"/>
+      <c r="J27" s="205" t="s">
         <v>82</v>
       </c>
-      <c r="K27" s="240"/>
-      <c r="L27" s="200" t="s">
+      <c r="K27" s="216"/>
+      <c r="L27" s="205" t="s">
         <v>83</v>
       </c>
-      <c r="M27" s="240"/>
-      <c r="N27" s="200" t="s">
+      <c r="M27" s="216"/>
+      <c r="N27" s="205" t="s">
         <v>84</v>
       </c>
-      <c r="O27" s="240"/>
-      <c r="P27" s="200" t="s">
+      <c r="O27" s="216"/>
+      <c r="P27" s="205" t="s">
         <v>85</v>
       </c>
-      <c r="Q27" s="240"/>
-      <c r="R27" s="200" t="s">
+      <c r="Q27" s="216"/>
+      <c r="R27" s="205" t="s">
         <v>86</v>
       </c>
-      <c r="S27" s="240"/>
-      <c r="T27" s="200" t="s">
+      <c r="S27" s="216"/>
+      <c r="T27" s="205" t="s">
         <v>87</v>
       </c>
-      <c r="U27" s="240"/>
+      <c r="U27" s="216"/>
     </row>
     <row r="28" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="76"/>
@@ -11686,6 +11754,33 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="AE3:AH3"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="M1:AL2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
     <mergeCell ref="P27:Q27"/>
     <mergeCell ref="R27:S27"/>
     <mergeCell ref="T27:U27"/>
@@ -11702,33 +11797,6 @@
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="M1:AL2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE3:AH3"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AL4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11750,95 +11818,95 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="205" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="200"/>
-      <c r="L1" s="200"/>
-      <c r="M1" s="200"/>
-      <c r="N1" s="200"/>
-      <c r="O1" s="200"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="205"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="205"/>
+      <c r="L1" s="205"/>
+      <c r="M1" s="205"/>
+      <c r="N1" s="205"/>
+      <c r="O1" s="205"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="203" t="s">
+      <c r="S1" s="197" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="203"/>
-      <c r="U1" s="203"/>
-      <c r="V1" s="203"/>
-      <c r="W1" s="203"/>
-      <c r="X1" s="203"/>
-      <c r="Y1" s="203"/>
-      <c r="Z1" s="203"/>
-      <c r="AA1" s="203"/>
-      <c r="AB1" s="203"/>
-      <c r="AC1" s="203"/>
-      <c r="AD1" s="203"/>
-      <c r="AE1" s="203"/>
-      <c r="AF1" s="203"/>
+      <c r="T1" s="197"/>
+      <c r="U1" s="197"/>
+      <c r="V1" s="197"/>
+      <c r="W1" s="197"/>
+      <c r="X1" s="197"/>
+      <c r="Y1" s="197"/>
+      <c r="Z1" s="197"/>
+      <c r="AA1" s="197"/>
+      <c r="AB1" s="197"/>
+      <c r="AC1" s="197"/>
+      <c r="AD1" s="197"/>
+      <c r="AE1" s="197"/>
+      <c r="AF1" s="197"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="201" t="s">
+      <c r="B2" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="201"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="201" t="s">
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="201"/>
-      <c r="J2" s="201"/>
-      <c r="K2" s="201" t="s">
+      <c r="I2" s="208"/>
+      <c r="J2" s="208"/>
+      <c r="K2" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="201"/>
-      <c r="M2" s="201"/>
-      <c r="N2" s="201" t="s">
+      <c r="L2" s="208"/>
+      <c r="M2" s="208"/>
+      <c r="N2" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="201"/>
-      <c r="P2" s="202"/>
+      <c r="O2" s="208"/>
+      <c r="P2" s="209"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="201" t="s">
+      <c r="S2" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="201"/>
-      <c r="U2" s="201"/>
-      <c r="V2" s="201" t="s">
+      <c r="T2" s="208"/>
+      <c r="U2" s="208"/>
+      <c r="V2" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="201"/>
-      <c r="X2" s="201"/>
-      <c r="Y2" s="201" t="s">
+      <c r="W2" s="208"/>
+      <c r="X2" s="208"/>
+      <c r="Y2" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="201"/>
-      <c r="AA2" s="201"/>
-      <c r="AB2" s="201" t="s">
+      <c r="Z2" s="208"/>
+      <c r="AA2" s="208"/>
+      <c r="AB2" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="201"/>
-      <c r="AD2" s="201"/>
-      <c r="AE2" s="201" t="s">
+      <c r="AC2" s="208"/>
+      <c r="AD2" s="208"/>
+      <c r="AE2" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="201"/>
-      <c r="AG2" s="202"/>
+      <c r="AF2" s="208"/>
+      <c r="AG2" s="209"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -12607,95 +12675,95 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="200" t="s">
+      <c r="B22" s="205" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="200"/>
-      <c r="D22" s="200"/>
-      <c r="E22" s="200"/>
-      <c r="F22" s="200"/>
-      <c r="G22" s="200"/>
-      <c r="H22" s="200"/>
-      <c r="I22" s="200"/>
-      <c r="J22" s="200"/>
-      <c r="K22" s="200"/>
-      <c r="L22" s="200"/>
-      <c r="M22" s="200"/>
-      <c r="N22" s="200"/>
-      <c r="O22" s="200"/>
+      <c r="C22" s="205"/>
+      <c r="D22" s="205"/>
+      <c r="E22" s="205"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="205"/>
+      <c r="K22" s="205"/>
+      <c r="L22" s="205"/>
+      <c r="M22" s="205"/>
+      <c r="N22" s="205"/>
+      <c r="O22" s="205"/>
       <c r="P22" s="2"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="203" t="s">
+      <c r="S22" s="197" t="s">
         <v>29</v>
       </c>
-      <c r="T22" s="203"/>
-      <c r="U22" s="203"/>
-      <c r="V22" s="203"/>
-      <c r="W22" s="203"/>
-      <c r="X22" s="203"/>
-      <c r="Y22" s="203"/>
-      <c r="Z22" s="203"/>
-      <c r="AA22" s="203"/>
-      <c r="AB22" s="203"/>
-      <c r="AC22" s="203"/>
-      <c r="AD22" s="203"/>
-      <c r="AE22" s="203"/>
-      <c r="AF22" s="203"/>
+      <c r="T22" s="197"/>
+      <c r="U22" s="197"/>
+      <c r="V22" s="197"/>
+      <c r="W22" s="197"/>
+      <c r="X22" s="197"/>
+      <c r="Y22" s="197"/>
+      <c r="Z22" s="197"/>
+      <c r="AA22" s="197"/>
+      <c r="AB22" s="197"/>
+      <c r="AC22" s="197"/>
+      <c r="AD22" s="197"/>
+      <c r="AE22" s="197"/>
+      <c r="AF22" s="197"/>
       <c r="AG22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="201" t="s">
+      <c r="B23" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="201"/>
-      <c r="D23" s="201"/>
-      <c r="E23" s="201" t="s">
+      <c r="C23" s="208"/>
+      <c r="D23" s="208"/>
+      <c r="E23" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="201"/>
-      <c r="G23" s="201"/>
-      <c r="H23" s="201" t="s">
+      <c r="F23" s="208"/>
+      <c r="G23" s="208"/>
+      <c r="H23" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="201"/>
-      <c r="J23" s="201"/>
-      <c r="K23" s="201" t="s">
+      <c r="I23" s="208"/>
+      <c r="J23" s="208"/>
+      <c r="K23" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="201"/>
-      <c r="M23" s="201"/>
-      <c r="N23" s="201" t="s">
+      <c r="L23" s="208"/>
+      <c r="M23" s="208"/>
+      <c r="N23" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="201"/>
+      <c r="O23" s="208"/>
       <c r="P23" s="5"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="201" t="s">
+      <c r="S23" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="201"/>
-      <c r="U23" s="201"/>
-      <c r="V23" s="201" t="s">
+      <c r="T23" s="208"/>
+      <c r="U23" s="208"/>
+      <c r="V23" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="W23" s="201"/>
-      <c r="X23" s="201"/>
-      <c r="Y23" s="201" t="s">
+      <c r="W23" s="208"/>
+      <c r="X23" s="208"/>
+      <c r="Y23" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="Z23" s="201"/>
-      <c r="AA23" s="201"/>
-      <c r="AB23" s="201" t="s">
+      <c r="Z23" s="208"/>
+      <c r="AA23" s="208"/>
+      <c r="AB23" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="AC23" s="201"/>
-      <c r="AD23" s="201"/>
-      <c r="AE23" s="201" t="s">
+      <c r="AC23" s="208"/>
+      <c r="AD23" s="208"/>
+      <c r="AE23" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="AF23" s="201"/>
-      <c r="AG23" s="202"/>
+      <c r="AF23" s="208"/>
+      <c r="AG23" s="209"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -13462,95 +13530,95 @@
     <row r="42" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="200" t="s">
+      <c r="B43" s="205" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="200"/>
-      <c r="D43" s="200"/>
-      <c r="E43" s="200"/>
-      <c r="F43" s="200"/>
-      <c r="G43" s="200"/>
-      <c r="H43" s="200"/>
-      <c r="I43" s="200"/>
-      <c r="J43" s="200"/>
-      <c r="K43" s="200"/>
-      <c r="L43" s="200"/>
-      <c r="M43" s="200"/>
-      <c r="N43" s="200"/>
-      <c r="O43" s="200"/>
+      <c r="C43" s="205"/>
+      <c r="D43" s="205"/>
+      <c r="E43" s="205"/>
+      <c r="F43" s="205"/>
+      <c r="G43" s="205"/>
+      <c r="H43" s="205"/>
+      <c r="I43" s="205"/>
+      <c r="J43" s="205"/>
+      <c r="K43" s="205"/>
+      <c r="L43" s="205"/>
+      <c r="M43" s="205"/>
+      <c r="N43" s="205"/>
+      <c r="O43" s="205"/>
       <c r="P43" s="2"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="200" t="s">
+      <c r="S43" s="205" t="s">
         <v>30</v>
       </c>
-      <c r="T43" s="200"/>
-      <c r="U43" s="200"/>
-      <c r="V43" s="200"/>
-      <c r="W43" s="200"/>
-      <c r="X43" s="200"/>
-      <c r="Y43" s="200"/>
-      <c r="Z43" s="200"/>
-      <c r="AA43" s="200"/>
-      <c r="AB43" s="200"/>
-      <c r="AC43" s="200"/>
-      <c r="AD43" s="200"/>
-      <c r="AE43" s="200"/>
-      <c r="AF43" s="200"/>
+      <c r="T43" s="205"/>
+      <c r="U43" s="205"/>
+      <c r="V43" s="205"/>
+      <c r="W43" s="205"/>
+      <c r="X43" s="205"/>
+      <c r="Y43" s="205"/>
+      <c r="Z43" s="205"/>
+      <c r="AA43" s="205"/>
+      <c r="AB43" s="205"/>
+      <c r="AC43" s="205"/>
+      <c r="AD43" s="205"/>
+      <c r="AE43" s="205"/>
+      <c r="AF43" s="205"/>
       <c r="AG43" s="2"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="201" t="s">
+      <c r="B44" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="201"/>
-      <c r="D44" s="201"/>
-      <c r="E44" s="201" t="s">
+      <c r="C44" s="208"/>
+      <c r="D44" s="208"/>
+      <c r="E44" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="201"/>
-      <c r="G44" s="201"/>
-      <c r="H44" s="201" t="s">
+      <c r="F44" s="208"/>
+      <c r="G44" s="208"/>
+      <c r="H44" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="201"/>
-      <c r="J44" s="201"/>
-      <c r="K44" s="201" t="s">
+      <c r="I44" s="208"/>
+      <c r="J44" s="208"/>
+      <c r="K44" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="L44" s="201"/>
-      <c r="M44" s="201"/>
+      <c r="L44" s="208"/>
+      <c r="M44" s="208"/>
       <c r="N44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="O44" s="14"/>
       <c r="P44" s="5"/>
       <c r="R44" s="9"/>
-      <c r="S44" s="201" t="s">
+      <c r="S44" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="T44" s="201"/>
-      <c r="U44" s="201"/>
-      <c r="V44" s="201" t="s">
+      <c r="T44" s="208"/>
+      <c r="U44" s="208"/>
+      <c r="V44" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="W44" s="201"/>
-      <c r="X44" s="201"/>
-      <c r="Y44" s="201" t="s">
+      <c r="W44" s="208"/>
+      <c r="X44" s="208"/>
+      <c r="Y44" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="Z44" s="201"/>
-      <c r="AA44" s="201"/>
-      <c r="AB44" s="201" t="s">
+      <c r="Z44" s="208"/>
+      <c r="AA44" s="208"/>
+      <c r="AB44" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="AC44" s="201"/>
-      <c r="AD44" s="201"/>
-      <c r="AE44" s="201" t="s">
+      <c r="AC44" s="208"/>
+      <c r="AD44" s="208"/>
+      <c r="AE44" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="AF44" s="201"/>
-      <c r="AG44" s="202"/>
+      <c r="AF44" s="208"/>
+      <c r="AG44" s="209"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
@@ -14318,41 +14386,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="B43:O43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="S1:AF1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="S22:AF22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AD23"/>
+    <mergeCell ref="AE23:AG23"/>
     <mergeCell ref="S43:AF43"/>
     <mergeCell ref="S44:U44"/>
     <mergeCell ref="V44:X44"/>
     <mergeCell ref="Y44:AA44"/>
     <mergeCell ref="AB44:AD44"/>
     <mergeCell ref="AE44:AG44"/>
-    <mergeCell ref="S22:AF22"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AD23"/>
-    <mergeCell ref="AE23:AG23"/>
-    <mergeCell ref="S1:AF1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="B43:O43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14374,69 +14442,69 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="205" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="200"/>
-      <c r="L1" s="200"/>
-      <c r="M1" s="200"/>
-      <c r="N1" s="200"/>
-      <c r="O1" s="200"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="205"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="205"/>
+      <c r="L1" s="205"/>
+      <c r="M1" s="205"/>
+      <c r="N1" s="205"/>
+      <c r="O1" s="205"/>
       <c r="P1" s="2"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="200" t="s">
+      <c r="S1" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="200"/>
-      <c r="U1" s="200"/>
-      <c r="V1" s="200"/>
-      <c r="W1" s="200"/>
-      <c r="X1" s="200"/>
-      <c r="Y1" s="200"/>
-      <c r="Z1" s="200"/>
-      <c r="AA1" s="200"/>
-      <c r="AB1" s="200"/>
-      <c r="AC1" s="200"/>
-      <c r="AD1" s="200"/>
-      <c r="AE1" s="200"/>
-      <c r="AF1" s="200"/>
+      <c r="T1" s="205"/>
+      <c r="U1" s="205"/>
+      <c r="V1" s="205"/>
+      <c r="W1" s="205"/>
+      <c r="X1" s="205"/>
+      <c r="Y1" s="205"/>
+      <c r="Z1" s="205"/>
+      <c r="AA1" s="205"/>
+      <c r="AB1" s="205"/>
+      <c r="AC1" s="205"/>
+      <c r="AD1" s="205"/>
+      <c r="AE1" s="205"/>
+      <c r="AF1" s="205"/>
       <c r="AG1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="201" t="s">
+      <c r="B2" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="201"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="201" t="s">
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="201"/>
-      <c r="J2" s="201"/>
-      <c r="K2" s="201" t="s">
+      <c r="I2" s="208"/>
+      <c r="J2" s="208"/>
+      <c r="K2" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="201"/>
-      <c r="M2" s="201"/>
-      <c r="N2" s="201" t="s">
+      <c r="L2" s="208"/>
+      <c r="M2" s="208"/>
+      <c r="N2" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="201"/>
-      <c r="P2" s="202"/>
+      <c r="O2" s="208"/>
+      <c r="P2" s="209"/>
       <c r="R2" s="3"/>
       <c r="S2" s="206" t="s">
         <v>17</v>
@@ -14462,7 +14530,7 @@
         <v>21</v>
       </c>
       <c r="AF2" s="206"/>
-      <c r="AG2" s="194"/>
+      <c r="AG2" s="207"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -15231,51 +15299,51 @@
     <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="200" t="s">
+      <c r="B22" s="205" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="200"/>
-      <c r="D22" s="200"/>
-      <c r="E22" s="200"/>
-      <c r="F22" s="200"/>
-      <c r="G22" s="200"/>
-      <c r="H22" s="200"/>
-      <c r="I22" s="200"/>
-      <c r="J22" s="200"/>
-      <c r="K22" s="200"/>
-      <c r="L22" s="200"/>
-      <c r="M22" s="200"/>
-      <c r="N22" s="200"/>
-      <c r="O22" s="200"/>
+      <c r="C22" s="205"/>
+      <c r="D22" s="205"/>
+      <c r="E22" s="205"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="205"/>
+      <c r="K22" s="205"/>
+      <c r="L22" s="205"/>
+      <c r="M22" s="205"/>
+      <c r="N22" s="205"/>
+      <c r="O22" s="205"/>
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="201" t="s">
+      <c r="B23" s="208" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="201"/>
-      <c r="D23" s="201"/>
-      <c r="E23" s="201" t="s">
+      <c r="C23" s="208"/>
+      <c r="D23" s="208"/>
+      <c r="E23" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="201"/>
-      <c r="G23" s="201"/>
-      <c r="H23" s="201" t="s">
+      <c r="F23" s="208"/>
+      <c r="G23" s="208"/>
+      <c r="H23" s="208" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="201"/>
-      <c r="J23" s="201"/>
-      <c r="K23" s="201" t="s">
+      <c r="I23" s="208"/>
+      <c r="J23" s="208"/>
+      <c r="K23" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="201"/>
-      <c r="M23" s="201"/>
-      <c r="N23" s="201" t="s">
+      <c r="L23" s="208"/>
+      <c r="M23" s="208"/>
+      <c r="N23" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="201"/>
-      <c r="P23" s="202"/>
+      <c r="O23" s="208"/>
+      <c r="P23" s="209"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -15679,24 +15747,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
     <mergeCell ref="S1:AF1"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="V2:X2"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>